<commit_message>
Board is now inside a player
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\PycharmProjects\dice_game_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5075D735-3AD7-44A7-B5E2-7522A87A55F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B024C83-01A9-48D6-9036-B70377796C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,30 +130,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>철갑기사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>도박꾼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>성직자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>연구원</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>옴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>검사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>HP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -414,10 +390,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>피의 귀족</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>특수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1345,6 +1317,34 @@
   </si>
   <si>
     <t>상점에서 스킬 업글을 할 수 있음 =&gt; 스킬 코스트를 1 줄일 수 있음 (1강만 가능)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>철갑기사 Baron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성직자 Riri</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유적 탐험가 Arisu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검사 Mirinae</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피의 귀족 Soamir</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">옴 Narin </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도박꾼 Cinavro</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2047,7 +2047,7 @@
   <dimension ref="A1:BM193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AL10" sqref="AL10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2071,21 +2071,21 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.45">
       <c r="J5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="P5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="W5" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.45">
       <c r="J6" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>9</v>
@@ -2100,13 +2100,13 @@
         <v>12</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -2138,47 +2138,47 @@
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.45">
       <c r="J8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K8">
-        <f>2^(K7-1)</f>
-        <v>1</v>
+        <f>2^(K7)</f>
+        <v>2</v>
       </c>
       <c r="L8">
-        <f t="shared" ref="L8:T8" si="0">2^(L7-1)</f>
-        <v>1</v>
+        <f t="shared" ref="L8:T8" si="0">2^(L7)</f>
+        <v>2</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="T8">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.45">
@@ -2186,7 +2186,7 @@
         <v>22</v>
       </c>
       <c r="L9" s="45" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="M9" s="45"/>
       <c r="N9" s="45"/>
@@ -2196,7 +2196,7 @@
       <c r="R9" s="45"/>
       <c r="S9" s="45"/>
       <c r="T9" s="45" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="U9" s="45"/>
       <c r="V9" s="45"/>
@@ -2206,7 +2206,7 @@
       <c r="Z9" s="45"/>
       <c r="AA9" s="45"/>
       <c r="AB9" s="45" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="AC9" s="45"/>
       <c r="AD9" s="45"/>
@@ -2216,7 +2216,7 @@
       <c r="AH9" s="45"/>
       <c r="AI9" s="45"/>
       <c r="AL9" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.45">
@@ -2264,13 +2264,13 @@
       <c r="AH10" s="40"/>
       <c r="AI10" s="40"/>
       <c r="AJ10" s="32" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="AK10" s="32" t="s">
         <v>16</v>
       </c>
       <c r="AL10" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.45">
@@ -2278,25 +2278,25 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H11" s="38" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="I11" s="38"/>
       <c r="J11" s="38" t="s">
@@ -2366,12 +2366,12 @@
       <c r="AJ11" s="32"/>
       <c r="AK11" s="32"/>
       <c r="AL11" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
-        <v>23</v>
+        <v>321</v>
       </c>
       <c r="B12" s="6">
         <v>150</v>
@@ -2390,21 +2390,21 @@
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="35" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I12" s="36"/>
       <c r="J12" s="37" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K12" s="37"/>
       <c r="L12" s="5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="M12" s="39"/>
       <c r="N12" s="39"/>
       <c r="O12" s="12"/>
       <c r="P12" s="11" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="Q12" s="37"/>
       <c r="R12" s="37"/>
@@ -2426,16 +2426,16 @@
       <c r="AH12" s="37"/>
       <c r="AI12" s="12"/>
       <c r="AJ12" s="33" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="AK12" s="33"/>
       <c r="AL12" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
-        <v>24</v>
+        <v>327</v>
       </c>
       <c r="B13" s="6">
         <v>100</v>
@@ -2453,60 +2453,60 @@
         <v>10</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I13" s="36"/>
       <c r="J13" s="37" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K13" s="37"/>
       <c r="L13" s="5" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="M13" s="39"/>
       <c r="N13" s="39"/>
       <c r="O13" s="12"/>
       <c r="P13" s="11" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="Q13" s="37"/>
       <c r="R13" s="37"/>
       <c r="S13" s="12"/>
       <c r="T13" s="11" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="U13" s="37"/>
       <c r="V13" s="37"/>
       <c r="W13" s="12"/>
       <c r="X13" s="11" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="Y13" s="37"/>
       <c r="Z13" s="37"/>
       <c r="AA13" s="12"/>
       <c r="AB13" s="11" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="AC13" s="37"/>
       <c r="AD13" s="37"/>
       <c r="AE13" s="12"/>
       <c r="AF13" s="11" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="AG13" s="37"/>
       <c r="AH13" s="37"/>
       <c r="AI13" s="12"/>
       <c r="AJ13" s="6" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="AK13" s="6"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
-        <v>94</v>
+        <v>325</v>
       </c>
       <c r="B14" s="6">
         <v>80</v>
@@ -2525,21 +2525,21 @@
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="35" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I14" s="36"/>
       <c r="J14" s="37" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K14" s="37"/>
       <c r="L14" s="5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="M14" s="39"/>
       <c r="N14" s="39"/>
       <c r="O14" s="12"/>
       <c r="P14" s="11" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="Q14" s="37"/>
       <c r="R14" s="37"/>
@@ -2557,19 +2557,19 @@
       <c r="AD14" s="37"/>
       <c r="AE14" s="12"/>
       <c r="AF14" s="11" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="AG14" s="37"/>
       <c r="AH14" s="37"/>
       <c r="AI14" s="12"/>
       <c r="AJ14" s="6" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="AK14" s="6"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
-        <v>25</v>
+        <v>322</v>
       </c>
       <c r="B15" s="6">
         <v>50</v>
@@ -2588,55 +2588,55 @@
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="35" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I15" s="36"/>
       <c r="J15" s="37"/>
       <c r="K15" s="37"/>
       <c r="L15" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="M15" s="39"/>
       <c r="N15" s="39"/>
       <c r="O15" s="12"/>
       <c r="P15" s="11" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="Q15" s="37"/>
       <c r="R15" s="37"/>
       <c r="S15" s="12"/>
       <c r="T15" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="U15" s="37"/>
       <c r="V15" s="37"/>
       <c r="W15" s="12"/>
       <c r="X15" s="11" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="Y15" s="37"/>
       <c r="Z15" s="37"/>
       <c r="AA15" s="12"/>
       <c r="AB15" s="11" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="AC15" s="37"/>
       <c r="AD15" s="37"/>
       <c r="AE15" s="12"/>
       <c r="AF15" s="11" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="AG15" s="37"/>
       <c r="AH15" s="37"/>
       <c r="AI15" s="12"/>
       <c r="AJ15" s="6" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="AK15" s="6"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
-        <v>27</v>
+        <v>326</v>
       </c>
       <c r="B16" s="6">
         <v>60</v>
@@ -2654,66 +2654,66 @@
         <v>10</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="11" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K16" s="11"/>
       <c r="L16" s="5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="M16" s="39"/>
       <c r="N16" s="39"/>
       <c r="O16" s="12"/>
       <c r="P16" s="11" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="Q16" s="37"/>
       <c r="R16" s="37"/>
       <c r="S16" s="12"/>
       <c r="T16" s="11" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="U16" s="37"/>
       <c r="V16" s="37"/>
       <c r="W16" s="12"/>
       <c r="X16" s="11" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="Y16" s="37"/>
       <c r="Z16" s="37"/>
       <c r="AA16" s="12"/>
       <c r="AB16" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="AC16" s="37"/>
       <c r="AD16" s="37"/>
       <c r="AE16" s="12"/>
       <c r="AF16" s="11" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="AG16" s="37"/>
       <c r="AH16" s="37"/>
       <c r="AI16" s="12"/>
       <c r="AJ16" s="6" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="AK16" s="6"/>
     </row>
     <row r="17" spans="1:65" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
-        <v>28</v>
+        <v>324</v>
       </c>
       <c r="B17" s="6">
         <v>80</v>
       </c>
       <c r="C17" s="8">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D17" s="6">
         <v>4</v>
@@ -2722,64 +2722,64 @@
         <v>4</v>
       </c>
       <c r="F17" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="35" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I17" s="36"/>
       <c r="J17" s="37" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="K17" s="37"/>
       <c r="L17" s="5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="M17" s="39"/>
       <c r="N17" s="39"/>
       <c r="O17" s="12"/>
       <c r="P17" s="11" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="Q17" s="37"/>
       <c r="R17" s="37"/>
       <c r="S17" s="12"/>
       <c r="T17" s="11" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="U17" s="37"/>
       <c r="V17" s="37"/>
       <c r="W17" s="12"/>
       <c r="X17" s="11" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="Y17" s="37"/>
       <c r="Z17" s="37"/>
       <c r="AA17" s="12"/>
       <c r="AB17" s="11" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="AC17" s="37"/>
       <c r="AD17" s="37"/>
       <c r="AE17" s="12"/>
       <c r="AF17" s="11" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="AG17" s="37"/>
       <c r="AH17" s="37"/>
       <c r="AI17" s="12"/>
       <c r="AJ17" s="6" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="AK17" s="6"/>
       <c r="AL17" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:65" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
-        <v>26</v>
+        <v>323</v>
       </c>
       <c r="B18" s="6">
         <v>80</v>
@@ -2798,11 +2798,11 @@
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="35" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="I18" s="36"/>
       <c r="J18" s="37" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="K18" s="37"/>
       <c r="L18" s="5"/>
@@ -2830,7 +2830,7 @@
       <c r="AH18" s="37"/>
       <c r="AI18" s="12"/>
       <c r="AJ18" s="6" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="AK18" s="6"/>
     </row>
@@ -3224,28 +3224,28 @@
       <c r="AJ28" s="6"/>
       <c r="AK28" s="6"/>
       <c r="AX28" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:65" x14ac:dyDescent="0.45">
       <c r="AX29" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:65" x14ac:dyDescent="0.45">
       <c r="AX30" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:65" x14ac:dyDescent="0.45">
       <c r="D31" s="2" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="T31" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="AB31" s="38" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="AC31" s="38"/>
       <c r="AD31" s="38"/>
@@ -3267,7 +3267,7 @@
       <c r="AT31" s="38"/>
       <c r="AU31" s="38"/>
       <c r="AX31" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:65" ht="17.5" x14ac:dyDescent="0.45">
@@ -3275,41 +3275,41 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F32" s="38"/>
       <c r="G32" s="38"/>
       <c r="H32" s="38" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="I32" s="38"/>
       <c r="J32" s="38"/>
       <c r="K32" s="38" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L32" s="38"/>
       <c r="M32" s="38"/>
       <c r="N32" s="38" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="O32" s="38"/>
       <c r="P32" s="38"/>
       <c r="Q32" s="38" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="R32" s="38"/>
       <c r="S32" s="38"/>
       <c r="T32" s="38" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="U32" s="38"/>
       <c r="V32" s="38"/>
@@ -3317,10 +3317,10 @@
       <c r="X32" s="38"/>
       <c r="Y32" s="38"/>
       <c r="Z32" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="AA32" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="AB32" s="1">
         <v>5</v>
@@ -3383,40 +3383,40 @@
         <v>100</v>
       </c>
       <c r="AX32" s="16" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="BA32" s="23" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="BD32" s="27" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="BG32" s="29" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="BJ32" s="20" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="BM32" s="30" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A33" s="15" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="37"/>
       <c r="F33" s="37"/>
       <c r="G33" s="37"/>
       <c r="H33" s="37" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="I33" s="37"/>
       <c r="J33" s="37"/>
@@ -3430,7 +3430,7 @@
       <c r="R33" s="37"/>
       <c r="S33" s="37"/>
       <c r="T33" s="44" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="U33" s="37"/>
       <c r="V33" s="37"/>
@@ -3478,33 +3478,33 @@
       <c r="AT33" s="19"/>
       <c r="AU33" s="19"/>
       <c r="AV33" s="25" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="AW33" s="26"/>
     </row>
     <row r="34" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A34" s="15" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="37" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F34" s="37"/>
       <c r="G34" s="37"/>
       <c r="H34" s="37" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="I34" s="37"/>
       <c r="J34" s="37"/>
       <c r="K34" s="37" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="L34" s="37"/>
       <c r="M34" s="37"/>
@@ -3515,7 +3515,7 @@
       <c r="R34" s="37"/>
       <c r="S34" s="37"/>
       <c r="T34" s="44" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="U34" s="37"/>
       <c r="V34" s="37"/>
@@ -3565,38 +3565,38 @@
       <c r="AT34" s="19"/>
       <c r="AU34" s="19"/>
       <c r="AV34" s="25" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="AW34" s="26"/>
     </row>
     <row r="35" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A35" s="15" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="37" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F35" s="37"/>
       <c r="G35" s="37"/>
       <c r="H35" s="37" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="I35" s="37"/>
       <c r="J35" s="37"/>
       <c r="K35" s="37" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="L35" s="37"/>
       <c r="M35" s="37"/>
       <c r="N35" s="37" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="O35" s="37"/>
       <c r="P35" s="37"/>
@@ -3604,7 +3604,7 @@
       <c r="R35" s="37"/>
       <c r="S35" s="37"/>
       <c r="T35" s="44" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="U35" s="37"/>
       <c r="V35" s="37"/>
@@ -3648,33 +3648,33 @@
       <c r="AT35" s="19"/>
       <c r="AU35" s="19"/>
       <c r="AV35" s="25" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="AW35" s="26"/>
     </row>
     <row r="36" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A36" s="15" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="37" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F36" s="37"/>
       <c r="G36" s="37"/>
       <c r="H36" s="37" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="I36" s="37"/>
       <c r="J36" s="37"/>
       <c r="K36" s="37" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="L36" s="37"/>
       <c r="M36" s="37"/>
@@ -3685,7 +3685,7 @@
       <c r="R36" s="37"/>
       <c r="S36" s="37"/>
       <c r="T36" s="44" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="U36" s="37"/>
       <c r="V36" s="37"/>
@@ -3735,46 +3735,46 @@
       <c r="AT36" s="19"/>
       <c r="AU36" s="19"/>
       <c r="AV36" s="25" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="AW36" s="26"/>
     </row>
     <row r="37" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A37" s="15" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="37"/>
       <c r="F37" s="37"/>
       <c r="G37" s="37"/>
       <c r="H37" s="37" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="I37" s="37"/>
       <c r="J37" s="37"/>
       <c r="K37" s="37" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="L37" s="37"/>
       <c r="M37" s="37"/>
       <c r="N37" s="37" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="O37" s="37"/>
       <c r="P37" s="37"/>
       <c r="Q37" s="37" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="R37" s="37"/>
       <c r="S37" s="37"/>
       <c r="T37" s="44" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U37" s="37"/>
       <c r="V37" s="37"/>
@@ -3811,36 +3811,36 @@
       <c r="AT37" s="19"/>
       <c r="AU37" s="19"/>
       <c r="AV37" s="25" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="AW37" s="26"/>
     </row>
     <row r="38" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A38" s="15" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="37"/>
       <c r="F38" s="37"/>
       <c r="G38" s="37"/>
       <c r="H38" s="37" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="I38" s="37"/>
       <c r="J38" s="37"/>
       <c r="K38" s="37" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="L38" s="37"/>
       <c r="M38" s="37"/>
       <c r="N38" s="37" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="O38" s="37"/>
       <c r="P38" s="37"/>
@@ -3848,7 +3848,7 @@
       <c r="R38" s="37"/>
       <c r="S38" s="37"/>
       <c r="T38" s="44" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="U38" s="37"/>
       <c r="V38" s="37"/>
@@ -3886,31 +3886,31 @@
       <c r="AT38" s="19"/>
       <c r="AU38" s="19"/>
       <c r="AV38" s="25" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="AW38" s="26"/>
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A39" s="15" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="37"/>
       <c r="F39" s="37"/>
       <c r="G39" s="37"/>
       <c r="H39" s="37" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="I39" s="37"/>
       <c r="J39" s="37"/>
       <c r="K39" s="37" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="L39" s="37"/>
       <c r="M39" s="37"/>
@@ -3921,7 +3921,7 @@
       <c r="R39" s="37"/>
       <c r="S39" s="37"/>
       <c r="T39" s="44" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="U39" s="37"/>
       <c r="V39" s="37"/>
@@ -3971,31 +3971,31 @@
       <c r="AT39" s="19"/>
       <c r="AU39" s="19"/>
       <c r="AV39" s="25" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="AW39" s="26"/>
     </row>
     <row r="40" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A40" s="15" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="37"/>
       <c r="F40" s="37"/>
       <c r="G40" s="37"/>
       <c r="H40" s="37" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="I40" s="37"/>
       <c r="J40" s="37"/>
       <c r="K40" s="37" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="L40" s="37"/>
       <c r="M40" s="37"/>
@@ -4006,7 +4006,7 @@
       <c r="R40" s="37"/>
       <c r="S40" s="37"/>
       <c r="T40" s="44" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="U40" s="37"/>
       <c r="V40" s="37"/>
@@ -4039,33 +4039,33 @@
       <c r="AT40" s="19"/>
       <c r="AU40" s="19"/>
       <c r="AV40" s="25" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="AW40" s="26"/>
     </row>
     <row r="41" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A41" s="15" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="37" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F41" s="37"/>
       <c r="G41" s="37"/>
       <c r="H41" s="37" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="I41" s="37"/>
       <c r="J41" s="37"/>
       <c r="K41" s="37" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="L41" s="37"/>
       <c r="M41" s="37"/>
@@ -4076,7 +4076,7 @@
       <c r="R41" s="37"/>
       <c r="S41" s="37"/>
       <c r="T41" s="44" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="U41" s="37"/>
       <c r="V41" s="37"/>
@@ -4115,33 +4115,33 @@
       <c r="AT41" s="19"/>
       <c r="AU41" s="19"/>
       <c r="AV41" s="25" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="AW41" s="26"/>
     </row>
     <row r="42" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A42" s="15" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="37" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F42" s="37"/>
       <c r="G42" s="37"/>
       <c r="H42" s="37" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="I42" s="37"/>
       <c r="J42" s="37"/>
       <c r="K42" s="37" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="L42" s="37"/>
       <c r="M42" s="37"/>
@@ -4152,7 +4152,7 @@
       <c r="R42" s="37"/>
       <c r="S42" s="37"/>
       <c r="T42" s="44" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="U42" s="37"/>
       <c r="V42" s="37"/>
@@ -4202,27 +4202,27 @@
     </row>
     <row r="43" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A43" s="15" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="37" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F43" s="37"/>
       <c r="G43" s="37"/>
       <c r="H43" s="37" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I43" s="37"/>
       <c r="J43" s="37"/>
       <c r="K43" s="37" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="L43" s="37"/>
       <c r="M43" s="37"/>
@@ -4233,7 +4233,7 @@
       <c r="R43" s="37"/>
       <c r="S43" s="37"/>
       <c r="T43" s="44" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="U43" s="37"/>
       <c r="V43" s="37"/>
@@ -4282,27 +4282,27 @@
     </row>
     <row r="44" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A44" s="15" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="37" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F44" s="37"/>
       <c r="G44" s="37"/>
       <c r="H44" s="37" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="I44" s="37"/>
       <c r="J44" s="37"/>
       <c r="K44" s="37" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="L44" s="37"/>
       <c r="M44" s="37"/>
@@ -4313,7 +4313,7 @@
       <c r="R44" s="37"/>
       <c r="S44" s="37"/>
       <c r="T44" s="44" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="U44" s="37"/>
       <c r="V44" s="37"/>
@@ -4362,30 +4362,30 @@
     </row>
     <row r="45" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A45" s="15" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="6" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="37" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F45" s="37"/>
       <c r="G45" s="37"/>
       <c r="H45" s="37" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="I45" s="37"/>
       <c r="J45" s="37"/>
       <c r="K45" s="41" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="L45" s="42"/>
       <c r="M45" s="43"/>
       <c r="N45" s="41" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="O45" s="42"/>
       <c r="P45" s="43"/>
@@ -4393,7 +4393,7 @@
       <c r="R45" s="37"/>
       <c r="S45" s="37"/>
       <c r="T45" s="37" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="U45" s="37"/>
       <c r="V45" s="37"/>
@@ -4443,7 +4443,7 @@
     </row>
     <row r="46" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A46" s="15" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="6">
@@ -4451,22 +4451,22 @@
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="37" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="F46" s="37"/>
       <c r="G46" s="37"/>
       <c r="H46" s="37" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="I46" s="37"/>
       <c r="J46" s="37"/>
       <c r="K46" s="37" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="L46" s="37"/>
       <c r="M46" s="37"/>
       <c r="N46" s="37" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="O46" s="37"/>
       <c r="P46" s="37"/>
@@ -4474,7 +4474,7 @@
       <c r="R46" s="37"/>
       <c r="S46" s="37"/>
       <c r="T46" s="37" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="U46" s="37"/>
       <c r="V46" s="37"/>
@@ -4514,7 +4514,7 @@
     </row>
     <row r="47" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A47" s="15" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="6">
@@ -4522,22 +4522,22 @@
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="37" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="F47" s="37"/>
       <c r="G47" s="37"/>
       <c r="H47" s="37" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="I47" s="37"/>
       <c r="J47" s="37"/>
       <c r="K47" s="37" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="L47" s="37"/>
       <c r="M47" s="37"/>
       <c r="N47" s="41" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="O47" s="42"/>
       <c r="P47" s="43"/>
@@ -4545,7 +4545,7 @@
       <c r="R47" s="37"/>
       <c r="S47" s="37"/>
       <c r="T47" s="37" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="U47" s="37"/>
       <c r="V47" s="37"/>
@@ -4585,7 +4585,7 @@
     </row>
     <row r="48" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A48" s="15" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="6">
@@ -4593,32 +4593,32 @@
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="37" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="F48" s="37"/>
       <c r="G48" s="37"/>
       <c r="H48" s="37" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="I48" s="37"/>
       <c r="J48" s="37"/>
       <c r="K48" s="37" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="L48" s="37"/>
       <c r="M48" s="37"/>
       <c r="N48" s="37" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="O48" s="37"/>
       <c r="P48" s="37"/>
       <c r="Q48" s="37" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="R48" s="37"/>
       <c r="S48" s="37"/>
       <c r="T48" s="37" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="U48" s="37"/>
       <c r="V48" s="37"/>
@@ -4658,7 +4658,7 @@
     </row>
     <row r="49" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A49" s="15" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="6">
@@ -4668,32 +4668,32 @@
         <v>10</v>
       </c>
       <c r="E49" s="37" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="F49" s="37"/>
       <c r="G49" s="37"/>
       <c r="H49" s="37" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="I49" s="37"/>
       <c r="J49" s="37"/>
       <c r="K49" s="37" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="L49" s="37"/>
       <c r="M49" s="37"/>
       <c r="N49" s="37" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="O49" s="37"/>
       <c r="P49" s="37"/>
       <c r="Q49" s="37" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="R49" s="37"/>
       <c r="S49" s="37"/>
       <c r="T49" s="44" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="U49" s="37"/>
       <c r="V49" s="37"/>
@@ -4701,7 +4701,7 @@
       <c r="X49" s="37"/>
       <c r="Y49" s="37"/>
       <c r="Z49" s="6" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="AA49" s="6"/>
       <c r="AB49" s="19"/>
@@ -4917,7 +4917,7 @@
       <c r="AG53" s="19"/>
       <c r="AH53" s="19"/>
       <c r="AI53" s="19"/>
-      <c r="AJ53" s="19"/>
+      <c r="AJ53" s="27"/>
       <c r="AK53" s="19"/>
       <c r="AL53" s="19"/>
       <c r="AM53" s="19"/>
@@ -5494,25 +5494,25 @@
     </row>
     <row r="65" spans="1:50" x14ac:dyDescent="0.45">
       <c r="A65" s="15" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="6" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E65" s="37"/>
       <c r="F65" s="37"/>
       <c r="G65" s="37"/>
       <c r="H65" s="37" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="I65" s="37"/>
       <c r="J65" s="37"/>
       <c r="K65" s="37" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="L65" s="37"/>
       <c r="M65" s="37"/>
@@ -5523,7 +5523,7 @@
       <c r="R65" s="37"/>
       <c r="S65" s="37"/>
       <c r="T65" s="44" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="U65" s="37"/>
       <c r="V65" s="37"/>
@@ -5556,27 +5556,27 @@
     </row>
     <row r="66" spans="1:50" x14ac:dyDescent="0.45">
       <c r="A66" s="15" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="6" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E66" s="37" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="F66" s="37"/>
       <c r="G66" s="37"/>
       <c r="H66" s="37" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="I66" s="37"/>
       <c r="J66" s="37"/>
       <c r="K66" s="37" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="L66" s="37"/>
       <c r="M66" s="37"/>
@@ -5587,7 +5587,7 @@
       <c r="R66" s="37"/>
       <c r="S66" s="37"/>
       <c r="T66" s="44" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="U66" s="37"/>
       <c r="V66" s="37"/>
@@ -5621,32 +5621,32 @@
     </row>
     <row r="67" spans="1:50" x14ac:dyDescent="0.45">
       <c r="A67" s="15" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="6" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="E67" s="37" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="F67" s="37"/>
       <c r="G67" s="37"/>
       <c r="H67" s="37" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="I67" s="37"/>
       <c r="J67" s="37"/>
       <c r="K67" s="37" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="L67" s="37"/>
       <c r="M67" s="37"/>
       <c r="N67" s="37" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="O67" s="37"/>
       <c r="P67" s="37"/>
@@ -5654,7 +5654,7 @@
       <c r="R67" s="37"/>
       <c r="S67" s="37"/>
       <c r="T67" s="37" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="U67" s="37"/>
       <c r="V67" s="37"/>
@@ -5877,7 +5877,7 @@
       <c r="AT71" s="19"/>
       <c r="AU71" s="19"/>
       <c r="AV71" s="25" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="AW71" s="26"/>
       <c r="AX71" s="26"/>
@@ -7455,7 +7455,7 @@
     </row>
     <row r="104" spans="1:50" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -7480,167 +7480,167 @@
     </row>
     <row r="105" spans="1:50" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B105" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="106" spans="1:50" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B106" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="107" spans="1:50" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B107" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="108" spans="1:50" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B108" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="109" spans="1:50" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="B109" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="110" spans="1:50" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B110" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="111" spans="1:50" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B111" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="112" spans="1:50" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B112" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B113" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B114" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B115" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B116" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B117" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B120" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B121" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B122" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B123" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B124" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B125" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B126" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B130" s="14" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C130" s="14"/>
     </row>
@@ -7649,10 +7649,10 @@
         <v>3</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C131" s="38" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D131" s="38"/>
       <c r="E131" s="1"/>
@@ -7675,13 +7675,13 @@
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A132" s="6" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B132" s="6">
         <v>2</v>
       </c>
       <c r="C132" s="25" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="D132" s="25"/>
       <c r="E132" s="25"/>
@@ -7704,13 +7704,13 @@
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A133" s="6" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B133" s="6">
         <v>2</v>
       </c>
       <c r="C133" s="25" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D133" s="25"/>
       <c r="E133" s="25"/>
@@ -7733,13 +7733,13 @@
     </row>
     <row r="134" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A134" s="6" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B134" s="6">
         <v>1</v>
       </c>
       <c r="C134" s="25" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D134" s="25"/>
       <c r="E134" s="25"/>
@@ -7762,13 +7762,13 @@
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A135" s="6" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B135" s="6">
         <v>3</v>
       </c>
       <c r="C135" s="25" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D135" s="25"/>
       <c r="E135" s="25"/>
@@ -7791,13 +7791,13 @@
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A136" s="6" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B136" s="6">
         <v>3</v>
       </c>
       <c r="C136" s="25" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D136" s="25"/>
       <c r="E136" s="25"/>
@@ -7820,13 +7820,13 @@
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A137" s="6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B137" s="6">
         <v>3</v>
       </c>
       <c r="C137" s="25" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D137" s="25"/>
       <c r="E137" s="25"/>
@@ -7849,13 +7849,13 @@
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A138" s="6" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B138" s="6">
         <v>3</v>
       </c>
       <c r="C138" s="25" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D138" s="25"/>
       <c r="E138" s="25"/>
@@ -7878,13 +7878,13 @@
     </row>
     <row r="139" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A139" s="6" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B139" s="6">
         <v>2</v>
       </c>
       <c r="C139" s="25" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D139" s="25"/>
       <c r="E139" s="25"/>
@@ -7907,13 +7907,13 @@
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A140" s="6" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B140" s="6">
         <v>2</v>
       </c>
       <c r="C140" s="25" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D140" s="25"/>
       <c r="E140" s="25"/>
@@ -7936,13 +7936,13 @@
     </row>
     <row r="141" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A141" s="6" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B141" s="6">
         <v>2</v>
       </c>
       <c r="C141" s="25" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D141" s="25"/>
       <c r="E141" s="25"/>
@@ -7965,13 +7965,13 @@
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A142" s="6" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B142" s="6">
         <v>1</v>
       </c>
       <c r="C142" s="25" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D142" s="25"/>
       <c r="E142" s="25"/>
@@ -7994,13 +7994,13 @@
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A143" s="6" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B143" s="6">
         <v>1</v>
       </c>
       <c r="C143" s="25" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="D143" s="25"/>
       <c r="E143" s="25"/>
@@ -8023,13 +8023,13 @@
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A144" s="6" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B144" s="6">
         <v>2</v>
       </c>
       <c r="C144" s="25" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D144" s="25"/>
       <c r="E144" s="25"/>
@@ -8052,13 +8052,13 @@
     </row>
     <row r="145" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A145" s="6" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B145" s="6">
         <v>2</v>
       </c>
       <c r="C145" s="25" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D145" s="25"/>
       <c r="E145" s="25"/>
@@ -8081,13 +8081,13 @@
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A146" s="6" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B146" s="6">
         <v>2</v>
       </c>
       <c r="C146" s="25" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D146" s="25"/>
       <c r="E146" s="25"/>
@@ -8110,13 +8110,13 @@
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A147" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B147" s="6">
         <v>1</v>
       </c>
       <c r="C147" s="25" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="D147" s="25"/>
       <c r="E147" s="25"/>
@@ -8139,13 +8139,13 @@
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A148" s="6" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B148" s="6">
         <v>2</v>
       </c>
       <c r="C148" s="25" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D148" s="25"/>
       <c r="E148" s="25"/>
@@ -8168,13 +8168,13 @@
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A149" s="6" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B149" s="6">
         <v>2</v>
       </c>
       <c r="C149" s="25" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="D149" s="25"/>
       <c r="E149" s="25"/>
@@ -8197,13 +8197,13 @@
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A150" s="6" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B150" s="6">
         <v>2</v>
       </c>
       <c r="C150" s="25" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D150" s="25"/>
       <c r="E150" s="25"/>
@@ -8226,13 +8226,13 @@
     </row>
     <row r="151" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A151" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B151" s="6">
         <v>2</v>
       </c>
       <c r="C151" s="25" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D151" s="25"/>
       <c r="E151" s="25"/>
@@ -8255,13 +8255,13 @@
     </row>
     <row r="152" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A152" s="6" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B152" s="6">
         <v>2</v>
       </c>
       <c r="C152" s="25" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="D152" s="25"/>
       <c r="E152" s="25"/>
@@ -8284,13 +8284,13 @@
     </row>
     <row r="153" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A153" s="6" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="B153" s="6">
         <v>2</v>
       </c>
       <c r="C153" s="25" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="D153" s="25"/>
       <c r="E153" s="25"/>
@@ -8313,13 +8313,13 @@
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A154" s="6" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B154" s="6">
         <v>2</v>
       </c>
       <c r="C154" s="25" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D154" s="25"/>
       <c r="E154" s="25"/>
@@ -8342,13 +8342,13 @@
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A155" s="6" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B155" s="6">
         <v>2</v>
       </c>
       <c r="C155" s="25" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D155" s="25"/>
       <c r="E155" s="25"/>

</xml_diff>

<commit_message>
Balance patch: nerfed tilted scale
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\PycharmProjects\dice_game_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32742412-5E48-496A-8715-0B0B965903C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0CB60C-773C-42EE-91D1-25BB4A0E6D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23650" yWindow="0" windowWidth="14810" windowHeight="21690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22500" yWindow="0" windowWidth="14810" windowHeight="21690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="401">
   <si>
     <t>Mobs</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1583,10 +1583,6 @@
     <t>refresh - 모든 상태이상 제거</t>
   </si>
   <si>
-    <t>매 턴 뽑은 공격타일 하나당 모든 적에게 5의 데미지를 준다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>매 턴 뽑은 방어타일 하나당 5의 방어도를 얻는다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1599,18 +1595,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>매 턴 뽑은 공격타일 하나당 가장 가까운 적에게 5의 데미지를 준다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>bag of dagger</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>전투 시작시 모든 적이 피해를 5받는다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>O</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1628,6 +1616,26 @@
   </si>
   <si>
     <t>공격 받을때마다 +1 추가 공격력을 얻는다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clover</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유적에서 전설등급 이상의 유물이 나타날 확률이 크게 증가한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전투 시작시 모든 적이 피해를 2받는다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매 턴 뽑은 공격타일 하나당 가장 가까운 적에게 1의 데미지를 준다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매 턴 뽑은 공격타일 하나당 모든 적에게 1의 데미지를 준다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2057,7 +2065,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2198,82 +2206,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2306,6 +2242,12 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2315,6 +2257,76 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -2602,8 +2614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BP254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E138" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q161" sqref="Q161"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I146" sqref="I146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -2741,84 +2753,84 @@
       <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="85" t="s">
+      <c r="L9" s="61" t="s">
         <v>158</v>
       </c>
-      <c r="M9" s="85"/>
-      <c r="N9" s="85"/>
-      <c r="O9" s="85"/>
-      <c r="P9" s="85"/>
-      <c r="Q9" s="85"/>
-      <c r="R9" s="85"/>
-      <c r="S9" s="85"/>
-      <c r="T9" s="85" t="s">
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="61"/>
+      <c r="S9" s="61"/>
+      <c r="T9" s="61" t="s">
         <v>159</v>
       </c>
-      <c r="U9" s="85"/>
-      <c r="V9" s="85"/>
-      <c r="W9" s="85"/>
-      <c r="X9" s="85"/>
-      <c r="Y9" s="85"/>
-      <c r="Z9" s="85"/>
-      <c r="AA9" s="85"/>
-      <c r="AB9" s="85" t="s">
+      <c r="U9" s="61"/>
+      <c r="V9" s="61"/>
+      <c r="W9" s="61"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="61"/>
+      <c r="Z9" s="61"/>
+      <c r="AA9" s="61"/>
+      <c r="AB9" s="61" t="s">
         <v>160</v>
       </c>
-      <c r="AC9" s="85"/>
-      <c r="AD9" s="85"/>
-      <c r="AE9" s="85"/>
-      <c r="AF9" s="85"/>
-      <c r="AG9" s="85"/>
-      <c r="AH9" s="85"/>
-      <c r="AI9" s="85"/>
+      <c r="AC9" s="61"/>
+      <c r="AD9" s="61"/>
+      <c r="AE9" s="61"/>
+      <c r="AF9" s="61"/>
+      <c r="AG9" s="61"/>
+      <c r="AH9" s="61"/>
+      <c r="AI9" s="61"/>
       <c r="AL9" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:38">
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="L10" s="67" t="s">
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="L10" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="67"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="67"/>
-      <c r="P10" s="67" t="s">
+      <c r="M10" s="79"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="79"/>
+      <c r="P10" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="67"/>
-      <c r="S10" s="67"/>
-      <c r="T10" s="67" t="s">
+      <c r="Q10" s="79"/>
+      <c r="R10" s="79"/>
+      <c r="S10" s="79"/>
+      <c r="T10" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="U10" s="67"/>
-      <c r="V10" s="67"/>
-      <c r="W10" s="67"/>
-      <c r="X10" s="67" t="s">
+      <c r="U10" s="79"/>
+      <c r="V10" s="79"/>
+      <c r="W10" s="79"/>
+      <c r="X10" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="Y10" s="67"/>
-      <c r="Z10" s="67"/>
-      <c r="AA10" s="67"/>
-      <c r="AB10" s="67" t="s">
+      <c r="Y10" s="79"/>
+      <c r="Z10" s="79"/>
+      <c r="AA10" s="79"/>
+      <c r="AB10" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="AC10" s="67"/>
-      <c r="AD10" s="67"/>
-      <c r="AE10" s="67"/>
-      <c r="AF10" s="67" t="s">
+      <c r="AC10" s="79"/>
+      <c r="AD10" s="79"/>
+      <c r="AE10" s="79"/>
+      <c r="AF10" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="AG10" s="67"/>
-      <c r="AH10" s="67"/>
-      <c r="AI10" s="67"/>
+      <c r="AG10" s="79"/>
+      <c r="AH10" s="79"/>
+      <c r="AI10" s="79"/>
       <c r="AJ10" s="24" t="s">
         <v>103</v>
       </c>
@@ -2851,71 +2863,71 @@
       <c r="G11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H11" s="52" t="s">
+      <c r="H11" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52" t="s">
+      <c r="I11" s="67"/>
+      <c r="J11" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="52"/>
+      <c r="K11" s="67"/>
       <c r="L11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="52" t="s">
+      <c r="M11" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="N11" s="52"/>
+      <c r="N11" s="67"/>
       <c r="O11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="P11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="Q11" s="52" t="s">
+      <c r="Q11" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="52"/>
+      <c r="R11" s="67"/>
       <c r="S11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="T11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="U11" s="52" t="s">
+      <c r="U11" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="V11" s="52"/>
+      <c r="V11" s="67"/>
       <c r="W11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="X11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="Y11" s="52" t="s">
+      <c r="Y11" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="Z11" s="52"/>
+      <c r="Z11" s="67"/>
       <c r="AA11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="AB11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AC11" s="52" t="s">
+      <c r="AC11" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="AD11" s="52"/>
+      <c r="AD11" s="67"/>
       <c r="AE11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="AF11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AG11" s="52" t="s">
+      <c r="AG11" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="AH11" s="52"/>
+      <c r="AH11" s="67"/>
       <c r="AI11" s="1" t="s">
         <v>14</v>
       </c>
@@ -2945,10 +2957,10 @@
         <v>4</v>
       </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="57" t="s">
+      <c r="H12" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="58"/>
+      <c r="I12" s="74"/>
       <c r="J12" s="62" t="s">
         <v>26</v>
       </c>
@@ -2956,8 +2968,8 @@
       <c r="L12" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="M12" s="63"/>
-      <c r="N12" s="63"/>
+      <c r="M12" s="75"/>
+      <c r="N12" s="75"/>
       <c r="O12" s="10"/>
       <c r="P12" s="9" t="s">
         <v>88</v>
@@ -3009,10 +3021,10 @@
       <c r="G13" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H13" s="57" t="s">
+      <c r="H13" s="72" t="s">
         <v>375</v>
       </c>
-      <c r="I13" s="58"/>
+      <c r="I13" s="74"/>
       <c r="J13" s="62" t="s">
         <v>25</v>
       </c>
@@ -3020,8 +3032,8 @@
       <c r="L13" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="M13" s="63"/>
-      <c r="N13" s="63"/>
+      <c r="M13" s="75"/>
+      <c r="N13" s="75"/>
       <c r="O13" s="10"/>
       <c r="P13" s="9" t="s">
         <v>290</v>
@@ -3076,10 +3088,10 @@
         <v>4</v>
       </c>
       <c r="G14" s="6"/>
-      <c r="H14" s="57" t="s">
+      <c r="H14" s="72" t="s">
         <v>376</v>
       </c>
-      <c r="I14" s="58"/>
+      <c r="I14" s="74"/>
       <c r="J14" s="62" t="s">
         <v>377</v>
       </c>
@@ -3087,8 +3099,8 @@
       <c r="L14" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="M14" s="63"/>
-      <c r="N14" s="63"/>
+      <c r="M14" s="75"/>
+      <c r="N14" s="75"/>
       <c r="O14" s="10"/>
       <c r="P14" s="9" t="s">
         <v>100</v>
@@ -3137,17 +3149,17 @@
         <v>6</v>
       </c>
       <c r="G15" s="6"/>
-      <c r="H15" s="57" t="s">
+      <c r="H15" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="58"/>
+      <c r="I15" s="74"/>
       <c r="J15" s="62"/>
       <c r="K15" s="62"/>
       <c r="L15" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="M15" s="63"/>
-      <c r="N15" s="63"/>
+      <c r="M15" s="75"/>
+      <c r="N15" s="75"/>
       <c r="O15" s="10"/>
       <c r="P15" s="9" t="s">
         <v>97</v>
@@ -3204,19 +3216,19 @@
       <c r="G16" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H16" s="64" t="s">
+      <c r="H16" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="66"/>
-      <c r="J16" s="64" t="s">
+      <c r="I16" s="51"/>
+      <c r="J16" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="66"/>
+      <c r="K16" s="51"/>
       <c r="L16" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="M16" s="63"/>
-      <c r="N16" s="63"/>
+      <c r="M16" s="75"/>
+      <c r="N16" s="75"/>
       <c r="O16" s="10"/>
       <c r="P16" s="9" t="s">
         <v>91</v>
@@ -3271,10 +3283,10 @@
         <v>4</v>
       </c>
       <c r="G17" s="6"/>
-      <c r="H17" s="57" t="s">
+      <c r="H17" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="I17" s="58"/>
+      <c r="I17" s="74"/>
       <c r="J17" s="62" t="s">
         <v>31</v>
       </c>
@@ -3282,8 +3294,8 @@
       <c r="L17" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="M17" s="63"/>
-      <c r="N17" s="63"/>
+      <c r="M17" s="75"/>
+      <c r="N17" s="75"/>
       <c r="O17" s="10"/>
       <c r="P17" s="27" t="s">
         <v>172</v>
@@ -3346,17 +3358,17 @@
         <v>7</v>
       </c>
       <c r="G18" s="6"/>
-      <c r="H18" s="57" t="s">
+      <c r="H18" s="72" t="s">
         <v>374</v>
       </c>
-      <c r="I18" s="58"/>
+      <c r="I18" s="74"/>
       <c r="J18" s="62" t="s">
         <v>102</v>
       </c>
       <c r="K18" s="62"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="63"/>
-      <c r="N18" s="63"/>
+      <c r="M18" s="75"/>
+      <c r="N18" s="75"/>
       <c r="O18" s="10"/>
       <c r="P18" s="9"/>
       <c r="Q18" s="62"/>
@@ -3392,13 +3404,13 @@
       <c r="E19" s="6"/>
       <c r="F19" s="11"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="58"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="74"/>
       <c r="J19" s="62"/>
       <c r="K19" s="62"/>
       <c r="L19" s="5"/>
-      <c r="M19" s="63"/>
-      <c r="N19" s="63"/>
+      <c r="M19" s="75"/>
+      <c r="N19" s="75"/>
       <c r="O19" s="10"/>
       <c r="P19" s="9"/>
       <c r="Q19" s="62"/>
@@ -3434,13 +3446,13 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58"/>
+      <c r="H20" s="72"/>
+      <c r="I20" s="74"/>
       <c r="J20" s="62"/>
       <c r="K20" s="62"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="63"/>
-      <c r="N20" s="63"/>
+      <c r="M20" s="75"/>
+      <c r="N20" s="75"/>
       <c r="O20" s="10"/>
       <c r="P20" s="9"/>
       <c r="Q20" s="62"/>
@@ -3476,13 +3488,13 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="58"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="74"/>
       <c r="J21" s="62"/>
       <c r="K21" s="62"/>
       <c r="L21" s="5"/>
-      <c r="M21" s="63"/>
-      <c r="N21" s="63"/>
+      <c r="M21" s="75"/>
+      <c r="N21" s="75"/>
       <c r="O21" s="10"/>
       <c r="P21" s="9"/>
       <c r="Q21" s="62"/>
@@ -3533,13 +3545,13 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="58"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="74"/>
       <c r="J22" s="62"/>
       <c r="K22" s="62"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="63"/>
-      <c r="N22" s="63"/>
+      <c r="M22" s="75"/>
+      <c r="N22" s="75"/>
       <c r="O22" s="10"/>
       <c r="P22" s="9"/>
       <c r="Q22" s="62"/>
@@ -3576,13 +3588,13 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="58"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="74"/>
       <c r="J23" s="62"/>
       <c r="K23" s="62"/>
       <c r="L23" s="5"/>
-      <c r="M23" s="63"/>
-      <c r="N23" s="63"/>
+      <c r="M23" s="75"/>
+      <c r="N23" s="75"/>
       <c r="O23" s="10"/>
       <c r="P23" s="9"/>
       <c r="Q23" s="62"/>
@@ -3619,13 +3631,13 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="58"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="74"/>
       <c r="J24" s="62"/>
       <c r="K24" s="62"/>
       <c r="L24" s="5"/>
-      <c r="M24" s="63"/>
-      <c r="N24" s="63"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="75"/>
       <c r="O24" s="10"/>
       <c r="P24" s="9"/>
       <c r="Q24" s="62"/>
@@ -3655,45 +3667,45 @@
       <c r="AW24" s="20"/>
     </row>
     <row r="25" spans="1:67">
-      <c r="A25" s="82" t="s">
+      <c r="A25" s="58" t="s">
         <v>211</v>
       </c>
-      <c r="B25" s="83"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
-      <c r="H25" s="83"/>
-      <c r="I25" s="83"/>
-      <c r="J25" s="83"/>
-      <c r="K25" s="83"/>
-      <c r="L25" s="83"/>
-      <c r="M25" s="83"/>
-      <c r="N25" s="83"/>
-      <c r="O25" s="83"/>
-      <c r="P25" s="83"/>
-      <c r="Q25" s="83"/>
-      <c r="R25" s="83"/>
-      <c r="S25" s="83"/>
-      <c r="T25" s="83"/>
-      <c r="U25" s="83"/>
-      <c r="V25" s="83"/>
-      <c r="W25" s="83"/>
-      <c r="X25" s="83"/>
-      <c r="Y25" s="83"/>
-      <c r="Z25" s="83"/>
-      <c r="AA25" s="83"/>
-      <c r="AB25" s="83"/>
-      <c r="AC25" s="83"/>
-      <c r="AD25" s="83"/>
-      <c r="AE25" s="83"/>
-      <c r="AF25" s="83"/>
-      <c r="AG25" s="83"/>
-      <c r="AH25" s="83"/>
-      <c r="AI25" s="83"/>
-      <c r="AJ25" s="83"/>
-      <c r="AK25" s="84"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="59"/>
+      <c r="T25" s="59"/>
+      <c r="U25" s="59"/>
+      <c r="V25" s="59"/>
+      <c r="W25" s="59"/>
+      <c r="X25" s="59"/>
+      <c r="Y25" s="59"/>
+      <c r="Z25" s="59"/>
+      <c r="AA25" s="59"/>
+      <c r="AB25" s="59"/>
+      <c r="AC25" s="59"/>
+      <c r="AD25" s="59"/>
+      <c r="AE25" s="59"/>
+      <c r="AF25" s="59"/>
+      <c r="AG25" s="59"/>
+      <c r="AH25" s="59"/>
+      <c r="AI25" s="59"/>
+      <c r="AJ25" s="59"/>
+      <c r="AK25" s="60"/>
       <c r="AV25" s="19" t="s">
         <v>122</v>
       </c>
@@ -3709,15 +3721,15 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="58"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="74"/>
       <c r="J26" s="62"/>
       <c r="K26" s="62"/>
       <c r="L26" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="M26" s="63"/>
-      <c r="N26" s="63"/>
+      <c r="M26" s="75"/>
+      <c r="N26" s="75"/>
       <c r="O26" s="10"/>
       <c r="P26" s="9"/>
       <c r="Q26" s="62"/>
@@ -3756,13 +3768,13 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="58"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="74"/>
       <c r="J27" s="62"/>
       <c r="K27" s="62"/>
       <c r="L27" s="5"/>
-      <c r="M27" s="63"/>
-      <c r="N27" s="63"/>
+      <c r="M27" s="75"/>
+      <c r="N27" s="75"/>
       <c r="O27" s="10"/>
       <c r="P27" s="9"/>
       <c r="Q27" s="62"/>
@@ -3777,7 +3789,7 @@
       <c r="Z27" s="62"/>
       <c r="AA27" s="10"/>
       <c r="AB27" s="9" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="AC27" s="62"/>
       <c r="AD27" s="62"/>
@@ -3803,15 +3815,15 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="58"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="74"/>
       <c r="J28" s="62"/>
       <c r="K28" s="62"/>
       <c r="L28" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="M28" s="63"/>
-      <c r="N28" s="63"/>
+      <c r="M28" s="75"/>
+      <c r="N28" s="75"/>
       <c r="O28" s="10"/>
       <c r="P28" s="9"/>
       <c r="Q28" s="62"/>
@@ -3846,7 +3858,7 @@
     </row>
     <row r="29" spans="1:67">
       <c r="A29" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="AV29" s="19" t="s">
         <v>121</v>
@@ -3866,48 +3878,48 @@
       <c r="T31" t="s">
         <v>154</v>
       </c>
-      <c r="AB31" s="52" t="s">
+      <c r="AB31" s="67" t="s">
         <v>111</v>
       </c>
-      <c r="AC31" s="52"/>
-      <c r="AD31" s="52"/>
-      <c r="AE31" s="52"/>
-      <c r="AF31" s="52"/>
-      <c r="AG31" s="52"/>
-      <c r="AH31" s="52"/>
-      <c r="AI31" s="52"/>
-      <c r="AJ31" s="52"/>
-      <c r="AK31" s="52"/>
-      <c r="AL31" s="52"/>
-      <c r="AM31" s="52"/>
-      <c r="AN31" s="52"/>
-      <c r="AO31" s="52"/>
-      <c r="AP31" s="52"/>
-      <c r="AQ31" s="52"/>
-      <c r="AR31" s="52"/>
-      <c r="AS31" s="52"/>
-      <c r="AT31" s="52"/>
-      <c r="AU31" s="52"/>
-      <c r="AV31" s="52"/>
-      <c r="AW31" s="52"/>
-      <c r="AX31" s="52"/>
-      <c r="AY31" s="52"/>
-      <c r="AZ31" s="52"/>
-      <c r="BA31" s="52"/>
-      <c r="BB31" s="52"/>
-      <c r="BC31" s="52"/>
-      <c r="BD31" s="52"/>
-      <c r="BE31" s="52"/>
-      <c r="BF31" s="52"/>
-      <c r="BG31" s="52"/>
-      <c r="BH31" s="52"/>
-      <c r="BI31" s="52"/>
-      <c r="BJ31" s="52"/>
-      <c r="BK31" s="52"/>
-      <c r="BL31" s="52"/>
-      <c r="BM31" s="52"/>
-      <c r="BN31" s="52"/>
-      <c r="BO31" s="52"/>
+      <c r="AC31" s="67"/>
+      <c r="AD31" s="67"/>
+      <c r="AE31" s="67"/>
+      <c r="AF31" s="67"/>
+      <c r="AG31" s="67"/>
+      <c r="AH31" s="67"/>
+      <c r="AI31" s="67"/>
+      <c r="AJ31" s="67"/>
+      <c r="AK31" s="67"/>
+      <c r="AL31" s="67"/>
+      <c r="AM31" s="67"/>
+      <c r="AN31" s="67"/>
+      <c r="AO31" s="67"/>
+      <c r="AP31" s="67"/>
+      <c r="AQ31" s="67"/>
+      <c r="AR31" s="67"/>
+      <c r="AS31" s="67"/>
+      <c r="AT31" s="67"/>
+      <c r="AU31" s="67"/>
+      <c r="AV31" s="67"/>
+      <c r="AW31" s="67"/>
+      <c r="AX31" s="67"/>
+      <c r="AY31" s="67"/>
+      <c r="AZ31" s="67"/>
+      <c r="BA31" s="67"/>
+      <c r="BB31" s="67"/>
+      <c r="BC31" s="67"/>
+      <c r="BD31" s="67"/>
+      <c r="BE31" s="67"/>
+      <c r="BF31" s="67"/>
+      <c r="BG31" s="67"/>
+      <c r="BH31" s="67"/>
+      <c r="BI31" s="67"/>
+      <c r="BJ31" s="67"/>
+      <c r="BK31" s="67"/>
+      <c r="BL31" s="67"/>
+      <c r="BM31" s="67"/>
+      <c r="BN31" s="67"/>
+      <c r="BO31" s="67"/>
     </row>
     <row r="32" spans="1:67">
       <c r="A32" s="1" t="s">
@@ -3922,39 +3934,39 @@
       <c r="D32" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E32" s="52" t="s">
+      <c r="E32" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52" t="s">
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52" t="s">
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
-      <c r="N32" s="52" t="s">
+      <c r="L32" s="67"/>
+      <c r="M32" s="67"/>
+      <c r="N32" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="O32" s="52"/>
-      <c r="P32" s="52"/>
-      <c r="Q32" s="52" t="s">
+      <c r="O32" s="67"/>
+      <c r="P32" s="67"/>
+      <c r="Q32" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="R32" s="52"/>
-      <c r="S32" s="52"/>
-      <c r="T32" s="52" t="s">
+      <c r="R32" s="67"/>
+      <c r="S32" s="67"/>
+      <c r="T32" s="67" t="s">
         <v>108</v>
       </c>
-      <c r="U32" s="52"/>
-      <c r="V32" s="52"/>
-      <c r="W32" s="52"/>
-      <c r="X32" s="52"/>
-      <c r="Y32" s="52"/>
+      <c r="U32" s="67"/>
+      <c r="V32" s="67"/>
+      <c r="W32" s="67"/>
+      <c r="X32" s="67"/>
+      <c r="Y32" s="67"/>
       <c r="Z32" s="1" t="s">
         <v>109</v>
       </c>
@@ -4054,82 +4066,82 @@
       <c r="BF32" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="BG32" s="52" t="s">
+      <c r="BG32" s="67" t="s">
         <v>215</v>
       </c>
-      <c r="BH32" s="52"/>
-      <c r="BI32" s="52"/>
-      <c r="BJ32" s="52"/>
-      <c r="BK32" s="52"/>
-      <c r="BL32" s="52"/>
-      <c r="BM32" s="52"/>
-      <c r="BN32" s="52"/>
-      <c r="BO32" s="52"/>
+      <c r="BH32" s="67"/>
+      <c r="BI32" s="67"/>
+      <c r="BJ32" s="67"/>
+      <c r="BK32" s="67"/>
+      <c r="BL32" s="67"/>
+      <c r="BM32" s="67"/>
+      <c r="BN32" s="67"/>
+      <c r="BO32" s="67"/>
     </row>
     <row r="33" spans="1:67">
-      <c r="A33" s="76" t="s">
+      <c r="A33" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="B33" s="77"/>
-      <c r="C33" s="77"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="77"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="77"/>
-      <c r="J33" s="77"/>
-      <c r="K33" s="77"/>
-      <c r="L33" s="77"/>
-      <c r="M33" s="77"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="77"/>
-      <c r="P33" s="77"/>
-      <c r="Q33" s="77"/>
-      <c r="R33" s="77"/>
-      <c r="S33" s="77"/>
-      <c r="T33" s="77"/>
-      <c r="U33" s="77"/>
-      <c r="V33" s="77"/>
-      <c r="W33" s="77"/>
-      <c r="X33" s="77"/>
-      <c r="Y33" s="77"/>
-      <c r="Z33" s="77"/>
-      <c r="AA33" s="78"/>
-      <c r="AB33" s="55" t="s">
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
+      <c r="L33" s="53"/>
+      <c r="M33" s="53"/>
+      <c r="N33" s="53"/>
+      <c r="O33" s="53"/>
+      <c r="P33" s="53"/>
+      <c r="Q33" s="53"/>
+      <c r="R33" s="53"/>
+      <c r="S33" s="53"/>
+      <c r="T33" s="53"/>
+      <c r="U33" s="53"/>
+      <c r="V33" s="53"/>
+      <c r="W33" s="53"/>
+      <c r="X33" s="53"/>
+      <c r="Y33" s="53"/>
+      <c r="Z33" s="53"/>
+      <c r="AA33" s="54"/>
+      <c r="AB33" s="86" t="s">
         <v>279</v>
       </c>
-      <c r="AC33" s="56"/>
-      <c r="AD33" s="56"/>
-      <c r="AE33" s="56"/>
-      <c r="AF33" s="54" t="s">
+      <c r="AC33" s="87"/>
+      <c r="AD33" s="87"/>
+      <c r="AE33" s="87"/>
+      <c r="AF33" s="85" t="s">
         <v>278</v>
       </c>
-      <c r="AG33" s="54"/>
-      <c r="AH33" s="54"/>
-      <c r="AI33" s="56" t="s">
+      <c r="AG33" s="85"/>
+      <c r="AH33" s="85"/>
+      <c r="AI33" s="87" t="s">
         <v>280</v>
       </c>
-      <c r="AJ33" s="56"/>
+      <c r="AJ33" s="87"/>
       <c r="AK33" s="39"/>
-      <c r="AL33" s="56" t="s">
+      <c r="AL33" s="87" t="s">
         <v>281</v>
       </c>
-      <c r="AM33" s="56"/>
-      <c r="AN33" s="56"/>
-      <c r="AO33" s="56"/>
-      <c r="AP33" s="56"/>
-      <c r="AQ33" s="56"/>
-      <c r="AR33" s="56"/>
-      <c r="AS33" s="56"/>
+      <c r="AM33" s="87"/>
+      <c r="AN33" s="87"/>
+      <c r="AO33" s="87"/>
+      <c r="AP33" s="87"/>
+      <c r="AQ33" s="87"/>
+      <c r="AR33" s="87"/>
+      <c r="AS33" s="87"/>
       <c r="AT33" s="39"/>
       <c r="AU33" s="39"/>
-      <c r="AV33" s="56" t="s">
+      <c r="AV33" s="87" t="s">
         <v>282</v>
       </c>
-      <c r="AW33" s="56"/>
-      <c r="AX33" s="56"/>
-      <c r="AY33" s="56"/>
+      <c r="AW33" s="87"/>
+      <c r="AX33" s="87"/>
+      <c r="AY33" s="87"/>
       <c r="AZ33" s="39"/>
       <c r="BA33" s="39"/>
       <c r="BB33" s="39"/>
@@ -4158,35 +4170,35 @@
       <c r="D34" s="6">
         <v>1</v>
       </c>
-      <c r="E34" s="64"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="66"/>
-      <c r="H34" s="64" t="s">
+      <c r="E34" s="50"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="50" t="s">
         <v>243</v>
       </c>
-      <c r="I34" s="65"/>
-      <c r="J34" s="66"/>
-      <c r="K34" s="64" t="s">
+      <c r="I34" s="71"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="50" t="s">
         <v>249</v>
       </c>
-      <c r="L34" s="65"/>
-      <c r="M34" s="66"/>
-      <c r="N34" s="64" t="s">
+      <c r="L34" s="71"/>
+      <c r="M34" s="51"/>
+      <c r="N34" s="50" t="s">
         <v>250</v>
       </c>
-      <c r="O34" s="65"/>
-      <c r="P34" s="66"/>
-      <c r="Q34" s="57"/>
-      <c r="R34" s="71"/>
-      <c r="S34" s="58"/>
-      <c r="T34" s="72" t="s">
+      <c r="O34" s="71"/>
+      <c r="P34" s="51"/>
+      <c r="Q34" s="72"/>
+      <c r="R34" s="73"/>
+      <c r="S34" s="74"/>
+      <c r="T34" s="68" t="s">
         <v>152</v>
       </c>
-      <c r="U34" s="73"/>
-      <c r="V34" s="73"/>
-      <c r="W34" s="73"/>
-      <c r="X34" s="73"/>
-      <c r="Y34" s="74"/>
+      <c r="U34" s="69"/>
+      <c r="V34" s="69"/>
+      <c r="W34" s="69"/>
+      <c r="X34" s="69"/>
+      <c r="Y34" s="70"/>
       <c r="Z34" s="6">
         <v>1</v>
       </c>
@@ -4223,35 +4235,35 @@
       <c r="D35" s="6">
         <v>2</v>
       </c>
-      <c r="E35" s="64" t="s">
+      <c r="E35" s="50" t="s">
         <v>251</v>
       </c>
-      <c r="F35" s="65"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="64" t="s">
+      <c r="F35" s="71"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="I35" s="65"/>
-      <c r="J35" s="66"/>
-      <c r="K35" s="64" t="s">
+      <c r="I35" s="71"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="50" t="s">
         <v>250</v>
       </c>
-      <c r="L35" s="65"/>
-      <c r="M35" s="66"/>
-      <c r="N35" s="64"/>
-      <c r="O35" s="65"/>
-      <c r="P35" s="66"/>
-      <c r="Q35" s="57"/>
-      <c r="R35" s="71"/>
-      <c r="S35" s="58"/>
-      <c r="T35" s="72" t="s">
+      <c r="L35" s="71"/>
+      <c r="M35" s="51"/>
+      <c r="N35" s="50"/>
+      <c r="O35" s="71"/>
+      <c r="P35" s="51"/>
+      <c r="Q35" s="72"/>
+      <c r="R35" s="73"/>
+      <c r="S35" s="74"/>
+      <c r="T35" s="68" t="s">
         <v>151</v>
       </c>
-      <c r="U35" s="73"/>
-      <c r="V35" s="73"/>
-      <c r="W35" s="73"/>
-      <c r="X35" s="73"/>
-      <c r="Y35" s="74"/>
+      <c r="U35" s="69"/>
+      <c r="V35" s="69"/>
+      <c r="W35" s="69"/>
+      <c r="X35" s="69"/>
+      <c r="Y35" s="70"/>
       <c r="Z35" s="6">
         <v>2</v>
       </c>
@@ -4288,35 +4300,35 @@
       <c r="D36" s="6">
         <v>2</v>
       </c>
-      <c r="E36" s="64"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="66"/>
-      <c r="H36" s="64" t="s">
+      <c r="E36" s="50"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="I36" s="65"/>
-      <c r="J36" s="66"/>
-      <c r="K36" s="64" t="s">
+      <c r="I36" s="71"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="50" t="s">
         <v>262</v>
       </c>
-      <c r="L36" s="65"/>
-      <c r="M36" s="66"/>
-      <c r="N36" s="64" t="s">
+      <c r="L36" s="71"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="50" t="s">
         <v>252</v>
       </c>
-      <c r="O36" s="65"/>
-      <c r="P36" s="66"/>
-      <c r="Q36" s="57"/>
-      <c r="R36" s="71"/>
-      <c r="S36" s="58"/>
-      <c r="T36" s="72" t="s">
+      <c r="O36" s="71"/>
+      <c r="P36" s="51"/>
+      <c r="Q36" s="72"/>
+      <c r="R36" s="73"/>
+      <c r="S36" s="74"/>
+      <c r="T36" s="68" t="s">
         <v>152</v>
       </c>
-      <c r="U36" s="73"/>
-      <c r="V36" s="73"/>
-      <c r="W36" s="73"/>
-      <c r="X36" s="73"/>
-      <c r="Y36" s="74"/>
+      <c r="U36" s="69"/>
+      <c r="V36" s="69"/>
+      <c r="W36" s="69"/>
+      <c r="X36" s="69"/>
+      <c r="Y36" s="70"/>
       <c r="Z36" s="6">
         <v>2</v>
       </c>
@@ -4353,27 +4365,27 @@
       <c r="D37" s="6">
         <v>3</v>
       </c>
-      <c r="E37" s="64"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="66"/>
-      <c r="K37" s="64"/>
-      <c r="L37" s="65"/>
-      <c r="M37" s="66"/>
-      <c r="N37" s="64"/>
-      <c r="O37" s="65"/>
-      <c r="P37" s="66"/>
-      <c r="Q37" s="57"/>
-      <c r="R37" s="71"/>
-      <c r="S37" s="58"/>
-      <c r="T37" s="72"/>
-      <c r="U37" s="73"/>
-      <c r="V37" s="73"/>
-      <c r="W37" s="73"/>
-      <c r="X37" s="73"/>
-      <c r="Y37" s="74"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="71"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="71"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="71"/>
+      <c r="P37" s="51"/>
+      <c r="Q37" s="72"/>
+      <c r="R37" s="73"/>
+      <c r="S37" s="74"/>
+      <c r="T37" s="68"/>
+      <c r="U37" s="69"/>
+      <c r="V37" s="69"/>
+      <c r="W37" s="69"/>
+      <c r="X37" s="69"/>
+      <c r="Y37" s="70"/>
       <c r="Z37" s="6"/>
       <c r="AA37" s="6"/>
       <c r="AB37" s="16"/>
@@ -4408,35 +4420,35 @@
       <c r="D38" s="6">
         <v>4</v>
       </c>
-      <c r="E38" s="64" t="s">
-        <v>389</v>
-      </c>
-      <c r="F38" s="65"/>
-      <c r="G38" s="66"/>
-      <c r="H38" s="64" t="s">
+      <c r="E38" s="50" t="s">
+        <v>388</v>
+      </c>
+      <c r="F38" s="71"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="I38" s="65"/>
-      <c r="J38" s="66"/>
-      <c r="K38" s="64" t="s">
+      <c r="I38" s="71"/>
+      <c r="J38" s="51"/>
+      <c r="K38" s="50" t="s">
         <v>254</v>
       </c>
-      <c r="L38" s="65"/>
-      <c r="M38" s="66"/>
-      <c r="N38" s="64" t="s">
+      <c r="L38" s="71"/>
+      <c r="M38" s="51"/>
+      <c r="N38" s="50" t="s">
         <v>234</v>
       </c>
-      <c r="O38" s="65"/>
-      <c r="P38" s="66"/>
-      <c r="Q38" s="57"/>
-      <c r="R38" s="71"/>
-      <c r="S38" s="58"/>
-      <c r="T38" s="72"/>
-      <c r="U38" s="73"/>
-      <c r="V38" s="73"/>
-      <c r="W38" s="73"/>
-      <c r="X38" s="73"/>
-      <c r="Y38" s="74"/>
+      <c r="O38" s="71"/>
+      <c r="P38" s="51"/>
+      <c r="Q38" s="72"/>
+      <c r="R38" s="73"/>
+      <c r="S38" s="74"/>
+      <c r="T38" s="68"/>
+      <c r="U38" s="69"/>
+      <c r="V38" s="69"/>
+      <c r="W38" s="69"/>
+      <c r="X38" s="69"/>
+      <c r="Y38" s="70"/>
       <c r="Z38" s="6">
         <v>4</v>
       </c>
@@ -4481,18 +4493,18 @@
       </c>
       <c r="I39" s="62"/>
       <c r="J39" s="62"/>
-      <c r="K39" s="64" t="s">
+      <c r="K39" s="50" t="s">
         <v>261</v>
       </c>
-      <c r="L39" s="65"/>
-      <c r="M39" s="66"/>
+      <c r="L39" s="71"/>
+      <c r="M39" s="51"/>
       <c r="N39" s="62"/>
       <c r="O39" s="62"/>
       <c r="P39" s="62"/>
-      <c r="Q39" s="63"/>
-      <c r="R39" s="63"/>
-      <c r="S39" s="63"/>
-      <c r="T39" s="75"/>
+      <c r="Q39" s="75"/>
+      <c r="R39" s="75"/>
+      <c r="S39" s="75"/>
+      <c r="T39" s="63"/>
       <c r="U39" s="62"/>
       <c r="V39" s="62"/>
       <c r="W39" s="62"/>
@@ -4552,12 +4564,12 @@
       </c>
       <c r="O40" s="62"/>
       <c r="P40" s="62"/>
-      <c r="Q40" s="57" t="s">
+      <c r="Q40" s="72" t="s">
         <v>240</v>
       </c>
-      <c r="R40" s="71"/>
-      <c r="S40" s="58"/>
-      <c r="T40" s="75"/>
+      <c r="R40" s="73"/>
+      <c r="S40" s="74"/>
+      <c r="T40" s="63"/>
       <c r="U40" s="62"/>
       <c r="V40" s="62"/>
       <c r="W40" s="62"/>
@@ -4615,10 +4627,10 @@
       <c r="N41" s="62"/>
       <c r="O41" s="62"/>
       <c r="P41" s="62"/>
-      <c r="Q41" s="63"/>
-      <c r="R41" s="63"/>
-      <c r="S41" s="63"/>
-      <c r="T41" s="75"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="75"/>
+      <c r="S41" s="75"/>
+      <c r="T41" s="63"/>
       <c r="U41" s="62"/>
       <c r="V41" s="62"/>
       <c r="W41" s="62"/>
@@ -4676,10 +4688,10 @@
       <c r="N42" s="62"/>
       <c r="O42" s="62"/>
       <c r="P42" s="62"/>
-      <c r="Q42" s="63"/>
-      <c r="R42" s="63"/>
-      <c r="S42" s="63"/>
-      <c r="T42" s="75"/>
+      <c r="Q42" s="75"/>
+      <c r="R42" s="75"/>
+      <c r="S42" s="75"/>
+      <c r="T42" s="63"/>
       <c r="U42" s="62"/>
       <c r="V42" s="62"/>
       <c r="W42" s="62"/>
@@ -4735,10 +4747,10 @@
       <c r="N43" s="62"/>
       <c r="O43" s="62"/>
       <c r="P43" s="62"/>
-      <c r="Q43" s="63"/>
-      <c r="R43" s="63"/>
-      <c r="S43" s="63"/>
-      <c r="T43" s="75"/>
+      <c r="Q43" s="75"/>
+      <c r="R43" s="75"/>
+      <c r="S43" s="75"/>
+      <c r="T43" s="63"/>
       <c r="U43" s="62"/>
       <c r="V43" s="62"/>
       <c r="W43" s="62"/>
@@ -4779,7 +4791,7 @@
         <v>149</v>
       </c>
       <c r="E44" s="62" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F44" s="62"/>
       <c r="G44" s="62"/>
@@ -4798,12 +4810,12 @@
       </c>
       <c r="O44" s="62"/>
       <c r="P44" s="62"/>
-      <c r="Q44" s="57" t="s">
+      <c r="Q44" s="72" t="s">
         <v>236</v>
       </c>
-      <c r="R44" s="71"/>
-      <c r="S44" s="58"/>
-      <c r="T44" s="75"/>
+      <c r="R44" s="73"/>
+      <c r="S44" s="74"/>
+      <c r="T44" s="63"/>
       <c r="U44" s="62"/>
       <c r="V44" s="62"/>
       <c r="W44" s="62"/>
@@ -4835,75 +4847,75 @@
       <c r="AU44" s="16"/>
     </row>
     <row r="45" spans="1:67">
-      <c r="A45" s="68" t="s">
+      <c r="A45" s="76" t="s">
         <v>205</v>
       </c>
-      <c r="B45" s="69"/>
-      <c r="C45" s="69"/>
-      <c r="D45" s="69"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="69"/>
-      <c r="G45" s="69"/>
-      <c r="H45" s="69"/>
-      <c r="I45" s="69"/>
-      <c r="J45" s="69"/>
-      <c r="K45" s="69"/>
-      <c r="L45" s="69"/>
-      <c r="M45" s="69"/>
-      <c r="N45" s="69"/>
-      <c r="O45" s="69"/>
-      <c r="P45" s="69"/>
-      <c r="Q45" s="69"/>
-      <c r="R45" s="69"/>
-      <c r="S45" s="69"/>
-      <c r="T45" s="69"/>
-      <c r="U45" s="69"/>
-      <c r="V45" s="69"/>
-      <c r="W45" s="69"/>
-      <c r="X45" s="69"/>
-      <c r="Y45" s="69"/>
-      <c r="Z45" s="69"/>
-      <c r="AA45" s="70"/>
-      <c r="AB45" s="53"/>
-      <c r="AC45" s="54"/>
-      <c r="AD45" s="54"/>
-      <c r="AE45" s="54"/>
-      <c r="AF45" s="54"/>
-      <c r="AG45" s="54"/>
-      <c r="AH45" s="54"/>
-      <c r="AI45" s="54"/>
-      <c r="AJ45" s="54"/>
-      <c r="AK45" s="54"/>
-      <c r="AL45" s="54"/>
-      <c r="AM45" s="54"/>
-      <c r="AN45" s="54"/>
-      <c r="AO45" s="54"/>
-      <c r="AP45" s="54"/>
-      <c r="AQ45" s="54"/>
-      <c r="AR45" s="54"/>
-      <c r="AS45" s="54"/>
-      <c r="AT45" s="54"/>
-      <c r="AU45" s="54"/>
-      <c r="AV45" s="54"/>
-      <c r="AW45" s="54"/>
-      <c r="AX45" s="54"/>
-      <c r="AY45" s="54"/>
-      <c r="AZ45" s="54"/>
-      <c r="BA45" s="54"/>
-      <c r="BB45" s="54"/>
-      <c r="BC45" s="54"/>
-      <c r="BD45" s="54"/>
-      <c r="BE45" s="54"/>
-      <c r="BF45" s="54"/>
-      <c r="BG45" s="54"/>
-      <c r="BH45" s="54"/>
-      <c r="BI45" s="54"/>
-      <c r="BJ45" s="54"/>
-      <c r="BK45" s="54"/>
-      <c r="BL45" s="54"/>
-      <c r="BM45" s="54"/>
-      <c r="BN45" s="54"/>
-      <c r="BO45" s="54"/>
+      <c r="B45" s="77"/>
+      <c r="C45" s="77"/>
+      <c r="D45" s="77"/>
+      <c r="E45" s="77"/>
+      <c r="F45" s="77"/>
+      <c r="G45" s="77"/>
+      <c r="H45" s="77"/>
+      <c r="I45" s="77"/>
+      <c r="J45" s="77"/>
+      <c r="K45" s="77"/>
+      <c r="L45" s="77"/>
+      <c r="M45" s="77"/>
+      <c r="N45" s="77"/>
+      <c r="O45" s="77"/>
+      <c r="P45" s="77"/>
+      <c r="Q45" s="77"/>
+      <c r="R45" s="77"/>
+      <c r="S45" s="77"/>
+      <c r="T45" s="77"/>
+      <c r="U45" s="77"/>
+      <c r="V45" s="77"/>
+      <c r="W45" s="77"/>
+      <c r="X45" s="77"/>
+      <c r="Y45" s="77"/>
+      <c r="Z45" s="77"/>
+      <c r="AA45" s="78"/>
+      <c r="AB45" s="84"/>
+      <c r="AC45" s="85"/>
+      <c r="AD45" s="85"/>
+      <c r="AE45" s="85"/>
+      <c r="AF45" s="85"/>
+      <c r="AG45" s="85"/>
+      <c r="AH45" s="85"/>
+      <c r="AI45" s="85"/>
+      <c r="AJ45" s="85"/>
+      <c r="AK45" s="85"/>
+      <c r="AL45" s="85"/>
+      <c r="AM45" s="85"/>
+      <c r="AN45" s="85"/>
+      <c r="AO45" s="85"/>
+      <c r="AP45" s="85"/>
+      <c r="AQ45" s="85"/>
+      <c r="AR45" s="85"/>
+      <c r="AS45" s="85"/>
+      <c r="AT45" s="85"/>
+      <c r="AU45" s="85"/>
+      <c r="AV45" s="85"/>
+      <c r="AW45" s="85"/>
+      <c r="AX45" s="85"/>
+      <c r="AY45" s="85"/>
+      <c r="AZ45" s="85"/>
+      <c r="BA45" s="85"/>
+      <c r="BB45" s="85"/>
+      <c r="BC45" s="85"/>
+      <c r="BD45" s="85"/>
+      <c r="BE45" s="85"/>
+      <c r="BF45" s="85"/>
+      <c r="BG45" s="85"/>
+      <c r="BH45" s="85"/>
+      <c r="BI45" s="85"/>
+      <c r="BJ45" s="85"/>
+      <c r="BK45" s="85"/>
+      <c r="BL45" s="85"/>
+      <c r="BM45" s="85"/>
+      <c r="BN45" s="85"/>
+      <c r="BO45" s="85"/>
     </row>
     <row r="46" spans="1:67">
       <c r="A46" s="7" t="s">
@@ -4916,33 +4928,33 @@
       <c r="D46" s="6">
         <v>4</v>
       </c>
-      <c r="E46" s="64"/>
-      <c r="F46" s="65"/>
-      <c r="G46" s="66"/>
-      <c r="H46" s="64" t="s">
+      <c r="E46" s="50"/>
+      <c r="F46" s="71"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="I46" s="65"/>
-      <c r="J46" s="66"/>
-      <c r="K46" s="64" t="s">
+      <c r="I46" s="71"/>
+      <c r="J46" s="51"/>
+      <c r="K46" s="50" t="s">
         <v>253</v>
       </c>
-      <c r="L46" s="65"/>
-      <c r="M46" s="66"/>
-      <c r="N46" s="64"/>
-      <c r="O46" s="65"/>
-      <c r="P46" s="66"/>
-      <c r="Q46" s="64"/>
-      <c r="R46" s="65"/>
-      <c r="S46" s="66"/>
-      <c r="T46" s="72" t="s">
+      <c r="L46" s="71"/>
+      <c r="M46" s="51"/>
+      <c r="N46" s="50"/>
+      <c r="O46" s="71"/>
+      <c r="P46" s="51"/>
+      <c r="Q46" s="50"/>
+      <c r="R46" s="71"/>
+      <c r="S46" s="51"/>
+      <c r="T46" s="68" t="s">
         <v>151</v>
       </c>
-      <c r="U46" s="73"/>
-      <c r="V46" s="73"/>
-      <c r="W46" s="73"/>
-      <c r="X46" s="73"/>
-      <c r="Y46" s="74"/>
+      <c r="U46" s="69"/>
+      <c r="V46" s="69"/>
+      <c r="W46" s="69"/>
+      <c r="X46" s="69"/>
+      <c r="Y46" s="70"/>
       <c r="Z46" s="6">
         <v>3</v>
       </c>
@@ -4993,10 +5005,10 @@
       <c r="N47" s="62"/>
       <c r="O47" s="62"/>
       <c r="P47" s="62"/>
-      <c r="Q47" s="64"/>
-      <c r="R47" s="65"/>
-      <c r="S47" s="66"/>
-      <c r="T47" s="75"/>
+      <c r="Q47" s="50"/>
+      <c r="R47" s="71"/>
+      <c r="S47" s="51"/>
+      <c r="T47" s="63"/>
       <c r="U47" s="62"/>
       <c r="V47" s="62"/>
       <c r="W47" s="62"/>
@@ -5040,11 +5052,11 @@
       <c r="D48" s="6">
         <v>6</v>
       </c>
-      <c r="E48" s="64" t="s">
-        <v>389</v>
-      </c>
-      <c r="F48" s="65"/>
-      <c r="G48" s="66"/>
+      <c r="E48" s="50" t="s">
+        <v>388</v>
+      </c>
+      <c r="F48" s="71"/>
+      <c r="G48" s="51"/>
       <c r="H48" s="62" t="s">
         <v>272</v>
       </c>
@@ -5058,10 +5070,10 @@
       <c r="N48" s="62"/>
       <c r="O48" s="62"/>
       <c r="P48" s="62"/>
-      <c r="Q48" s="64"/>
-      <c r="R48" s="65"/>
-      <c r="S48" s="66"/>
-      <c r="T48" s="75"/>
+      <c r="Q48" s="50"/>
+      <c r="R48" s="71"/>
+      <c r="S48" s="51"/>
+      <c r="T48" s="63"/>
       <c r="U48" s="62"/>
       <c r="V48" s="62"/>
       <c r="W48" s="62"/>
@@ -5123,10 +5135,10 @@
       </c>
       <c r="O49" s="62"/>
       <c r="P49" s="62"/>
-      <c r="Q49" s="64"/>
-      <c r="R49" s="65"/>
-      <c r="S49" s="66"/>
-      <c r="T49" s="75"/>
+      <c r="Q49" s="50"/>
+      <c r="R49" s="71"/>
+      <c r="S49" s="51"/>
+      <c r="T49" s="63"/>
       <c r="U49" s="62"/>
       <c r="V49" s="62"/>
       <c r="W49" s="62"/>
@@ -5169,29 +5181,29 @@
       <c r="D50" s="6">
         <v>5</v>
       </c>
-      <c r="E50" s="64" t="s">
+      <c r="E50" s="50" t="s">
         <v>284</v>
       </c>
-      <c r="F50" s="65"/>
-      <c r="G50" s="66"/>
-      <c r="H50" s="64"/>
-      <c r="I50" s="65"/>
-      <c r="J50" s="66"/>
-      <c r="K50" s="64"/>
-      <c r="L50" s="65"/>
-      <c r="M50" s="66"/>
-      <c r="N50" s="64"/>
-      <c r="O50" s="65"/>
-      <c r="P50" s="66"/>
-      <c r="Q50" s="64"/>
-      <c r="R50" s="65"/>
-      <c r="S50" s="66"/>
-      <c r="T50" s="72"/>
-      <c r="U50" s="73"/>
-      <c r="V50" s="73"/>
-      <c r="W50" s="73"/>
-      <c r="X50" s="73"/>
-      <c r="Y50" s="74"/>
+      <c r="F50" s="71"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="50"/>
+      <c r="I50" s="71"/>
+      <c r="J50" s="51"/>
+      <c r="K50" s="50"/>
+      <c r="L50" s="71"/>
+      <c r="M50" s="51"/>
+      <c r="N50" s="50"/>
+      <c r="O50" s="71"/>
+      <c r="P50" s="51"/>
+      <c r="Q50" s="50"/>
+      <c r="R50" s="71"/>
+      <c r="S50" s="51"/>
+      <c r="T50" s="68"/>
+      <c r="U50" s="69"/>
+      <c r="V50" s="69"/>
+      <c r="W50" s="69"/>
+      <c r="X50" s="69"/>
+      <c r="Y50" s="70"/>
       <c r="Z50" s="6"/>
       <c r="AA50" s="6"/>
       <c r="AB50" s="16"/>
@@ -5228,29 +5240,29 @@
       <c r="D51" s="6">
         <v>7</v>
       </c>
-      <c r="E51" s="64" t="s">
+      <c r="E51" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="F51" s="65"/>
-      <c r="G51" s="66"/>
-      <c r="H51" s="64"/>
-      <c r="I51" s="65"/>
-      <c r="J51" s="66"/>
-      <c r="K51" s="64"/>
-      <c r="L51" s="65"/>
-      <c r="M51" s="66"/>
-      <c r="N51" s="64"/>
-      <c r="O51" s="65"/>
-      <c r="P51" s="66"/>
-      <c r="Q51" s="64"/>
-      <c r="R51" s="65"/>
-      <c r="S51" s="66"/>
-      <c r="T51" s="72"/>
-      <c r="U51" s="73"/>
-      <c r="V51" s="73"/>
-      <c r="W51" s="73"/>
-      <c r="X51" s="73"/>
-      <c r="Y51" s="74"/>
+      <c r="F51" s="71"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="71"/>
+      <c r="J51" s="51"/>
+      <c r="K51" s="50"/>
+      <c r="L51" s="71"/>
+      <c r="M51" s="51"/>
+      <c r="N51" s="50"/>
+      <c r="O51" s="71"/>
+      <c r="P51" s="51"/>
+      <c r="Q51" s="50"/>
+      <c r="R51" s="71"/>
+      <c r="S51" s="51"/>
+      <c r="T51" s="68"/>
+      <c r="U51" s="69"/>
+      <c r="V51" s="69"/>
+      <c r="W51" s="69"/>
+      <c r="X51" s="69"/>
+      <c r="Y51" s="70"/>
       <c r="Z51" s="6"/>
       <c r="AA51" s="6"/>
       <c r="AB51" s="16"/>
@@ -5287,11 +5299,11 @@
       <c r="D52" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="E52" s="64" t="s">
+      <c r="E52" s="50" t="s">
         <v>226</v>
       </c>
-      <c r="F52" s="65"/>
-      <c r="G52" s="66"/>
+      <c r="F52" s="71"/>
+      <c r="G52" s="51"/>
       <c r="H52" s="62"/>
       <c r="I52" s="62"/>
       <c r="J52" s="62"/>
@@ -5301,10 +5313,10 @@
       <c r="N52" s="62"/>
       <c r="O52" s="62"/>
       <c r="P52" s="62"/>
-      <c r="Q52" s="64"/>
-      <c r="R52" s="65"/>
-      <c r="S52" s="66"/>
-      <c r="T52" s="75"/>
+      <c r="Q52" s="50"/>
+      <c r="R52" s="71"/>
+      <c r="S52" s="51"/>
+      <c r="T52" s="63"/>
       <c r="U52" s="62"/>
       <c r="V52" s="62"/>
       <c r="W52" s="62"/>
@@ -5354,10 +5366,10 @@
       <c r="N53" s="62"/>
       <c r="O53" s="62"/>
       <c r="P53" s="62"/>
-      <c r="Q53" s="64"/>
-      <c r="R53" s="65"/>
-      <c r="S53" s="66"/>
-      <c r="T53" s="75"/>
+      <c r="Q53" s="50"/>
+      <c r="R53" s="71"/>
+      <c r="S53" s="51"/>
+      <c r="T53" s="63"/>
       <c r="U53" s="62"/>
       <c r="V53" s="62"/>
       <c r="W53" s="62"/>
@@ -5418,12 +5430,12 @@
       </c>
       <c r="O54" s="62"/>
       <c r="P54" s="62"/>
-      <c r="Q54" s="64" t="s">
+      <c r="Q54" s="50" t="s">
         <v>269</v>
       </c>
-      <c r="R54" s="65"/>
-      <c r="S54" s="66"/>
-      <c r="T54" s="75" t="s">
+      <c r="R54" s="71"/>
+      <c r="S54" s="51"/>
+      <c r="T54" s="63" t="s">
         <v>270</v>
       </c>
       <c r="U54" s="62"/>
@@ -5458,75 +5470,75 @@
       <c r="AW54" s="20"/>
     </row>
     <row r="55" spans="1:68">
-      <c r="A55" s="86" t="s">
+      <c r="A55" s="64" t="s">
         <v>206</v>
       </c>
-      <c r="B55" s="87"/>
-      <c r="C55" s="87"/>
-      <c r="D55" s="87"/>
-      <c r="E55" s="87"/>
-      <c r="F55" s="87"/>
-      <c r="G55" s="87"/>
-      <c r="H55" s="87"/>
-      <c r="I55" s="87"/>
-      <c r="J55" s="87"/>
-      <c r="K55" s="87"/>
-      <c r="L55" s="87"/>
-      <c r="M55" s="87"/>
-      <c r="N55" s="87"/>
-      <c r="O55" s="87"/>
-      <c r="P55" s="87"/>
-      <c r="Q55" s="87"/>
-      <c r="R55" s="87"/>
-      <c r="S55" s="87"/>
-      <c r="T55" s="87"/>
-      <c r="U55" s="87"/>
-      <c r="V55" s="87"/>
-      <c r="W55" s="87"/>
-      <c r="X55" s="87"/>
-      <c r="Y55" s="87"/>
-      <c r="Z55" s="87"/>
-      <c r="AA55" s="88"/>
-      <c r="AB55" s="53"/>
-      <c r="AC55" s="54"/>
-      <c r="AD55" s="54"/>
-      <c r="AE55" s="54"/>
-      <c r="AF55" s="54"/>
-      <c r="AG55" s="54"/>
-      <c r="AH55" s="54"/>
-      <c r="AI55" s="54"/>
-      <c r="AJ55" s="54"/>
-      <c r="AK55" s="54"/>
-      <c r="AL55" s="54"/>
-      <c r="AM55" s="54"/>
-      <c r="AN55" s="54"/>
-      <c r="AO55" s="54"/>
-      <c r="AP55" s="54"/>
-      <c r="AQ55" s="54"/>
-      <c r="AR55" s="54"/>
-      <c r="AS55" s="54"/>
-      <c r="AT55" s="54"/>
-      <c r="AU55" s="54"/>
-      <c r="AV55" s="54"/>
-      <c r="AW55" s="54"/>
-      <c r="AX55" s="54"/>
-      <c r="AY55" s="54"/>
-      <c r="AZ55" s="54"/>
-      <c r="BA55" s="54"/>
-      <c r="BB55" s="54"/>
-      <c r="BC55" s="54"/>
-      <c r="BD55" s="54"/>
-      <c r="BE55" s="54"/>
-      <c r="BF55" s="54"/>
-      <c r="BG55" s="54"/>
-      <c r="BH55" s="54"/>
-      <c r="BI55" s="54"/>
-      <c r="BJ55" s="54"/>
-      <c r="BK55" s="54"/>
-      <c r="BL55" s="54"/>
-      <c r="BM55" s="54"/>
-      <c r="BN55" s="54"/>
-      <c r="BO55" s="54"/>
+      <c r="B55" s="65"/>
+      <c r="C55" s="65"/>
+      <c r="D55" s="65"/>
+      <c r="E55" s="65"/>
+      <c r="F55" s="65"/>
+      <c r="G55" s="65"/>
+      <c r="H55" s="65"/>
+      <c r="I55" s="65"/>
+      <c r="J55" s="65"/>
+      <c r="K55" s="65"/>
+      <c r="L55" s="65"/>
+      <c r="M55" s="65"/>
+      <c r="N55" s="65"/>
+      <c r="O55" s="65"/>
+      <c r="P55" s="65"/>
+      <c r="Q55" s="65"/>
+      <c r="R55" s="65"/>
+      <c r="S55" s="65"/>
+      <c r="T55" s="65"/>
+      <c r="U55" s="65"/>
+      <c r="V55" s="65"/>
+      <c r="W55" s="65"/>
+      <c r="X55" s="65"/>
+      <c r="Y55" s="65"/>
+      <c r="Z55" s="65"/>
+      <c r="AA55" s="66"/>
+      <c r="AB55" s="84"/>
+      <c r="AC55" s="85"/>
+      <c r="AD55" s="85"/>
+      <c r="AE55" s="85"/>
+      <c r="AF55" s="85"/>
+      <c r="AG55" s="85"/>
+      <c r="AH55" s="85"/>
+      <c r="AI55" s="85"/>
+      <c r="AJ55" s="85"/>
+      <c r="AK55" s="85"/>
+      <c r="AL55" s="85"/>
+      <c r="AM55" s="85"/>
+      <c r="AN55" s="85"/>
+      <c r="AO55" s="85"/>
+      <c r="AP55" s="85"/>
+      <c r="AQ55" s="85"/>
+      <c r="AR55" s="85"/>
+      <c r="AS55" s="85"/>
+      <c r="AT55" s="85"/>
+      <c r="AU55" s="85"/>
+      <c r="AV55" s="85"/>
+      <c r="AW55" s="85"/>
+      <c r="AX55" s="85"/>
+      <c r="AY55" s="85"/>
+      <c r="AZ55" s="85"/>
+      <c r="BA55" s="85"/>
+      <c r="BB55" s="85"/>
+      <c r="BC55" s="85"/>
+      <c r="BD55" s="85"/>
+      <c r="BE55" s="85"/>
+      <c r="BF55" s="85"/>
+      <c r="BG55" s="85"/>
+      <c r="BH55" s="85"/>
+      <c r="BI55" s="85"/>
+      <c r="BJ55" s="85"/>
+      <c r="BK55" s="85"/>
+      <c r="BL55" s="85"/>
+      <c r="BM55" s="85"/>
+      <c r="BN55" s="85"/>
+      <c r="BO55" s="85"/>
     </row>
     <row r="56" spans="1:68">
       <c r="A56" s="7" t="s">
@@ -5541,11 +5553,11 @@
       <c r="D56" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E56" s="64" t="s">
+      <c r="E56" s="50" t="s">
         <v>230</v>
       </c>
-      <c r="F56" s="65"/>
-      <c r="G56" s="66"/>
+      <c r="F56" s="71"/>
+      <c r="G56" s="51"/>
       <c r="H56" s="62"/>
       <c r="I56" s="62"/>
       <c r="J56" s="62"/>
@@ -5885,12 +5897,12 @@
       </c>
       <c r="O61" s="62"/>
       <c r="P61" s="62"/>
-      <c r="Q61" s="64" t="s">
+      <c r="Q61" s="50" t="s">
         <v>248</v>
       </c>
-      <c r="R61" s="65"/>
-      <c r="S61" s="66"/>
-      <c r="T61" s="75"/>
+      <c r="R61" s="71"/>
+      <c r="S61" s="51"/>
+      <c r="T61" s="63"/>
       <c r="U61" s="62"/>
       <c r="V61" s="62"/>
       <c r="W61" s="62"/>
@@ -5986,75 +5998,75 @@
       <c r="BF62" s="30"/>
     </row>
     <row r="63" spans="1:68">
-      <c r="A63" s="59" t="s">
+      <c r="A63" s="80" t="s">
         <v>215</v>
       </c>
-      <c r="B63" s="60"/>
-      <c r="C63" s="60"/>
-      <c r="D63" s="60"/>
-      <c r="E63" s="60"/>
-      <c r="F63" s="60"/>
-      <c r="G63" s="60"/>
-      <c r="H63" s="60"/>
-      <c r="I63" s="60"/>
-      <c r="J63" s="60"/>
-      <c r="K63" s="60"/>
-      <c r="L63" s="60"/>
-      <c r="M63" s="60"/>
-      <c r="N63" s="60"/>
-      <c r="O63" s="60"/>
-      <c r="P63" s="60"/>
-      <c r="Q63" s="60"/>
-      <c r="R63" s="60"/>
-      <c r="S63" s="60"/>
-      <c r="T63" s="60"/>
-      <c r="U63" s="60"/>
-      <c r="V63" s="60"/>
-      <c r="W63" s="60"/>
-      <c r="X63" s="60"/>
-      <c r="Y63" s="60"/>
-      <c r="Z63" s="60"/>
-      <c r="AA63" s="61"/>
-      <c r="AB63" s="53"/>
-      <c r="AC63" s="54"/>
-      <c r="AD63" s="54"/>
-      <c r="AE63" s="54"/>
-      <c r="AF63" s="54"/>
-      <c r="AG63" s="54"/>
-      <c r="AH63" s="54"/>
-      <c r="AI63" s="54"/>
-      <c r="AJ63" s="54"/>
-      <c r="AK63" s="54"/>
-      <c r="AL63" s="54"/>
-      <c r="AM63" s="54"/>
-      <c r="AN63" s="54"/>
-      <c r="AO63" s="54"/>
-      <c r="AP63" s="54"/>
-      <c r="AQ63" s="54"/>
-      <c r="AR63" s="54"/>
-      <c r="AS63" s="54"/>
-      <c r="AT63" s="54"/>
-      <c r="AU63" s="54"/>
-      <c r="AV63" s="54"/>
-      <c r="AW63" s="54"/>
-      <c r="AX63" s="54"/>
-      <c r="AY63" s="54"/>
-      <c r="AZ63" s="54"/>
-      <c r="BA63" s="54"/>
-      <c r="BB63" s="54"/>
-      <c r="BC63" s="54"/>
-      <c r="BD63" s="54"/>
-      <c r="BE63" s="54"/>
-      <c r="BF63" s="54"/>
-      <c r="BG63" s="54"/>
-      <c r="BH63" s="54"/>
-      <c r="BI63" s="54"/>
-      <c r="BJ63" s="54"/>
-      <c r="BK63" s="54"/>
-      <c r="BL63" s="54"/>
-      <c r="BM63" s="54"/>
-      <c r="BN63" s="54"/>
-      <c r="BO63" s="54"/>
+      <c r="B63" s="81"/>
+      <c r="C63" s="81"/>
+      <c r="D63" s="81"/>
+      <c r="E63" s="81"/>
+      <c r="F63" s="81"/>
+      <c r="G63" s="81"/>
+      <c r="H63" s="81"/>
+      <c r="I63" s="81"/>
+      <c r="J63" s="81"/>
+      <c r="K63" s="81"/>
+      <c r="L63" s="81"/>
+      <c r="M63" s="81"/>
+      <c r="N63" s="81"/>
+      <c r="O63" s="81"/>
+      <c r="P63" s="81"/>
+      <c r="Q63" s="81"/>
+      <c r="R63" s="81"/>
+      <c r="S63" s="81"/>
+      <c r="T63" s="81"/>
+      <c r="U63" s="81"/>
+      <c r="V63" s="81"/>
+      <c r="W63" s="81"/>
+      <c r="X63" s="81"/>
+      <c r="Y63" s="81"/>
+      <c r="Z63" s="81"/>
+      <c r="AA63" s="82"/>
+      <c r="AB63" s="84"/>
+      <c r="AC63" s="85"/>
+      <c r="AD63" s="85"/>
+      <c r="AE63" s="85"/>
+      <c r="AF63" s="85"/>
+      <c r="AG63" s="85"/>
+      <c r="AH63" s="85"/>
+      <c r="AI63" s="85"/>
+      <c r="AJ63" s="85"/>
+      <c r="AK63" s="85"/>
+      <c r="AL63" s="85"/>
+      <c r="AM63" s="85"/>
+      <c r="AN63" s="85"/>
+      <c r="AO63" s="85"/>
+      <c r="AP63" s="85"/>
+      <c r="AQ63" s="85"/>
+      <c r="AR63" s="85"/>
+      <c r="AS63" s="85"/>
+      <c r="AT63" s="85"/>
+      <c r="AU63" s="85"/>
+      <c r="AV63" s="85"/>
+      <c r="AW63" s="85"/>
+      <c r="AX63" s="85"/>
+      <c r="AY63" s="85"/>
+      <c r="AZ63" s="85"/>
+      <c r="BA63" s="85"/>
+      <c r="BB63" s="85"/>
+      <c r="BC63" s="85"/>
+      <c r="BD63" s="85"/>
+      <c r="BE63" s="85"/>
+      <c r="BF63" s="85"/>
+      <c r="BG63" s="85"/>
+      <c r="BH63" s="85"/>
+      <c r="BI63" s="85"/>
+      <c r="BJ63" s="85"/>
+      <c r="BK63" s="85"/>
+      <c r="BL63" s="85"/>
+      <c r="BM63" s="85"/>
+      <c r="BN63" s="85"/>
+      <c r="BO63" s="85"/>
     </row>
     <row r="64" spans="1:68">
       <c r="A64" s="29" t="s">
@@ -6141,7 +6153,7 @@
       <c r="Q65" s="62"/>
       <c r="R65" s="62"/>
       <c r="S65" s="62"/>
-      <c r="T65" s="75"/>
+      <c r="T65" s="63"/>
       <c r="U65" s="62"/>
       <c r="V65" s="62"/>
       <c r="W65" s="62"/>
@@ -6199,7 +6211,7 @@
       <c r="Q66" s="62"/>
       <c r="R66" s="62"/>
       <c r="S66" s="62"/>
-      <c r="T66" s="75"/>
+      <c r="T66" s="63"/>
       <c r="U66" s="62"/>
       <c r="V66" s="62"/>
       <c r="W66" s="62"/>
@@ -6350,75 +6362,75 @@
       <c r="BO68" s="37"/>
     </row>
     <row r="69" spans="1:67">
-      <c r="A69" s="79" t="s">
+      <c r="A69" s="55" t="s">
         <v>208</v>
       </c>
-      <c r="B69" s="80"/>
-      <c r="C69" s="80"/>
-      <c r="D69" s="80"/>
-      <c r="E69" s="80"/>
-      <c r="F69" s="80"/>
-      <c r="G69" s="80"/>
-      <c r="H69" s="80"/>
-      <c r="I69" s="80"/>
-      <c r="J69" s="80"/>
-      <c r="K69" s="80"/>
-      <c r="L69" s="80"/>
-      <c r="M69" s="80"/>
-      <c r="N69" s="80"/>
-      <c r="O69" s="80"/>
-      <c r="P69" s="80"/>
-      <c r="Q69" s="80"/>
-      <c r="R69" s="80"/>
-      <c r="S69" s="80"/>
-      <c r="T69" s="80"/>
-      <c r="U69" s="80"/>
-      <c r="V69" s="80"/>
-      <c r="W69" s="80"/>
-      <c r="X69" s="80"/>
-      <c r="Y69" s="80"/>
-      <c r="Z69" s="80"/>
-      <c r="AA69" s="81"/>
-      <c r="AB69" s="53"/>
-      <c r="AC69" s="54"/>
-      <c r="AD69" s="54"/>
-      <c r="AE69" s="54"/>
-      <c r="AF69" s="54"/>
-      <c r="AG69" s="54"/>
-      <c r="AH69" s="54"/>
-      <c r="AI69" s="54"/>
-      <c r="AJ69" s="54"/>
-      <c r="AK69" s="54"/>
-      <c r="AL69" s="54"/>
-      <c r="AM69" s="54"/>
-      <c r="AN69" s="54"/>
-      <c r="AO69" s="54"/>
-      <c r="AP69" s="54"/>
-      <c r="AQ69" s="54"/>
-      <c r="AR69" s="54"/>
-      <c r="AS69" s="54"/>
-      <c r="AT69" s="54"/>
-      <c r="AU69" s="54"/>
-      <c r="AV69" s="54"/>
-      <c r="AW69" s="54"/>
-      <c r="AX69" s="54"/>
-      <c r="AY69" s="54"/>
-      <c r="AZ69" s="54"/>
-      <c r="BA69" s="54"/>
-      <c r="BB69" s="54"/>
-      <c r="BC69" s="54"/>
-      <c r="BD69" s="54"/>
-      <c r="BE69" s="54"/>
-      <c r="BF69" s="54"/>
-      <c r="BG69" s="54"/>
-      <c r="BH69" s="54"/>
-      <c r="BI69" s="54"/>
-      <c r="BJ69" s="54"/>
-      <c r="BK69" s="54"/>
-      <c r="BL69" s="54"/>
-      <c r="BM69" s="54"/>
-      <c r="BN69" s="54"/>
-      <c r="BO69" s="54"/>
+      <c r="B69" s="56"/>
+      <c r="C69" s="56"/>
+      <c r="D69" s="56"/>
+      <c r="E69" s="56"/>
+      <c r="F69" s="56"/>
+      <c r="G69" s="56"/>
+      <c r="H69" s="56"/>
+      <c r="I69" s="56"/>
+      <c r="J69" s="56"/>
+      <c r="K69" s="56"/>
+      <c r="L69" s="56"/>
+      <c r="M69" s="56"/>
+      <c r="N69" s="56"/>
+      <c r="O69" s="56"/>
+      <c r="P69" s="56"/>
+      <c r="Q69" s="56"/>
+      <c r="R69" s="56"/>
+      <c r="S69" s="56"/>
+      <c r="T69" s="56"/>
+      <c r="U69" s="56"/>
+      <c r="V69" s="56"/>
+      <c r="W69" s="56"/>
+      <c r="X69" s="56"/>
+      <c r="Y69" s="56"/>
+      <c r="Z69" s="56"/>
+      <c r="AA69" s="57"/>
+      <c r="AB69" s="84"/>
+      <c r="AC69" s="85"/>
+      <c r="AD69" s="85"/>
+      <c r="AE69" s="85"/>
+      <c r="AF69" s="85"/>
+      <c r="AG69" s="85"/>
+      <c r="AH69" s="85"/>
+      <c r="AI69" s="85"/>
+      <c r="AJ69" s="85"/>
+      <c r="AK69" s="85"/>
+      <c r="AL69" s="85"/>
+      <c r="AM69" s="85"/>
+      <c r="AN69" s="85"/>
+      <c r="AO69" s="85"/>
+      <c r="AP69" s="85"/>
+      <c r="AQ69" s="85"/>
+      <c r="AR69" s="85"/>
+      <c r="AS69" s="85"/>
+      <c r="AT69" s="85"/>
+      <c r="AU69" s="85"/>
+      <c r="AV69" s="85"/>
+      <c r="AW69" s="85"/>
+      <c r="AX69" s="85"/>
+      <c r="AY69" s="85"/>
+      <c r="AZ69" s="85"/>
+      <c r="BA69" s="85"/>
+      <c r="BB69" s="85"/>
+      <c r="BC69" s="85"/>
+      <c r="BD69" s="85"/>
+      <c r="BE69" s="85"/>
+      <c r="BF69" s="85"/>
+      <c r="BG69" s="85"/>
+      <c r="BH69" s="85"/>
+      <c r="BI69" s="85"/>
+      <c r="BJ69" s="85"/>
+      <c r="BK69" s="85"/>
+      <c r="BL69" s="85"/>
+      <c r="BM69" s="85"/>
+      <c r="BN69" s="85"/>
+      <c r="BO69" s="85"/>
     </row>
     <row r="70" spans="1:67">
       <c r="A70" s="7" t="s">
@@ -6450,7 +6462,7 @@
       <c r="Q70" s="62"/>
       <c r="R70" s="62"/>
       <c r="S70" s="62"/>
-      <c r="T70" s="75"/>
+      <c r="T70" s="63"/>
       <c r="U70" s="62"/>
       <c r="V70" s="62"/>
       <c r="W70" s="62"/>
@@ -6483,18 +6495,18 @@
       <c r="AV70" s="19"/>
       <c r="AW70" s="20"/>
       <c r="AX70" s="20"/>
-      <c r="BF70" s="51" t="s">
+      <c r="BF70" s="83" t="s">
         <v>285</v>
       </c>
-      <c r="BG70" s="51"/>
-      <c r="BH70" s="51"/>
-      <c r="BI70" s="51"/>
-      <c r="BJ70" s="51"/>
-      <c r="BK70" s="51"/>
-      <c r="BL70" s="51"/>
-      <c r="BM70" s="51"/>
-      <c r="BN70" s="51"/>
-      <c r="BO70" s="51"/>
+      <c r="BG70" s="83"/>
+      <c r="BH70" s="83"/>
+      <c r="BI70" s="83"/>
+      <c r="BJ70" s="83"/>
+      <c r="BK70" s="83"/>
+      <c r="BL70" s="83"/>
+      <c r="BM70" s="83"/>
+      <c r="BN70" s="83"/>
+      <c r="BO70" s="83"/>
     </row>
     <row r="71" spans="1:67">
       <c r="A71" s="7" t="s">
@@ -6557,16 +6569,16 @@
       <c r="AV71" s="19"/>
       <c r="AW71" s="20"/>
       <c r="AX71" s="20"/>
-      <c r="BF71" s="51"/>
-      <c r="BG71" s="51"/>
-      <c r="BH71" s="51"/>
-      <c r="BI71" s="51"/>
-      <c r="BJ71" s="51"/>
-      <c r="BK71" s="51"/>
-      <c r="BL71" s="51"/>
-      <c r="BM71" s="51"/>
-      <c r="BN71" s="51"/>
-      <c r="BO71" s="51"/>
+      <c r="BF71" s="83"/>
+      <c r="BG71" s="83"/>
+      <c r="BH71" s="83"/>
+      <c r="BI71" s="83"/>
+      <c r="BJ71" s="83"/>
+      <c r="BK71" s="83"/>
+      <c r="BL71" s="83"/>
+      <c r="BM71" s="83"/>
+      <c r="BN71" s="83"/>
+      <c r="BO71" s="83"/>
     </row>
     <row r="72" spans="1:67">
       <c r="A72" s="7"/>
@@ -6621,16 +6633,16 @@
       <c r="AV72" s="19"/>
       <c r="AW72" s="20"/>
       <c r="AX72" s="20"/>
-      <c r="BF72" s="51"/>
-      <c r="BG72" s="51"/>
-      <c r="BH72" s="51"/>
-      <c r="BI72" s="51"/>
-      <c r="BJ72" s="51"/>
-      <c r="BK72" s="51"/>
-      <c r="BL72" s="51"/>
-      <c r="BM72" s="51"/>
-      <c r="BN72" s="51"/>
-      <c r="BO72" s="51"/>
+      <c r="BF72" s="83"/>
+      <c r="BG72" s="83"/>
+      <c r="BH72" s="83"/>
+      <c r="BI72" s="83"/>
+      <c r="BJ72" s="83"/>
+      <c r="BK72" s="83"/>
+      <c r="BL72" s="83"/>
+      <c r="BM72" s="83"/>
+      <c r="BN72" s="83"/>
+      <c r="BO72" s="83"/>
     </row>
     <row r="73" spans="1:67">
       <c r="A73" s="7" t="s">
@@ -6643,9 +6655,9 @@
       <c r="D73" s="6">
         <v>7</v>
       </c>
-      <c r="E73" s="63"/>
-      <c r="F73" s="63"/>
-      <c r="G73" s="63"/>
+      <c r="E73" s="75"/>
+      <c r="F73" s="75"/>
+      <c r="G73" s="75"/>
       <c r="H73" s="62" t="s">
         <v>238</v>
       </c>
@@ -6699,16 +6711,16 @@
       <c r="AV73" s="19"/>
       <c r="AW73" s="20"/>
       <c r="AX73" s="20"/>
-      <c r="BF73" s="51"/>
-      <c r="BG73" s="51"/>
-      <c r="BH73" s="51"/>
-      <c r="BI73" s="51"/>
-      <c r="BJ73" s="51"/>
-      <c r="BK73" s="51"/>
-      <c r="BL73" s="51"/>
-      <c r="BM73" s="51"/>
-      <c r="BN73" s="51"/>
-      <c r="BO73" s="51"/>
+      <c r="BF73" s="83"/>
+      <c r="BG73" s="83"/>
+      <c r="BH73" s="83"/>
+      <c r="BI73" s="83"/>
+      <c r="BJ73" s="83"/>
+      <c r="BK73" s="83"/>
+      <c r="BL73" s="83"/>
+      <c r="BM73" s="83"/>
+      <c r="BN73" s="83"/>
+      <c r="BO73" s="83"/>
     </row>
     <row r="74" spans="1:67">
       <c r="A74" s="7" t="s">
@@ -6721,11 +6733,11 @@
       <c r="D74" s="6">
         <v>8</v>
       </c>
-      <c r="E74" s="57" t="s">
+      <c r="E74" s="72" t="s">
         <v>381</v>
       </c>
-      <c r="F74" s="71"/>
-      <c r="G74" s="58"/>
+      <c r="F74" s="73"/>
+      <c r="G74" s="74"/>
       <c r="H74" s="62" t="s">
         <v>243</v>
       </c>
@@ -6742,7 +6754,7 @@
       <c r="Q74" s="62"/>
       <c r="R74" s="62"/>
       <c r="S74" s="62"/>
-      <c r="T74" s="75"/>
+      <c r="T74" s="63"/>
       <c r="U74" s="62"/>
       <c r="V74" s="62"/>
       <c r="W74" s="62"/>
@@ -6775,16 +6787,16 @@
       <c r="AV74" s="19"/>
       <c r="AW74" s="20"/>
       <c r="AX74" s="20"/>
-      <c r="BF74" s="51"/>
-      <c r="BG74" s="51"/>
-      <c r="BH74" s="51"/>
-      <c r="BI74" s="51"/>
-      <c r="BJ74" s="51"/>
-      <c r="BK74" s="51"/>
-      <c r="BL74" s="51"/>
-      <c r="BM74" s="51"/>
-      <c r="BN74" s="51"/>
-      <c r="BO74" s="51"/>
+      <c r="BF74" s="83"/>
+      <c r="BG74" s="83"/>
+      <c r="BH74" s="83"/>
+      <c r="BI74" s="83"/>
+      <c r="BJ74" s="83"/>
+      <c r="BK74" s="83"/>
+      <c r="BL74" s="83"/>
+      <c r="BM74" s="83"/>
+      <c r="BN74" s="83"/>
+      <c r="BO74" s="83"/>
     </row>
     <row r="75" spans="1:67">
       <c r="A75" s="7" t="s">
@@ -6797,11 +6809,11 @@
       <c r="D75" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E75" s="57" t="s">
+      <c r="E75" s="72" t="s">
         <v>382</v>
       </c>
-      <c r="F75" s="71"/>
-      <c r="G75" s="58"/>
+      <c r="F75" s="73"/>
+      <c r="G75" s="74"/>
       <c r="H75" s="62" t="s">
         <v>235</v>
       </c>
@@ -6820,7 +6832,7 @@
       <c r="Q75" s="62"/>
       <c r="R75" s="62"/>
       <c r="S75" s="62"/>
-      <c r="T75" s="75"/>
+      <c r="T75" s="63"/>
       <c r="U75" s="62"/>
       <c r="V75" s="62"/>
       <c r="W75" s="62"/>
@@ -6853,16 +6865,16 @@
       <c r="AV75" s="19"/>
       <c r="AW75" s="20"/>
       <c r="AX75" s="20"/>
-      <c r="BF75" s="51"/>
-      <c r="BG75" s="51"/>
-      <c r="BH75" s="51"/>
-      <c r="BI75" s="51"/>
-      <c r="BJ75" s="51"/>
-      <c r="BK75" s="51"/>
-      <c r="BL75" s="51"/>
-      <c r="BM75" s="51"/>
-      <c r="BN75" s="51"/>
-      <c r="BO75" s="51"/>
+      <c r="BF75" s="83"/>
+      <c r="BG75" s="83"/>
+      <c r="BH75" s="83"/>
+      <c r="BI75" s="83"/>
+      <c r="BJ75" s="83"/>
+      <c r="BK75" s="83"/>
+      <c r="BL75" s="83"/>
+      <c r="BM75" s="83"/>
+      <c r="BN75" s="83"/>
+      <c r="BO75" s="83"/>
     </row>
     <row r="76" spans="1:67">
       <c r="A76" s="29" t="s">
@@ -6875,11 +6887,11 @@
       <c r="D76" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="E76" s="57" t="s">
+      <c r="E76" s="72" t="s">
         <v>380</v>
       </c>
-      <c r="F76" s="71"/>
-      <c r="G76" s="58"/>
+      <c r="F76" s="73"/>
+      <c r="G76" s="74"/>
       <c r="H76" s="62" t="s">
         <v>233</v>
       </c>
@@ -6938,25 +6950,25 @@
       <c r="BC76" s="32"/>
       <c r="BD76" s="32"/>
       <c r="BE76" s="32"/>
-      <c r="BF76" s="51"/>
-      <c r="BG76" s="51"/>
-      <c r="BH76" s="51"/>
-      <c r="BI76" s="51"/>
-      <c r="BJ76" s="51"/>
-      <c r="BK76" s="51"/>
-      <c r="BL76" s="51"/>
-      <c r="BM76" s="51"/>
-      <c r="BN76" s="51"/>
-      <c r="BO76" s="51"/>
+      <c r="BF76" s="83"/>
+      <c r="BG76" s="83"/>
+      <c r="BH76" s="83"/>
+      <c r="BI76" s="83"/>
+      <c r="BJ76" s="83"/>
+      <c r="BK76" s="83"/>
+      <c r="BL76" s="83"/>
+      <c r="BM76" s="83"/>
+      <c r="BN76" s="83"/>
+      <c r="BO76" s="83"/>
     </row>
     <row r="77" spans="1:67">
       <c r="A77" s="12"/>
       <c r="B77" s="5"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
-      <c r="E77" s="63"/>
-      <c r="F77" s="63"/>
-      <c r="G77" s="63"/>
+      <c r="E77" s="75"/>
+      <c r="F77" s="75"/>
+      <c r="G77" s="75"/>
       <c r="H77" s="62"/>
       <c r="I77" s="62"/>
       <c r="J77" s="62"/>
@@ -8550,10 +8562,10 @@
       <c r="B131" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C131" s="52" t="s">
+      <c r="C131" s="67" t="s">
         <v>141</v>
       </c>
-      <c r="D131" s="52"/>
+      <c r="D131" s="67"/>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
@@ -8623,7 +8635,7 @@
       <c r="M133" s="19"/>
       <c r="N133" s="19"/>
       <c r="O133" s="19"/>
-      <c r="P133" s="19"/>
+      <c r="P133" s="41"/>
       <c r="Q133" s="19"/>
       <c r="R133" s="19"/>
       <c r="S133" s="19"/>
@@ -8652,7 +8664,7 @@
       <c r="M134" s="19"/>
       <c r="N134" s="19"/>
       <c r="O134" s="19"/>
-      <c r="P134" s="19"/>
+      <c r="P134" s="41"/>
       <c r="Q134" s="19"/>
       <c r="R134" s="19"/>
       <c r="S134" s="19"/>
@@ -8681,7 +8693,7 @@
       <c r="M135" s="19"/>
       <c r="N135" s="19"/>
       <c r="O135" s="19"/>
-      <c r="P135" s="19"/>
+      <c r="P135" s="41"/>
       <c r="Q135" s="19"/>
       <c r="R135" s="19"/>
       <c r="S135" s="19"/>
@@ -8696,15 +8708,15 @@
         <v>12</v>
       </c>
       <c r="C136" s="19" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
       <c r="K136" s="19"/>
       <c r="L136" s="19"/>
       <c r="M136" s="19"/>
       <c r="N136" s="19"/>
       <c r="O136" s="19"/>
-      <c r="P136" s="50" t="s">
-        <v>394</v>
+      <c r="P136" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q136" s="19"/>
       <c r="R136" s="19"/>
@@ -8714,13 +8726,13 @@
     </row>
     <row r="137" spans="1:21">
       <c r="A137" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B137" s="47" t="s">
         <v>311</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="D137" s="19"/>
       <c r="E137" s="19"/>
@@ -8734,8 +8746,8 @@
       <c r="M137" s="19"/>
       <c r="N137" s="19"/>
       <c r="O137" s="19"/>
-      <c r="P137" s="50" t="s">
-        <v>394</v>
+      <c r="P137" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q137" s="19"/>
       <c r="R137" s="19"/>
@@ -8751,7 +8763,7 @@
         <v>149</v>
       </c>
       <c r="C138" s="19" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="D138" s="19"/>
       <c r="E138" s="19"/>
@@ -8765,8 +8777,8 @@
       <c r="M138" s="19"/>
       <c r="N138" s="19"/>
       <c r="O138" s="19"/>
-      <c r="P138" s="50" t="s">
-        <v>394</v>
+      <c r="P138" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q138" s="19"/>
       <c r="R138" s="19"/>
@@ -8796,7 +8808,7 @@
       <c r="M139" s="19"/>
       <c r="N139" s="19"/>
       <c r="O139" s="19"/>
-      <c r="P139" s="19"/>
+      <c r="P139" s="41"/>
       <c r="Q139" s="19"/>
       <c r="R139" s="19"/>
       <c r="S139" s="19"/>
@@ -8825,8 +8837,8 @@
       <c r="M140" s="19"/>
       <c r="N140" s="19"/>
       <c r="O140" s="19"/>
-      <c r="P140" s="50" t="s">
-        <v>394</v>
+      <c r="P140" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q140" s="19"/>
       <c r="R140" s="19"/>
@@ -8856,8 +8868,8 @@
       <c r="M141" s="19"/>
       <c r="N141" s="19"/>
       <c r="O141" s="19"/>
-      <c r="P141" s="50" t="s">
-        <v>394</v>
+      <c r="P141" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q141" s="19"/>
       <c r="R141" s="19"/>
@@ -8887,8 +8899,8 @@
       <c r="M142" s="19"/>
       <c r="N142" s="19"/>
       <c r="O142" s="19"/>
-      <c r="P142" s="50" t="s">
-        <v>394</v>
+      <c r="P142" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q142" s="19"/>
       <c r="R142" s="19"/>
@@ -8918,8 +8930,8 @@
       <c r="M143" s="19"/>
       <c r="N143" s="19"/>
       <c r="O143" s="19"/>
-      <c r="P143" s="50" t="s">
-        <v>394</v>
+      <c r="P143" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q143" s="19"/>
       <c r="R143" s="19"/>
@@ -8949,8 +8961,8 @@
       <c r="M144" s="19"/>
       <c r="N144" s="19"/>
       <c r="O144" s="19"/>
-      <c r="P144" s="50" t="s">
-        <v>394</v>
+      <c r="P144" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q144" s="19"/>
       <c r="R144" s="19"/>
@@ -8980,7 +8992,7 @@
       <c r="M145" s="19"/>
       <c r="N145" s="19"/>
       <c r="O145" s="19"/>
-      <c r="P145" s="19"/>
+      <c r="P145" s="41"/>
       <c r="Q145" s="19"/>
       <c r="R145" s="19"/>
       <c r="S145" s="19"/>
@@ -9026,7 +9038,7 @@
       <c r="M147" s="19"/>
       <c r="N147" s="19"/>
       <c r="O147" s="19"/>
-      <c r="P147" s="19"/>
+      <c r="P147" s="89"/>
       <c r="Q147" s="19"/>
       <c r="R147" s="19"/>
       <c r="S147" s="19"/>
@@ -9049,7 +9061,7 @@
       <c r="M148" s="19"/>
       <c r="N148" s="19"/>
       <c r="O148" s="19"/>
-      <c r="P148" s="19"/>
+      <c r="P148" s="89"/>
       <c r="Q148" s="19"/>
       <c r="R148" s="19"/>
       <c r="S148" s="19"/>
@@ -9076,7 +9088,7 @@
       <c r="M149" s="19"/>
       <c r="N149" s="19"/>
       <c r="O149" s="19"/>
-      <c r="P149" s="19"/>
+      <c r="P149" s="89"/>
       <c r="Q149" s="19"/>
       <c r="R149" s="19"/>
       <c r="S149" s="19"/>
@@ -9105,8 +9117,8 @@
       <c r="M150" s="19"/>
       <c r="N150" s="19"/>
       <c r="O150" s="19"/>
-      <c r="P150" s="50" t="s">
-        <v>394</v>
+      <c r="P150" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q150" s="19"/>
       <c r="R150" s="19"/>
@@ -9136,8 +9148,8 @@
       <c r="M151" s="19"/>
       <c r="N151" s="19"/>
       <c r="O151" s="19"/>
-      <c r="P151" s="50" t="s">
-        <v>394</v>
+      <c r="P151" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q151" s="19"/>
       <c r="R151" s="19"/>
@@ -9167,7 +9179,7 @@
       <c r="M152" s="19"/>
       <c r="N152" s="19"/>
       <c r="O152" s="19"/>
-      <c r="P152" s="19"/>
+      <c r="P152" s="41"/>
       <c r="Q152" s="19"/>
       <c r="R152" s="19"/>
       <c r="S152" s="19"/>
@@ -9182,7 +9194,7 @@
         <v>149</v>
       </c>
       <c r="C153" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D153" s="19"/>
       <c r="E153" s="19"/>
@@ -9196,8 +9208,8 @@
       <c r="M153" s="19"/>
       <c r="N153" s="19"/>
       <c r="O153" s="19"/>
-      <c r="P153" s="50" t="s">
-        <v>394</v>
+      <c r="P153" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q153" s="19"/>
       <c r="R153" s="19"/>
@@ -9227,7 +9239,7 @@
       <c r="M154" s="19"/>
       <c r="N154" s="19"/>
       <c r="O154" s="19"/>
-      <c r="P154" s="19"/>
+      <c r="P154" s="41"/>
       <c r="Q154" s="19"/>
       <c r="R154" s="19"/>
       <c r="S154" s="19"/>
@@ -9256,7 +9268,7 @@
       <c r="M155" s="19"/>
       <c r="N155" s="19"/>
       <c r="O155" s="19"/>
-      <c r="P155" s="19"/>
+      <c r="P155" s="41"/>
       <c r="Q155" s="19"/>
       <c r="R155" s="19"/>
       <c r="S155" s="19"/>
@@ -9285,8 +9297,8 @@
       <c r="M156" s="19"/>
       <c r="N156" s="19"/>
       <c r="O156" s="19"/>
-      <c r="P156" s="50" t="s">
-        <v>394</v>
+      <c r="P156" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q156" s="19"/>
       <c r="R156" s="19"/>
@@ -9316,8 +9328,8 @@
       <c r="M157" s="19"/>
       <c r="N157" s="19"/>
       <c r="O157" s="19"/>
-      <c r="P157" s="50" t="s">
-        <v>394</v>
+      <c r="P157" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q157" s="19"/>
       <c r="R157" s="19"/>
@@ -9347,8 +9359,8 @@
       <c r="M158" s="19"/>
       <c r="N158" s="19"/>
       <c r="O158" s="19"/>
-      <c r="P158" s="50" t="s">
-        <v>394</v>
+      <c r="P158" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q158" s="19"/>
       <c r="R158" s="19"/>
@@ -9378,8 +9390,8 @@
       <c r="M159" s="19"/>
       <c r="N159" s="19"/>
       <c r="O159" s="19"/>
-      <c r="P159" s="50" t="s">
-        <v>394</v>
+      <c r="P159" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q159" s="19"/>
       <c r="R159" s="19"/>
@@ -9408,8 +9420,8 @@
       <c r="L160" s="19"/>
       <c r="M160" s="19"/>
       <c r="N160" s="19"/>
-      <c r="P160" s="50" t="s">
-        <v>394</v>
+      <c r="P160" s="88" t="s">
+        <v>391</v>
       </c>
       <c r="Q160" s="19"/>
       <c r="R160" s="19"/>
@@ -9425,7 +9437,7 @@
         <v>12</v>
       </c>
       <c r="C161" s="19" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D161" s="19"/>
       <c r="E161" s="19"/>
@@ -9438,7 +9450,7 @@
       <c r="L161" s="19"/>
       <c r="M161" s="19"/>
       <c r="N161" s="19"/>
-      <c r="P161" s="19"/>
+      <c r="P161" s="41"/>
       <c r="Q161" s="19"/>
       <c r="R161" s="19"/>
       <c r="S161" s="19"/>
@@ -9467,7 +9479,7 @@
       <c r="M162" s="19"/>
       <c r="N162" s="19"/>
       <c r="O162" s="19"/>
-      <c r="P162" s="19"/>
+      <c r="P162" s="41"/>
       <c r="Q162" s="19"/>
       <c r="R162" s="19"/>
       <c r="S162" s="19"/>
@@ -9490,7 +9502,7 @@
       <c r="M163" s="19"/>
       <c r="N163" s="19"/>
       <c r="O163" s="19"/>
-      <c r="P163" s="19"/>
+      <c r="P163" s="89"/>
       <c r="Q163" s="19"/>
       <c r="R163" s="19"/>
       <c r="S163" s="19"/>
@@ -9512,7 +9524,7 @@
       <c r="M164" s="19"/>
       <c r="N164" s="19"/>
       <c r="O164" s="19"/>
-      <c r="P164" s="19"/>
+      <c r="P164" s="89"/>
       <c r="Q164" s="19"/>
       <c r="R164" s="19"/>
       <c r="S164" s="19"/>
@@ -9534,7 +9546,7 @@
       <c r="M165" s="19"/>
       <c r="N165" s="19"/>
       <c r="O165" s="19"/>
-      <c r="P165" s="19"/>
+      <c r="P165" s="89"/>
       <c r="Q165" s="19"/>
       <c r="R165" s="19"/>
       <c r="S165" s="19"/>
@@ -9561,7 +9573,7 @@
       <c r="M166" s="19"/>
       <c r="N166" s="19"/>
       <c r="O166" s="19"/>
-      <c r="P166" s="19"/>
+      <c r="P166" s="89"/>
       <c r="Q166" s="19"/>
       <c r="R166" s="19"/>
       <c r="S166" s="19"/>
@@ -9588,7 +9600,7 @@
       <c r="M167" s="19"/>
       <c r="N167" s="19"/>
       <c r="O167" s="19"/>
-      <c r="P167" s="50"/>
+      <c r="P167" s="41"/>
       <c r="Q167" s="19"/>
       <c r="R167" s="19"/>
       <c r="S167" s="19"/>
@@ -9615,7 +9627,7 @@
       <c r="M168" s="19"/>
       <c r="N168" s="19"/>
       <c r="O168" s="19"/>
-      <c r="P168" s="50"/>
+      <c r="P168" s="41"/>
       <c r="Q168" s="19"/>
       <c r="R168" s="19"/>
       <c r="S168" s="19"/>
@@ -10270,45 +10282,45 @@
       <c r="A208" s="6"/>
       <c r="B208" s="6"/>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:16">
       <c r="A209" s="6"/>
       <c r="B209" s="6"/>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:16">
       <c r="A210" s="6"/>
       <c r="B210" s="6"/>
     </row>
-    <row r="211" spans="1:3">
+    <row r="211" spans="1:16">
       <c r="A211" s="6"/>
       <c r="B211" s="6"/>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:16">
       <c r="A212" s="6"/>
       <c r="B212" s="6"/>
     </row>
-    <row r="213" spans="1:3">
+    <row r="213" spans="1:16">
       <c r="A213" s="6"/>
       <c r="B213" s="6"/>
     </row>
-    <row r="214" spans="1:3">
+    <row r="214" spans="1:16">
       <c r="A214" s="6"/>
       <c r="B214" s="6"/>
     </row>
-    <row r="215" spans="1:3">
+    <row r="215" spans="1:16">
       <c r="A215" s="6"/>
       <c r="B215" s="6"/>
     </row>
-    <row r="216" spans="1:3">
+    <row r="216" spans="1:16">
       <c r="A216" s="6"/>
       <c r="B216" s="6"/>
     </row>
-    <row r="217" spans="1:3">
+    <row r="217" spans="1:16">
       <c r="A217" s="12" t="s">
         <v>366</v>
       </c>
       <c r="B217" s="6"/>
     </row>
-    <row r="218" spans="1:3">
+    <row r="218" spans="1:16">
       <c r="A218" s="6" t="s">
         <v>370</v>
       </c>
@@ -10319,7 +10331,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="219" spans="1:3">
+    <row r="219" spans="1:16">
       <c r="A219" s="6" t="s">
         <v>369</v>
       </c>
@@ -10327,26 +10339,34 @@
         <v>311</v>
       </c>
       <c r="C219" s="19" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3">
-      <c r="A220" s="6"/>
-      <c r="B220" s="6"/>
-    </row>
-    <row r="221" spans="1:3">
+        <v>392</v>
+      </c>
+      <c r="P219" s="90"/>
+    </row>
+    <row r="220" spans="1:16">
+      <c r="A220" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="B220" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C220" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="221" spans="1:16">
       <c r="A221" s="6"/>
       <c r="B221" s="6"/>
     </row>
-    <row r="222" spans="1:3">
+    <row r="222" spans="1:16">
       <c r="A222" s="6"/>
       <c r="B222" s="6"/>
     </row>
-    <row r="223" spans="1:3">
+    <row r="223" spans="1:16">
       <c r="A223" s="6"/>
       <c r="B223" s="6"/>
     </row>
-    <row r="224" spans="1:3">
+    <row r="224" spans="1:16">
       <c r="A224" s="6"/>
       <c r="B224" s="6"/>
     </row>
@@ -10476,6 +10496,537 @@
     </row>
   </sheetData>
   <mergeCells count="555">
+    <mergeCell ref="BF70:BO76"/>
+    <mergeCell ref="AB31:BO31"/>
+    <mergeCell ref="BG32:BO32"/>
+    <mergeCell ref="AB45:BO45"/>
+    <mergeCell ref="AB55:BO55"/>
+    <mergeCell ref="AB63:BO63"/>
+    <mergeCell ref="AB69:BO69"/>
+    <mergeCell ref="AB33:AE33"/>
+    <mergeCell ref="AF33:AH33"/>
+    <mergeCell ref="AI33:AJ33"/>
+    <mergeCell ref="AL33:AS33"/>
+    <mergeCell ref="AV33:AY33"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="A63:AA63"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="Y22:Z22"/>
+    <mergeCell ref="Y23:Z23"/>
+    <mergeCell ref="Y24:Z24"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="Y27:Z27"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="AG24:AH24"/>
+    <mergeCell ref="AG26:AH26"/>
+    <mergeCell ref="AG27:AH27"/>
+    <mergeCell ref="AG28:AH28"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="AG18:AH18"/>
+    <mergeCell ref="AG19:AH19"/>
+    <mergeCell ref="AG20:AH20"/>
+    <mergeCell ref="AG21:AH21"/>
+    <mergeCell ref="AG22:AH22"/>
+    <mergeCell ref="AG23:AH23"/>
+    <mergeCell ref="AC26:AD26"/>
+    <mergeCell ref="AC27:AD27"/>
+    <mergeCell ref="AC28:AD28"/>
+    <mergeCell ref="AC22:AD22"/>
+    <mergeCell ref="AC23:AD23"/>
+    <mergeCell ref="AC24:AD24"/>
+    <mergeCell ref="Y28:Z28"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="AG16:AH16"/>
+    <mergeCell ref="AG17:AH17"/>
+    <mergeCell ref="AC20:AD20"/>
+    <mergeCell ref="AC21:AD21"/>
+    <mergeCell ref="AC11:AD11"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AC13:AD13"/>
+    <mergeCell ref="AC14:AD14"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="AC16:AD16"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="Y20:Z20"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="U28:V28"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="AF10:AI10"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="T10:W10"/>
+    <mergeCell ref="X10:AA10"/>
+    <mergeCell ref="AB10:AE10"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="AG11:AH11"/>
+    <mergeCell ref="AG12:AH12"/>
+    <mergeCell ref="AG13:AH13"/>
+    <mergeCell ref="AG14:AH14"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="A45:AA45"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="H49:J49"/>
+    <mergeCell ref="H50:J50"/>
+    <mergeCell ref="H51:J51"/>
+    <mergeCell ref="H52:J52"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="H54:J54"/>
+    <mergeCell ref="H56:J56"/>
+    <mergeCell ref="K46:M46"/>
+    <mergeCell ref="K47:M47"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="K49:M49"/>
+    <mergeCell ref="K50:M50"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="K52:M52"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="E101:G101"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="N32:P32"/>
+    <mergeCell ref="Q32:S32"/>
+    <mergeCell ref="T32:Y32"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="E91:G91"/>
+    <mergeCell ref="E92:G92"/>
+    <mergeCell ref="E93:G93"/>
+    <mergeCell ref="E94:G94"/>
+    <mergeCell ref="E95:G95"/>
+    <mergeCell ref="E100:G100"/>
+    <mergeCell ref="E96:G96"/>
+    <mergeCell ref="E97:G97"/>
+    <mergeCell ref="E98:G98"/>
+    <mergeCell ref="E99:G99"/>
+    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="E83:G83"/>
+    <mergeCell ref="E84:G84"/>
+    <mergeCell ref="E85:G85"/>
+    <mergeCell ref="E86:G86"/>
+    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="E88:G88"/>
+    <mergeCell ref="E89:G89"/>
+    <mergeCell ref="E90:G90"/>
+    <mergeCell ref="H74:J74"/>
+    <mergeCell ref="H57:J57"/>
+    <mergeCell ref="H58:J58"/>
+    <mergeCell ref="H59:J59"/>
+    <mergeCell ref="H60:J60"/>
+    <mergeCell ref="H61:J61"/>
+    <mergeCell ref="H62:J62"/>
+    <mergeCell ref="H64:J64"/>
+    <mergeCell ref="H65:J65"/>
+    <mergeCell ref="H94:J94"/>
+    <mergeCell ref="H95:J95"/>
+    <mergeCell ref="H96:J96"/>
+    <mergeCell ref="H97:J97"/>
+    <mergeCell ref="H98:J98"/>
+    <mergeCell ref="H99:J99"/>
+    <mergeCell ref="H100:J100"/>
+    <mergeCell ref="H101:J101"/>
+    <mergeCell ref="H84:J84"/>
+    <mergeCell ref="H85:J85"/>
+    <mergeCell ref="H86:J86"/>
+    <mergeCell ref="H87:J87"/>
+    <mergeCell ref="H88:J88"/>
+    <mergeCell ref="H89:J89"/>
+    <mergeCell ref="H90:J90"/>
+    <mergeCell ref="H91:J91"/>
+    <mergeCell ref="H92:J92"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="H93:J93"/>
+    <mergeCell ref="H75:J75"/>
+    <mergeCell ref="H76:J76"/>
+    <mergeCell ref="H77:J77"/>
+    <mergeCell ref="H78:J78"/>
+    <mergeCell ref="H79:J79"/>
+    <mergeCell ref="H80:J80"/>
+    <mergeCell ref="H81:J81"/>
+    <mergeCell ref="H82:J82"/>
+    <mergeCell ref="H83:J83"/>
+    <mergeCell ref="H66:J66"/>
+    <mergeCell ref="H67:J67"/>
+    <mergeCell ref="H68:J68"/>
+    <mergeCell ref="H70:J70"/>
+    <mergeCell ref="H71:J71"/>
+    <mergeCell ref="H72:J72"/>
+    <mergeCell ref="H73:J73"/>
+    <mergeCell ref="K53:M53"/>
+    <mergeCell ref="K54:M54"/>
+    <mergeCell ref="K64:M64"/>
+    <mergeCell ref="K65:M65"/>
+    <mergeCell ref="K66:M66"/>
+    <mergeCell ref="K67:M67"/>
+    <mergeCell ref="K68:M68"/>
+    <mergeCell ref="K70:M70"/>
+    <mergeCell ref="K71:M71"/>
+    <mergeCell ref="K72:M72"/>
+    <mergeCell ref="K56:M56"/>
+    <mergeCell ref="K57:M57"/>
+    <mergeCell ref="K58:M58"/>
+    <mergeCell ref="K59:M59"/>
+    <mergeCell ref="K60:M60"/>
+    <mergeCell ref="K61:M61"/>
+    <mergeCell ref="K62:M62"/>
+    <mergeCell ref="K73:M73"/>
+    <mergeCell ref="K74:M74"/>
+    <mergeCell ref="K75:M75"/>
+    <mergeCell ref="K76:M76"/>
+    <mergeCell ref="K77:M77"/>
+    <mergeCell ref="K78:M78"/>
+    <mergeCell ref="K79:M79"/>
+    <mergeCell ref="K80:M80"/>
+    <mergeCell ref="K81:M81"/>
+    <mergeCell ref="K95:M95"/>
+    <mergeCell ref="K96:M96"/>
+    <mergeCell ref="K97:M97"/>
+    <mergeCell ref="K98:M98"/>
+    <mergeCell ref="K99:M99"/>
+    <mergeCell ref="K82:M82"/>
+    <mergeCell ref="K83:M83"/>
+    <mergeCell ref="K84:M84"/>
+    <mergeCell ref="K85:M85"/>
+    <mergeCell ref="K86:M86"/>
+    <mergeCell ref="K87:M87"/>
+    <mergeCell ref="K88:M88"/>
+    <mergeCell ref="K89:M89"/>
+    <mergeCell ref="K90:M90"/>
+    <mergeCell ref="K100:M100"/>
+    <mergeCell ref="K101:M101"/>
+    <mergeCell ref="N34:P34"/>
+    <mergeCell ref="N35:P35"/>
+    <mergeCell ref="N36:P36"/>
+    <mergeCell ref="N37:P37"/>
+    <mergeCell ref="N38:P38"/>
+    <mergeCell ref="N39:P39"/>
+    <mergeCell ref="N40:P40"/>
+    <mergeCell ref="N41:P41"/>
+    <mergeCell ref="N42:P42"/>
+    <mergeCell ref="N43:P43"/>
+    <mergeCell ref="N44:P44"/>
+    <mergeCell ref="N46:P46"/>
+    <mergeCell ref="N47:P47"/>
+    <mergeCell ref="N48:P48"/>
+    <mergeCell ref="N49:P49"/>
+    <mergeCell ref="N50:P50"/>
+    <mergeCell ref="N51:P51"/>
+    <mergeCell ref="N52:P52"/>
+    <mergeCell ref="K91:M91"/>
+    <mergeCell ref="K92:M92"/>
+    <mergeCell ref="K93:M93"/>
+    <mergeCell ref="K94:M94"/>
+    <mergeCell ref="N62:P62"/>
+    <mergeCell ref="N64:P64"/>
+    <mergeCell ref="N65:P65"/>
+    <mergeCell ref="N66:P66"/>
+    <mergeCell ref="N67:P67"/>
+    <mergeCell ref="N68:P68"/>
+    <mergeCell ref="N70:P70"/>
+    <mergeCell ref="N53:P53"/>
+    <mergeCell ref="N54:P54"/>
+    <mergeCell ref="N56:P56"/>
+    <mergeCell ref="N57:P57"/>
+    <mergeCell ref="N58:P58"/>
+    <mergeCell ref="N59:P59"/>
+    <mergeCell ref="N60:P60"/>
+    <mergeCell ref="N61:P61"/>
+    <mergeCell ref="N88:P88"/>
+    <mergeCell ref="N71:P71"/>
+    <mergeCell ref="N72:P72"/>
+    <mergeCell ref="N73:P73"/>
+    <mergeCell ref="N74:P74"/>
+    <mergeCell ref="N75:P75"/>
+    <mergeCell ref="N76:P76"/>
+    <mergeCell ref="N77:P77"/>
+    <mergeCell ref="N78:P78"/>
+    <mergeCell ref="N79:P79"/>
+    <mergeCell ref="N99:P99"/>
+    <mergeCell ref="N100:P100"/>
+    <mergeCell ref="N101:P101"/>
+    <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="Q35:S35"/>
+    <mergeCell ref="Q36:S36"/>
+    <mergeCell ref="Q37:S37"/>
+    <mergeCell ref="Q38:S38"/>
+    <mergeCell ref="Q39:S39"/>
+    <mergeCell ref="Q40:S40"/>
+    <mergeCell ref="Q41:S41"/>
+    <mergeCell ref="Q42:S42"/>
+    <mergeCell ref="Q43:S43"/>
+    <mergeCell ref="Q44:S44"/>
+    <mergeCell ref="Q46:S46"/>
+    <mergeCell ref="Q47:S47"/>
+    <mergeCell ref="Q48:S48"/>
+    <mergeCell ref="Q49:S49"/>
+    <mergeCell ref="Q50:S50"/>
+    <mergeCell ref="Q51:S51"/>
+    <mergeCell ref="Q52:S52"/>
+    <mergeCell ref="Q53:S53"/>
+    <mergeCell ref="N89:P89"/>
+    <mergeCell ref="N90:P90"/>
+    <mergeCell ref="Q54:S54"/>
+    <mergeCell ref="Q56:S56"/>
+    <mergeCell ref="Q57:S57"/>
+    <mergeCell ref="Q58:S58"/>
+    <mergeCell ref="Q59:S59"/>
+    <mergeCell ref="Q60:S60"/>
+    <mergeCell ref="Q61:S61"/>
+    <mergeCell ref="Q62:S62"/>
+    <mergeCell ref="N98:P98"/>
+    <mergeCell ref="N91:P91"/>
+    <mergeCell ref="N92:P92"/>
+    <mergeCell ref="N93:P93"/>
+    <mergeCell ref="N94:P94"/>
+    <mergeCell ref="N95:P95"/>
+    <mergeCell ref="N96:P96"/>
+    <mergeCell ref="N97:P97"/>
+    <mergeCell ref="N80:P80"/>
+    <mergeCell ref="N81:P81"/>
+    <mergeCell ref="N82:P82"/>
+    <mergeCell ref="N83:P83"/>
+    <mergeCell ref="N84:P84"/>
+    <mergeCell ref="N85:P85"/>
+    <mergeCell ref="N86:P86"/>
+    <mergeCell ref="N87:P87"/>
+    <mergeCell ref="Q73:S73"/>
+    <mergeCell ref="Q74:S74"/>
+    <mergeCell ref="Q75:S75"/>
+    <mergeCell ref="Q76:S76"/>
+    <mergeCell ref="Q77:S77"/>
+    <mergeCell ref="Q78:S78"/>
+    <mergeCell ref="Q79:S79"/>
+    <mergeCell ref="Q80:S80"/>
+    <mergeCell ref="Q64:S64"/>
+    <mergeCell ref="Q65:S65"/>
+    <mergeCell ref="Q66:S66"/>
+    <mergeCell ref="Q67:S67"/>
+    <mergeCell ref="Q68:S68"/>
+    <mergeCell ref="Q70:S70"/>
+    <mergeCell ref="Q71:S71"/>
+    <mergeCell ref="Q72:S72"/>
+    <mergeCell ref="Q100:S100"/>
+    <mergeCell ref="Q101:S101"/>
+    <mergeCell ref="T34:Y34"/>
+    <mergeCell ref="T35:Y35"/>
+    <mergeCell ref="T36:Y36"/>
+    <mergeCell ref="T37:Y37"/>
+    <mergeCell ref="T38:Y38"/>
+    <mergeCell ref="T39:Y39"/>
+    <mergeCell ref="T40:Y40"/>
+    <mergeCell ref="T41:Y41"/>
+    <mergeCell ref="T42:Y42"/>
+    <mergeCell ref="T43:Y43"/>
+    <mergeCell ref="T44:Y44"/>
+    <mergeCell ref="T46:Y46"/>
+    <mergeCell ref="T47:Y47"/>
+    <mergeCell ref="T48:Y48"/>
+    <mergeCell ref="T49:Y49"/>
+    <mergeCell ref="T50:Y50"/>
+    <mergeCell ref="T51:Y51"/>
+    <mergeCell ref="T52:Y52"/>
+    <mergeCell ref="T53:Y53"/>
+    <mergeCell ref="T54:Y54"/>
+    <mergeCell ref="Q90:S90"/>
+    <mergeCell ref="Q98:S98"/>
+    <mergeCell ref="Q81:S81"/>
+    <mergeCell ref="Q82:S82"/>
+    <mergeCell ref="Q83:S83"/>
+    <mergeCell ref="Q84:S84"/>
+    <mergeCell ref="Q85:S85"/>
+    <mergeCell ref="Q86:S86"/>
+    <mergeCell ref="Q87:S87"/>
+    <mergeCell ref="Q88:S88"/>
+    <mergeCell ref="Q89:S89"/>
+    <mergeCell ref="Q91:S91"/>
+    <mergeCell ref="C131:D131"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="T91:Y91"/>
+    <mergeCell ref="T92:Y92"/>
+    <mergeCell ref="T93:Y93"/>
+    <mergeCell ref="T94:Y94"/>
+    <mergeCell ref="T95:Y95"/>
+    <mergeCell ref="T96:Y96"/>
+    <mergeCell ref="T97:Y97"/>
+    <mergeCell ref="T98:Y98"/>
+    <mergeCell ref="T99:Y99"/>
+    <mergeCell ref="T82:Y82"/>
+    <mergeCell ref="T83:Y83"/>
+    <mergeCell ref="T84:Y84"/>
+    <mergeCell ref="T85:Y85"/>
+    <mergeCell ref="T86:Y86"/>
+    <mergeCell ref="T87:Y87"/>
+    <mergeCell ref="T88:Y88"/>
+    <mergeCell ref="T89:Y89"/>
+    <mergeCell ref="T90:Y90"/>
+    <mergeCell ref="T73:Y73"/>
+    <mergeCell ref="T74:Y74"/>
+    <mergeCell ref="T75:Y75"/>
+    <mergeCell ref="T76:Y76"/>
+    <mergeCell ref="T101:Y101"/>
+    <mergeCell ref="T77:Y77"/>
+    <mergeCell ref="T78:Y78"/>
+    <mergeCell ref="T79:Y79"/>
+    <mergeCell ref="T80:Y80"/>
+    <mergeCell ref="T81:Y81"/>
+    <mergeCell ref="T64:Y64"/>
+    <mergeCell ref="T65:Y65"/>
+    <mergeCell ref="T66:Y66"/>
+    <mergeCell ref="T67:Y67"/>
+    <mergeCell ref="T68:Y68"/>
+    <mergeCell ref="T70:Y70"/>
+    <mergeCell ref="T71:Y71"/>
+    <mergeCell ref="T72:Y72"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="A33:AA33"/>
     <mergeCell ref="A69:AA69"/>
@@ -10500,537 +11051,6 @@
     <mergeCell ref="Q95:S95"/>
     <mergeCell ref="Q96:S96"/>
     <mergeCell ref="Q97:S97"/>
-    <mergeCell ref="T76:Y76"/>
-    <mergeCell ref="T101:Y101"/>
-    <mergeCell ref="T77:Y77"/>
-    <mergeCell ref="T78:Y78"/>
-    <mergeCell ref="T79:Y79"/>
-    <mergeCell ref="T80:Y80"/>
-    <mergeCell ref="T81:Y81"/>
-    <mergeCell ref="T64:Y64"/>
-    <mergeCell ref="T65:Y65"/>
-    <mergeCell ref="T66:Y66"/>
-    <mergeCell ref="T67:Y67"/>
-    <mergeCell ref="T68:Y68"/>
-    <mergeCell ref="T70:Y70"/>
-    <mergeCell ref="T71:Y71"/>
-    <mergeCell ref="T72:Y72"/>
-    <mergeCell ref="Q91:S91"/>
-    <mergeCell ref="C131:D131"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="T91:Y91"/>
-    <mergeCell ref="T92:Y92"/>
-    <mergeCell ref="T93:Y93"/>
-    <mergeCell ref="T94:Y94"/>
-    <mergeCell ref="T95:Y95"/>
-    <mergeCell ref="T96:Y96"/>
-    <mergeCell ref="T97:Y97"/>
-    <mergeCell ref="T98:Y98"/>
-    <mergeCell ref="T99:Y99"/>
-    <mergeCell ref="T82:Y82"/>
-    <mergeCell ref="T83:Y83"/>
-    <mergeCell ref="T84:Y84"/>
-    <mergeCell ref="T85:Y85"/>
-    <mergeCell ref="T86:Y86"/>
-    <mergeCell ref="T87:Y87"/>
-    <mergeCell ref="T88:Y88"/>
-    <mergeCell ref="T89:Y89"/>
-    <mergeCell ref="T90:Y90"/>
-    <mergeCell ref="T73:Y73"/>
-    <mergeCell ref="T74:Y74"/>
-    <mergeCell ref="T75:Y75"/>
-    <mergeCell ref="Q81:S81"/>
-    <mergeCell ref="Q82:S82"/>
-    <mergeCell ref="Q83:S83"/>
-    <mergeCell ref="Q84:S84"/>
-    <mergeCell ref="Q85:S85"/>
-    <mergeCell ref="Q86:S86"/>
-    <mergeCell ref="Q87:S87"/>
-    <mergeCell ref="Q88:S88"/>
-    <mergeCell ref="Q89:S89"/>
-    <mergeCell ref="Q100:S100"/>
-    <mergeCell ref="Q101:S101"/>
-    <mergeCell ref="T34:Y34"/>
-    <mergeCell ref="T35:Y35"/>
-    <mergeCell ref="T36:Y36"/>
-    <mergeCell ref="T37:Y37"/>
-    <mergeCell ref="T38:Y38"/>
-    <mergeCell ref="T39:Y39"/>
-    <mergeCell ref="T40:Y40"/>
-    <mergeCell ref="T41:Y41"/>
-    <mergeCell ref="T42:Y42"/>
-    <mergeCell ref="T43:Y43"/>
-    <mergeCell ref="T44:Y44"/>
-    <mergeCell ref="T46:Y46"/>
-    <mergeCell ref="T47:Y47"/>
-    <mergeCell ref="T48:Y48"/>
-    <mergeCell ref="T49:Y49"/>
-    <mergeCell ref="T50:Y50"/>
-    <mergeCell ref="T51:Y51"/>
-    <mergeCell ref="T52:Y52"/>
-    <mergeCell ref="T53:Y53"/>
-    <mergeCell ref="T54:Y54"/>
-    <mergeCell ref="Q90:S90"/>
-    <mergeCell ref="Q98:S98"/>
-    <mergeCell ref="Q73:S73"/>
-    <mergeCell ref="Q74:S74"/>
-    <mergeCell ref="Q75:S75"/>
-    <mergeCell ref="Q76:S76"/>
-    <mergeCell ref="Q77:S77"/>
-    <mergeCell ref="Q78:S78"/>
-    <mergeCell ref="Q79:S79"/>
-    <mergeCell ref="Q80:S80"/>
-    <mergeCell ref="Q64:S64"/>
-    <mergeCell ref="Q65:S65"/>
-    <mergeCell ref="Q66:S66"/>
-    <mergeCell ref="Q67:S67"/>
-    <mergeCell ref="Q68:S68"/>
-    <mergeCell ref="Q70:S70"/>
-    <mergeCell ref="Q71:S71"/>
-    <mergeCell ref="Q72:S72"/>
-    <mergeCell ref="Q54:S54"/>
-    <mergeCell ref="Q56:S56"/>
-    <mergeCell ref="Q57:S57"/>
-    <mergeCell ref="Q58:S58"/>
-    <mergeCell ref="Q59:S59"/>
-    <mergeCell ref="Q60:S60"/>
-    <mergeCell ref="Q61:S61"/>
-    <mergeCell ref="Q62:S62"/>
-    <mergeCell ref="N98:P98"/>
-    <mergeCell ref="N91:P91"/>
-    <mergeCell ref="N92:P92"/>
-    <mergeCell ref="N93:P93"/>
-    <mergeCell ref="N94:P94"/>
-    <mergeCell ref="N95:P95"/>
-    <mergeCell ref="N96:P96"/>
-    <mergeCell ref="N97:P97"/>
-    <mergeCell ref="N80:P80"/>
-    <mergeCell ref="N81:P81"/>
-    <mergeCell ref="N82:P82"/>
-    <mergeCell ref="N83:P83"/>
-    <mergeCell ref="N84:P84"/>
-    <mergeCell ref="N85:P85"/>
-    <mergeCell ref="N86:P86"/>
-    <mergeCell ref="N87:P87"/>
-    <mergeCell ref="N99:P99"/>
-    <mergeCell ref="N100:P100"/>
-    <mergeCell ref="N101:P101"/>
-    <mergeCell ref="Q34:S34"/>
-    <mergeCell ref="Q35:S35"/>
-    <mergeCell ref="Q36:S36"/>
-    <mergeCell ref="Q37:S37"/>
-    <mergeCell ref="Q38:S38"/>
-    <mergeCell ref="Q39:S39"/>
-    <mergeCell ref="Q40:S40"/>
-    <mergeCell ref="Q41:S41"/>
-    <mergeCell ref="Q42:S42"/>
-    <mergeCell ref="Q43:S43"/>
-    <mergeCell ref="Q44:S44"/>
-    <mergeCell ref="Q46:S46"/>
-    <mergeCell ref="Q47:S47"/>
-    <mergeCell ref="Q48:S48"/>
-    <mergeCell ref="Q49:S49"/>
-    <mergeCell ref="Q50:S50"/>
-    <mergeCell ref="Q51:S51"/>
-    <mergeCell ref="Q52:S52"/>
-    <mergeCell ref="Q53:S53"/>
-    <mergeCell ref="N89:P89"/>
-    <mergeCell ref="N90:P90"/>
-    <mergeCell ref="N88:P88"/>
-    <mergeCell ref="N71:P71"/>
-    <mergeCell ref="N72:P72"/>
-    <mergeCell ref="N73:P73"/>
-    <mergeCell ref="N74:P74"/>
-    <mergeCell ref="N75:P75"/>
-    <mergeCell ref="N76:P76"/>
-    <mergeCell ref="N77:P77"/>
-    <mergeCell ref="N78:P78"/>
-    <mergeCell ref="N79:P79"/>
-    <mergeCell ref="N62:P62"/>
-    <mergeCell ref="N64:P64"/>
-    <mergeCell ref="N65:P65"/>
-    <mergeCell ref="N66:P66"/>
-    <mergeCell ref="N67:P67"/>
-    <mergeCell ref="N68:P68"/>
-    <mergeCell ref="N70:P70"/>
-    <mergeCell ref="N53:P53"/>
-    <mergeCell ref="N54:P54"/>
-    <mergeCell ref="N56:P56"/>
-    <mergeCell ref="N57:P57"/>
-    <mergeCell ref="N58:P58"/>
-    <mergeCell ref="N59:P59"/>
-    <mergeCell ref="N60:P60"/>
-    <mergeCell ref="N61:P61"/>
-    <mergeCell ref="K100:M100"/>
-    <mergeCell ref="K101:M101"/>
-    <mergeCell ref="N34:P34"/>
-    <mergeCell ref="N35:P35"/>
-    <mergeCell ref="N36:P36"/>
-    <mergeCell ref="N37:P37"/>
-    <mergeCell ref="N38:P38"/>
-    <mergeCell ref="N39:P39"/>
-    <mergeCell ref="N40:P40"/>
-    <mergeCell ref="N41:P41"/>
-    <mergeCell ref="N42:P42"/>
-    <mergeCell ref="N43:P43"/>
-    <mergeCell ref="N44:P44"/>
-    <mergeCell ref="N46:P46"/>
-    <mergeCell ref="N47:P47"/>
-    <mergeCell ref="N48:P48"/>
-    <mergeCell ref="N49:P49"/>
-    <mergeCell ref="N50:P50"/>
-    <mergeCell ref="N51:P51"/>
-    <mergeCell ref="N52:P52"/>
-    <mergeCell ref="K91:M91"/>
-    <mergeCell ref="K92:M92"/>
-    <mergeCell ref="K93:M93"/>
-    <mergeCell ref="K94:M94"/>
-    <mergeCell ref="K96:M96"/>
-    <mergeCell ref="K97:M97"/>
-    <mergeCell ref="K98:M98"/>
-    <mergeCell ref="K99:M99"/>
-    <mergeCell ref="K82:M82"/>
-    <mergeCell ref="K83:M83"/>
-    <mergeCell ref="K84:M84"/>
-    <mergeCell ref="K85:M85"/>
-    <mergeCell ref="K86:M86"/>
-    <mergeCell ref="K87:M87"/>
-    <mergeCell ref="K88:M88"/>
-    <mergeCell ref="K89:M89"/>
-    <mergeCell ref="K90:M90"/>
-    <mergeCell ref="K74:M74"/>
-    <mergeCell ref="K75:M75"/>
-    <mergeCell ref="K76:M76"/>
-    <mergeCell ref="K77:M77"/>
-    <mergeCell ref="K78:M78"/>
-    <mergeCell ref="K79:M79"/>
-    <mergeCell ref="K80:M80"/>
-    <mergeCell ref="K81:M81"/>
-    <mergeCell ref="K95:M95"/>
-    <mergeCell ref="K72:M72"/>
-    <mergeCell ref="K56:M56"/>
-    <mergeCell ref="K57:M57"/>
-    <mergeCell ref="K58:M58"/>
-    <mergeCell ref="K59:M59"/>
-    <mergeCell ref="K60:M60"/>
-    <mergeCell ref="K61:M61"/>
-    <mergeCell ref="K62:M62"/>
-    <mergeCell ref="K73:M73"/>
-    <mergeCell ref="K53:M53"/>
-    <mergeCell ref="K54:M54"/>
-    <mergeCell ref="K64:M64"/>
-    <mergeCell ref="K65:M65"/>
-    <mergeCell ref="K66:M66"/>
-    <mergeCell ref="K67:M67"/>
-    <mergeCell ref="K68:M68"/>
-    <mergeCell ref="K70:M70"/>
-    <mergeCell ref="K71:M71"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="K42:M42"/>
-    <mergeCell ref="K43:M43"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="H93:J93"/>
-    <mergeCell ref="H75:J75"/>
-    <mergeCell ref="H76:J76"/>
-    <mergeCell ref="H77:J77"/>
-    <mergeCell ref="H78:J78"/>
-    <mergeCell ref="H79:J79"/>
-    <mergeCell ref="H80:J80"/>
-    <mergeCell ref="H81:J81"/>
-    <mergeCell ref="H82:J82"/>
-    <mergeCell ref="H83:J83"/>
-    <mergeCell ref="H66:J66"/>
-    <mergeCell ref="H67:J67"/>
-    <mergeCell ref="H68:J68"/>
-    <mergeCell ref="H70:J70"/>
-    <mergeCell ref="H71:J71"/>
-    <mergeCell ref="H72:J72"/>
-    <mergeCell ref="H73:J73"/>
-    <mergeCell ref="H94:J94"/>
-    <mergeCell ref="H95:J95"/>
-    <mergeCell ref="H96:J96"/>
-    <mergeCell ref="H97:J97"/>
-    <mergeCell ref="H98:J98"/>
-    <mergeCell ref="H99:J99"/>
-    <mergeCell ref="H100:J100"/>
-    <mergeCell ref="H101:J101"/>
-    <mergeCell ref="H84:J84"/>
-    <mergeCell ref="H85:J85"/>
-    <mergeCell ref="H86:J86"/>
-    <mergeCell ref="H87:J87"/>
-    <mergeCell ref="H88:J88"/>
-    <mergeCell ref="H89:J89"/>
-    <mergeCell ref="H90:J90"/>
-    <mergeCell ref="H91:J91"/>
-    <mergeCell ref="H92:J92"/>
-    <mergeCell ref="H74:J74"/>
-    <mergeCell ref="H57:J57"/>
-    <mergeCell ref="H58:J58"/>
-    <mergeCell ref="H59:J59"/>
-    <mergeCell ref="H60:J60"/>
-    <mergeCell ref="H61:J61"/>
-    <mergeCell ref="H62:J62"/>
-    <mergeCell ref="H64:J64"/>
-    <mergeCell ref="H65:J65"/>
-    <mergeCell ref="E100:G100"/>
-    <mergeCell ref="E96:G96"/>
-    <mergeCell ref="E97:G97"/>
-    <mergeCell ref="E98:G98"/>
-    <mergeCell ref="E99:G99"/>
-    <mergeCell ref="E82:G82"/>
-    <mergeCell ref="E83:G83"/>
-    <mergeCell ref="E84:G84"/>
-    <mergeCell ref="E85:G85"/>
-    <mergeCell ref="E86:G86"/>
-    <mergeCell ref="E87:G87"/>
-    <mergeCell ref="E88:G88"/>
-    <mergeCell ref="E89:G89"/>
-    <mergeCell ref="E90:G90"/>
-    <mergeCell ref="E101:G101"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="K32:M32"/>
-    <mergeCell ref="N32:P32"/>
-    <mergeCell ref="Q32:S32"/>
-    <mergeCell ref="T32:Y32"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="E91:G91"/>
-    <mergeCell ref="E92:G92"/>
-    <mergeCell ref="E93:G93"/>
-    <mergeCell ref="E94:G94"/>
-    <mergeCell ref="E95:G95"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="E77:G77"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="E81:G81"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="E72:G72"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="A45:AA45"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="H49:J49"/>
-    <mergeCell ref="H50:J50"/>
-    <mergeCell ref="H51:J51"/>
-    <mergeCell ref="H52:J52"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="H54:J54"/>
-    <mergeCell ref="H56:J56"/>
-    <mergeCell ref="K46:M46"/>
-    <mergeCell ref="K47:M47"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="K49:M49"/>
-    <mergeCell ref="K50:M50"/>
-    <mergeCell ref="K51:M51"/>
-    <mergeCell ref="K52:M52"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="AF10:AI10"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="T10:W10"/>
-    <mergeCell ref="X10:AA10"/>
-    <mergeCell ref="AB10:AE10"/>
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="AG11:AH11"/>
-    <mergeCell ref="AG12:AH12"/>
-    <mergeCell ref="AG13:AH13"/>
-    <mergeCell ref="AG14:AH14"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="Y18:Z18"/>
-    <mergeCell ref="Y19:Z19"/>
-    <mergeCell ref="Y20:Z20"/>
-    <mergeCell ref="Y21:Z21"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="U28:V28"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="AG15:AH15"/>
-    <mergeCell ref="AG16:AH16"/>
-    <mergeCell ref="AG17:AH17"/>
-    <mergeCell ref="AC20:AD20"/>
-    <mergeCell ref="AC21:AD21"/>
-    <mergeCell ref="AC11:AD11"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AC13:AD13"/>
-    <mergeCell ref="AC14:AD14"/>
-    <mergeCell ref="AC15:AD15"/>
-    <mergeCell ref="AC16:AD16"/>
-    <mergeCell ref="AC17:AD17"/>
-    <mergeCell ref="AC18:AD18"/>
-    <mergeCell ref="AC19:AD19"/>
-    <mergeCell ref="AG24:AH24"/>
-    <mergeCell ref="AG26:AH26"/>
-    <mergeCell ref="AG27:AH27"/>
-    <mergeCell ref="AG28:AH28"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="AG18:AH18"/>
-    <mergeCell ref="AG19:AH19"/>
-    <mergeCell ref="AG20:AH20"/>
-    <mergeCell ref="AG21:AH21"/>
-    <mergeCell ref="AG22:AH22"/>
-    <mergeCell ref="AG23:AH23"/>
-    <mergeCell ref="AC26:AD26"/>
-    <mergeCell ref="AC27:AD27"/>
-    <mergeCell ref="AC28:AD28"/>
-    <mergeCell ref="AC22:AD22"/>
-    <mergeCell ref="AC23:AD23"/>
-    <mergeCell ref="AC24:AD24"/>
-    <mergeCell ref="Y28:Z28"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="A63:AA63"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="Y22:Z22"/>
-    <mergeCell ref="Y23:Z23"/>
-    <mergeCell ref="Y24:Z24"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="Y27:Z27"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="BF70:BO76"/>
-    <mergeCell ref="AB31:BO31"/>
-    <mergeCell ref="BG32:BO32"/>
-    <mergeCell ref="AB45:BO45"/>
-    <mergeCell ref="AB55:BO55"/>
-    <mergeCell ref="AB63:BO63"/>
-    <mergeCell ref="AB69:BO69"/>
-    <mergeCell ref="AB33:AE33"/>
-    <mergeCell ref="AF33:AH33"/>
-    <mergeCell ref="AI33:AJ33"/>
-    <mergeCell ref="AL33:AS33"/>
-    <mergeCell ref="AV33:AY33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added altar board reset frequency +1 bless
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingc\PycharmProjects\dice_game_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A967C9C-8576-4154-8E56-C28DE8757827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DE2755-58D8-4582-96BE-8B0635C49462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2756,6 +2756,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2778,15 +2787,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2849,6 +2849,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2869,15 +2878,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3355,15 +3355,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BP290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N118" sqref="N118"/>
+    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M172" sqref="M172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999"/>
   <cols>
     <col min="1" max="1" width="14.75" customWidth="1"/>
-    <col min="2" max="3" width="8.6640625" customWidth="1"/>
-    <col min="37" max="37" width="9.33203125" customWidth="1"/>
+    <col min="2" max="3" width="8.6875" customWidth="1"/>
+    <col min="37" max="37" width="9.3125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40">
@@ -3714,10 +3714,10 @@
       <c r="L12" s="5" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="M12" s="57" t="s">
+      <c r="M12" s="60" t="s">
         <v>153</v>
       </c>
-      <c r="N12" s="58"/>
+      <c r="N12" s="61"/>
       <c r="O12" s="10"/>
       <c r="P12" s="27" t="e" vm="2">
         <v>#VALUE!</v>
@@ -3725,44 +3725,44 @@
       <c r="Q12" s="87" t="s">
         <v>154</v>
       </c>
-      <c r="R12" s="58"/>
+      <c r="R12" s="61"/>
       <c r="S12" s="10"/>
       <c r="T12" s="9" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
-      <c r="U12" s="57" t="s">
+      <c r="U12" s="60" t="s">
         <v>155</v>
       </c>
-      <c r="V12" s="58"/>
+      <c r="V12" s="61"/>
       <c r="W12" s="10"/>
       <c r="X12" s="9" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
-      <c r="Y12" s="57" t="s">
+      <c r="Y12" s="60" t="s">
         <v>156</v>
       </c>
-      <c r="Z12" s="58"/>
+      <c r="Z12" s="61"/>
       <c r="AA12" s="10"/>
       <c r="AB12" s="9" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
-      <c r="AC12" s="57" t="s">
+      <c r="AC12" s="60" t="s">
         <v>420</v>
       </c>
-      <c r="AD12" s="58"/>
+      <c r="AD12" s="61"/>
       <c r="AE12" s="10"/>
       <c r="AF12" s="9" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
-      <c r="AG12" s="57" t="s">
+      <c r="AG12" s="60" t="s">
         <v>419</v>
       </c>
-      <c r="AH12" s="58"/>
+      <c r="AH12" s="61"/>
       <c r="AI12" s="10"/>
       <c r="AJ12" s="28" t="s">
         <v>356</v>
       </c>
-      <c r="AK12" s="96" t="s">
+      <c r="AK12" s="58" t="s">
         <v>370</v>
       </c>
       <c r="AL12" s="6" t="s">
@@ -3801,55 +3801,55 @@
       <c r="L13" s="5" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
-      <c r="M13" s="57" t="s">
+      <c r="M13" s="60" t="s">
         <v>451</v>
       </c>
-      <c r="N13" s="58"/>
+      <c r="N13" s="61"/>
       <c r="O13" s="10"/>
       <c r="P13" s="9" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
-      <c r="Q13" s="57" t="s">
+      <c r="Q13" s="60" t="s">
         <v>450</v>
       </c>
-      <c r="R13" s="58"/>
+      <c r="R13" s="61"/>
       <c r="S13" s="10"/>
       <c r="T13" s="9" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
-      <c r="U13" s="57" t="s">
+      <c r="U13" s="60" t="s">
         <v>448</v>
       </c>
-      <c r="V13" s="58"/>
+      <c r="V13" s="61"/>
       <c r="W13" s="10"/>
       <c r="X13" s="9" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
-      <c r="Y13" s="57" t="s">
+      <c r="Y13" s="60" t="s">
         <v>449</v>
       </c>
-      <c r="Z13" s="58"/>
+      <c r="Z13" s="61"/>
       <c r="AA13" s="10"/>
       <c r="AB13" s="9" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
-      <c r="AC13" s="57" t="s">
+      <c r="AC13" s="60" t="s">
         <v>447</v>
       </c>
-      <c r="AD13" s="58"/>
+      <c r="AD13" s="61"/>
       <c r="AE13" s="10"/>
       <c r="AF13" s="9" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
-      <c r="AG13" s="57" t="s">
+      <c r="AG13" s="60" t="s">
         <v>446</v>
       </c>
-      <c r="AH13" s="58"/>
+      <c r="AH13" s="61"/>
       <c r="AI13" s="10"/>
       <c r="AJ13" s="28" t="s">
         <v>356</v>
       </c>
-      <c r="AK13" s="95" t="s">
+      <c r="AK13" s="57" t="s">
         <v>455</v>
       </c>
       <c r="AL13" s="25" t="s">
@@ -3890,55 +3890,55 @@
       <c r="L14" s="5" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
-      <c r="M14" s="57" t="s">
+      <c r="M14" s="60" t="s">
         <v>431</v>
       </c>
-      <c r="N14" s="58"/>
+      <c r="N14" s="61"/>
       <c r="O14" s="10"/>
       <c r="P14" s="9" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
-      <c r="Q14" s="57" t="s">
+      <c r="Q14" s="60" t="s">
         <v>432</v>
       </c>
-      <c r="R14" s="58"/>
+      <c r="R14" s="61"/>
       <c r="S14" s="10"/>
       <c r="T14" s="9" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
-      <c r="U14" s="57" t="s">
+      <c r="U14" s="60" t="s">
         <v>433</v>
       </c>
-      <c r="V14" s="58"/>
+      <c r="V14" s="61"/>
       <c r="W14" s="10"/>
       <c r="X14" s="9" t="e" vm="16">
         <v>#VALUE!</v>
       </c>
-      <c r="Y14" s="57" t="s">
+      <c r="Y14" s="60" t="s">
         <v>436</v>
       </c>
-      <c r="Z14" s="58"/>
+      <c r="Z14" s="61"/>
       <c r="AA14" s="10"/>
       <c r="AB14" s="9" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
-      <c r="AC14" s="57" t="s">
+      <c r="AC14" s="60" t="s">
         <v>434</v>
       </c>
-      <c r="AD14" s="58"/>
+      <c r="AD14" s="61"/>
       <c r="AE14" s="10"/>
       <c r="AF14" s="9" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
-      <c r="AG14" s="57" t="s">
+      <c r="AG14" s="60" t="s">
         <v>435</v>
       </c>
-      <c r="AH14" s="58"/>
+      <c r="AH14" s="61"/>
       <c r="AI14" s="10"/>
       <c r="AJ14" s="28" t="s">
         <v>356</v>
       </c>
-      <c r="AK14" s="97" t="s">
+      <c r="AK14" s="59" t="s">
         <v>456</v>
       </c>
       <c r="AL14" s="49" t="s">
@@ -3968,47 +3968,47 @@
       <c r="G15" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H15" s="57" t="s">
+      <c r="H15" s="60" t="s">
         <v>375</v>
       </c>
-      <c r="I15" s="58"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="58"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="61"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="57" t="s">
+      <c r="M15" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="N15" s="58"/>
+      <c r="N15" s="61"/>
       <c r="O15" s="10"/>
       <c r="P15" s="9"/>
-      <c r="Q15" s="57" t="s">
+      <c r="Q15" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="R15" s="58"/>
+      <c r="R15" s="61"/>
       <c r="S15" s="10"/>
       <c r="T15" s="9"/>
-      <c r="U15" s="57" t="s">
+      <c r="U15" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="V15" s="58"/>
+      <c r="V15" s="61"/>
       <c r="W15" s="10"/>
       <c r="X15" s="9"/>
-      <c r="Y15" s="57" t="s">
+      <c r="Y15" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="Z15" s="58"/>
+      <c r="Z15" s="61"/>
       <c r="AA15" s="10"/>
       <c r="AB15" s="5"/>
-      <c r="AC15" s="57" t="s">
+      <c r="AC15" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="AD15" s="58"/>
+      <c r="AD15" s="61"/>
       <c r="AE15" s="10"/>
       <c r="AF15" s="9"/>
-      <c r="AG15" s="57" t="s">
+      <c r="AG15" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="AH15" s="58"/>
+      <c r="AH15" s="61"/>
       <c r="AI15" s="10"/>
       <c r="AJ15" s="6"/>
       <c r="AK15" s="6"/>
@@ -4046,40 +4046,40 @@
       </c>
       <c r="K16" s="69"/>
       <c r="L16" s="5"/>
-      <c r="M16" s="57" t="s">
+      <c r="M16" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="N16" s="58"/>
+      <c r="N16" s="61"/>
       <c r="O16" s="10"/>
       <c r="P16" s="9"/>
-      <c r="Q16" s="57" t="s">
+      <c r="Q16" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="R16" s="58"/>
+      <c r="R16" s="61"/>
       <c r="S16" s="10"/>
       <c r="T16" s="9"/>
-      <c r="U16" s="57" t="s">
+      <c r="U16" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="V16" s="58"/>
+      <c r="V16" s="61"/>
       <c r="W16" s="10"/>
       <c r="X16" s="9"/>
-      <c r="Y16" s="57" t="s">
+      <c r="Y16" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="Z16" s="58"/>
+      <c r="Z16" s="61"/>
       <c r="AA16" s="10"/>
       <c r="AB16" s="9"/>
-      <c r="AC16" s="57" t="s">
+      <c r="AC16" s="60" t="s">
         <v>132</v>
       </c>
-      <c r="AD16" s="58"/>
+      <c r="AD16" s="61"/>
       <c r="AE16" s="10"/>
       <c r="AF16" s="9"/>
-      <c r="AG16" s="57" t="s">
+      <c r="AG16" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="AH16" s="58"/>
+      <c r="AH16" s="61"/>
       <c r="AI16" s="10"/>
       <c r="AJ16" s="6"/>
       <c r="AK16" s="6"/>
@@ -4176,34 +4176,34 @@
       </c>
       <c r="K18" s="69"/>
       <c r="L18" s="5"/>
-      <c r="M18" s="57" t="s">
+      <c r="M18" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="N18" s="58"/>
+      <c r="N18" s="61"/>
       <c r="O18" s="10"/>
       <c r="P18" s="9"/>
-      <c r="Q18" s="57" t="s">
+      <c r="Q18" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="R18" s="58"/>
+      <c r="R18" s="61"/>
       <c r="S18" s="10"/>
       <c r="T18" s="9"/>
-      <c r="U18" s="57"/>
-      <c r="V18" s="58"/>
+      <c r="U18" s="60"/>
+      <c r="V18" s="61"/>
       <c r="W18" s="10"/>
       <c r="X18" s="9"/>
-      <c r="Y18" s="57"/>
-      <c r="Z18" s="58"/>
+      <c r="Y18" s="60"/>
+      <c r="Z18" s="61"/>
       <c r="AA18" s="10"/>
       <c r="AB18" s="9"/>
-      <c r="AC18" s="57"/>
-      <c r="AD18" s="58"/>
+      <c r="AC18" s="60"/>
+      <c r="AD18" s="61"/>
       <c r="AE18" s="10"/>
       <c r="AF18" s="9"/>
-      <c r="AG18" s="57" t="s">
+      <c r="AG18" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="AH18" s="58"/>
+      <c r="AH18" s="61"/>
       <c r="AI18" s="10"/>
       <c r="AJ18" s="6"/>
       <c r="AK18" s="6"/>
@@ -4225,31 +4225,31 @@
       <c r="G19" s="6"/>
       <c r="H19" s="79"/>
       <c r="I19" s="81"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="58"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="61"/>
       <c r="L19" s="5"/>
       <c r="M19" s="79"/>
       <c r="N19" s="81"/>
       <c r="O19" s="10"/>
       <c r="P19" s="9"/>
-      <c r="Q19" s="57"/>
-      <c r="R19" s="58"/>
+      <c r="Q19" s="60"/>
+      <c r="R19" s="61"/>
       <c r="S19" s="10"/>
       <c r="T19" s="9"/>
-      <c r="U19" s="57"/>
-      <c r="V19" s="58"/>
+      <c r="U19" s="60"/>
+      <c r="V19" s="61"/>
       <c r="W19" s="10"/>
       <c r="X19" s="9"/>
-      <c r="Y19" s="57"/>
-      <c r="Z19" s="58"/>
+      <c r="Y19" s="60"/>
+      <c r="Z19" s="61"/>
       <c r="AA19" s="10"/>
       <c r="AB19" s="9"/>
-      <c r="AC19" s="57"/>
-      <c r="AD19" s="58"/>
+      <c r="AC19" s="60"/>
+      <c r="AD19" s="61"/>
       <c r="AE19" s="10"/>
       <c r="AF19" s="9"/>
-      <c r="AG19" s="57"/>
-      <c r="AH19" s="58"/>
+      <c r="AG19" s="60"/>
+      <c r="AH19" s="61"/>
       <c r="AI19" s="10"/>
       <c r="AJ19" s="6"/>
       <c r="AK19" s="6"/>
@@ -4268,31 +4268,31 @@
       <c r="G20" s="6"/>
       <c r="H20" s="79"/>
       <c r="I20" s="81"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="58"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="61"/>
       <c r="L20" s="5"/>
       <c r="M20" s="79"/>
       <c r="N20" s="81"/>
       <c r="O20" s="10"/>
       <c r="P20" s="9"/>
-      <c r="Q20" s="57"/>
-      <c r="R20" s="58"/>
+      <c r="Q20" s="60"/>
+      <c r="R20" s="61"/>
       <c r="S20" s="10"/>
       <c r="T20" s="9"/>
-      <c r="U20" s="57"/>
-      <c r="V20" s="58"/>
+      <c r="U20" s="60"/>
+      <c r="V20" s="61"/>
       <c r="W20" s="10"/>
       <c r="X20" s="9"/>
-      <c r="Y20" s="57"/>
-      <c r="Z20" s="58"/>
+      <c r="Y20" s="60"/>
+      <c r="Z20" s="61"/>
       <c r="AA20" s="10"/>
       <c r="AB20" s="9"/>
-      <c r="AC20" s="57"/>
-      <c r="AD20" s="58"/>
+      <c r="AC20" s="60"/>
+      <c r="AD20" s="61"/>
       <c r="AE20" s="10"/>
       <c r="AF20" s="9"/>
-      <c r="AG20" s="57"/>
-      <c r="AH20" s="58"/>
+      <c r="AG20" s="60"/>
+      <c r="AH20" s="61"/>
       <c r="AI20" s="10"/>
       <c r="AJ20" s="6"/>
       <c r="AK20" s="6"/>
@@ -4301,7 +4301,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:67" ht="17.5" hidden="1">
+    <row r="21" spans="1:67" ht="19.149999999999999" hidden="1">
       <c r="A21" s="7"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -4311,31 +4311,31 @@
       <c r="G21" s="6"/>
       <c r="H21" s="79"/>
       <c r="I21" s="81"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="58"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="61"/>
       <c r="L21" s="5"/>
       <c r="M21" s="79"/>
       <c r="N21" s="81"/>
       <c r="O21" s="10"/>
       <c r="P21" s="9"/>
-      <c r="Q21" s="57"/>
-      <c r="R21" s="58"/>
+      <c r="Q21" s="60"/>
+      <c r="R21" s="61"/>
       <c r="S21" s="10"/>
       <c r="T21" s="9"/>
-      <c r="U21" s="57"/>
-      <c r="V21" s="58"/>
+      <c r="U21" s="60"/>
+      <c r="V21" s="61"/>
       <c r="W21" s="10"/>
       <c r="X21" s="9"/>
-      <c r="Y21" s="57"/>
-      <c r="Z21" s="58"/>
+      <c r="Y21" s="60"/>
+      <c r="Z21" s="61"/>
       <c r="AA21" s="10"/>
       <c r="AB21" s="9"/>
-      <c r="AC21" s="57"/>
-      <c r="AD21" s="58"/>
+      <c r="AC21" s="60"/>
+      <c r="AD21" s="61"/>
       <c r="AE21" s="10"/>
       <c r="AF21" s="9"/>
-      <c r="AG21" s="57"/>
-      <c r="AH21" s="58"/>
+      <c r="AG21" s="60"/>
+      <c r="AH21" s="61"/>
       <c r="AI21" s="10"/>
       <c r="AJ21" s="6"/>
       <c r="AK21" s="6"/>
@@ -4369,31 +4369,31 @@
       <c r="G22" s="6"/>
       <c r="H22" s="79"/>
       <c r="I22" s="81"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="58"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="61"/>
       <c r="L22" s="5"/>
       <c r="M22" s="79"/>
       <c r="N22" s="81"/>
       <c r="O22" s="10"/>
       <c r="P22" s="9"/>
-      <c r="Q22" s="57"/>
-      <c r="R22" s="58"/>
+      <c r="Q22" s="60"/>
+      <c r="R22" s="61"/>
       <c r="S22" s="10"/>
       <c r="T22" s="9"/>
-      <c r="U22" s="57"/>
-      <c r="V22" s="58"/>
+      <c r="U22" s="60"/>
+      <c r="V22" s="61"/>
       <c r="W22" s="10"/>
       <c r="X22" s="9"/>
-      <c r="Y22" s="57"/>
-      <c r="Z22" s="58"/>
+      <c r="Y22" s="60"/>
+      <c r="Z22" s="61"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="9"/>
-      <c r="AC22" s="57"/>
-      <c r="AD22" s="58"/>
+      <c r="AC22" s="60"/>
+      <c r="AD22" s="61"/>
       <c r="AE22" s="10"/>
       <c r="AF22" s="9"/>
-      <c r="AG22" s="57"/>
-      <c r="AH22" s="58"/>
+      <c r="AG22" s="60"/>
+      <c r="AH22" s="61"/>
       <c r="AI22" s="10"/>
       <c r="AJ22" s="6"/>
       <c r="AK22" s="6"/>
@@ -4411,31 +4411,31 @@
       <c r="G23" s="6"/>
       <c r="H23" s="79"/>
       <c r="I23" s="81"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="58"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="61"/>
       <c r="L23" s="5"/>
       <c r="M23" s="79"/>
       <c r="N23" s="81"/>
       <c r="O23" s="10"/>
       <c r="P23" s="9"/>
-      <c r="Q23" s="57"/>
-      <c r="R23" s="58"/>
+      <c r="Q23" s="60"/>
+      <c r="R23" s="61"/>
       <c r="S23" s="10"/>
       <c r="T23" s="9"/>
-      <c r="U23" s="57"/>
-      <c r="V23" s="58"/>
+      <c r="U23" s="60"/>
+      <c r="V23" s="61"/>
       <c r="W23" s="10"/>
       <c r="X23" s="9"/>
-      <c r="Y23" s="57"/>
-      <c r="Z23" s="58"/>
+      <c r="Y23" s="60"/>
+      <c r="Z23" s="61"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="9"/>
-      <c r="AC23" s="57"/>
-      <c r="AD23" s="58"/>
+      <c r="AC23" s="60"/>
+      <c r="AD23" s="61"/>
       <c r="AE23" s="10"/>
       <c r="AF23" s="9"/>
-      <c r="AG23" s="57"/>
-      <c r="AH23" s="58"/>
+      <c r="AG23" s="60"/>
+      <c r="AH23" s="61"/>
       <c r="AI23" s="10"/>
       <c r="AJ23" s="6"/>
       <c r="AK23" s="6"/>
@@ -4453,31 +4453,31 @@
       <c r="G24" s="6"/>
       <c r="H24" s="79"/>
       <c r="I24" s="81"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="58"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="61"/>
       <c r="L24" s="5"/>
       <c r="M24" s="79"/>
       <c r="N24" s="81"/>
       <c r="O24" s="10"/>
       <c r="P24" s="9"/>
-      <c r="Q24" s="57"/>
-      <c r="R24" s="58"/>
+      <c r="Q24" s="60"/>
+      <c r="R24" s="61"/>
       <c r="S24" s="10"/>
       <c r="T24" s="9"/>
-      <c r="U24" s="57"/>
-      <c r="V24" s="58"/>
+      <c r="U24" s="60"/>
+      <c r="V24" s="61"/>
       <c r="W24" s="10"/>
       <c r="X24" s="9"/>
-      <c r="Y24" s="57"/>
-      <c r="Z24" s="58"/>
+      <c r="Y24" s="60"/>
+      <c r="Z24" s="61"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="9"/>
-      <c r="AC24" s="57"/>
-      <c r="AD24" s="58"/>
+      <c r="AC24" s="60"/>
+      <c r="AD24" s="61"/>
       <c r="AE24" s="10"/>
       <c r="AF24" s="9"/>
-      <c r="AG24" s="57"/>
-      <c r="AH24" s="58"/>
+      <c r="AG24" s="60"/>
+      <c r="AH24" s="61"/>
       <c r="AI24" s="10"/>
       <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
@@ -4488,52 +4488,52 @@
       <c r="AW24" s="20"/>
     </row>
     <row r="25" spans="1:67">
-      <c r="A25" s="65" t="s">
+      <c r="A25" s="88" t="s">
         <v>192</v>
       </c>
-      <c r="B25" s="66"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="66"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="66"/>
-      <c r="J25" s="66"/>
-      <c r="K25" s="66"/>
-      <c r="L25" s="66"/>
-      <c r="M25" s="66"/>
-      <c r="N25" s="66"/>
-      <c r="O25" s="66"/>
-      <c r="P25" s="66"/>
-      <c r="Q25" s="66"/>
-      <c r="R25" s="66"/>
-      <c r="S25" s="66"/>
-      <c r="T25" s="66"/>
-      <c r="U25" s="66"/>
-      <c r="V25" s="66"/>
-      <c r="W25" s="66"/>
-      <c r="X25" s="66"/>
-      <c r="Y25" s="66"/>
-      <c r="Z25" s="66"/>
-      <c r="AA25" s="66"/>
-      <c r="AB25" s="66"/>
-      <c r="AC25" s="66"/>
-      <c r="AD25" s="66"/>
-      <c r="AE25" s="66"/>
-      <c r="AF25" s="66"/>
-      <c r="AG25" s="66"/>
-      <c r="AH25" s="66"/>
-      <c r="AI25" s="66"/>
-      <c r="AJ25" s="66"/>
-      <c r="AK25" s="66"/>
-      <c r="AL25" s="67"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="89"/>
+      <c r="I25" s="89"/>
+      <c r="J25" s="89"/>
+      <c r="K25" s="89"/>
+      <c r="L25" s="89"/>
+      <c r="M25" s="89"/>
+      <c r="N25" s="89"/>
+      <c r="O25" s="89"/>
+      <c r="P25" s="89"/>
+      <c r="Q25" s="89"/>
+      <c r="R25" s="89"/>
+      <c r="S25" s="89"/>
+      <c r="T25" s="89"/>
+      <c r="U25" s="89"/>
+      <c r="V25" s="89"/>
+      <c r="W25" s="89"/>
+      <c r="X25" s="89"/>
+      <c r="Y25" s="89"/>
+      <c r="Z25" s="89"/>
+      <c r="AA25" s="89"/>
+      <c r="AB25" s="89"/>
+      <c r="AC25" s="89"/>
+      <c r="AD25" s="89"/>
+      <c r="AE25" s="89"/>
+      <c r="AF25" s="89"/>
+      <c r="AG25" s="89"/>
+      <c r="AH25" s="89"/>
+      <c r="AI25" s="89"/>
+      <c r="AJ25" s="89"/>
+      <c r="AK25" s="89"/>
+      <c r="AL25" s="90"/>
       <c r="AV25" s="19" t="s">
         <v>109</v>
       </c>
       <c r="AW25" s="20"/>
     </row>
-    <row r="26" spans="1:67" ht="53.5" customHeight="1">
+    <row r="26" spans="1:67" ht="53.55" customHeight="1">
       <c r="A26" s="7" t="s">
         <v>193</v>
       </c>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="AW26" s="20"/>
     </row>
-    <row r="27" spans="1:67" ht="53.5" customHeight="1">
+    <row r="27" spans="1:67" ht="53.55" customHeight="1">
       <c r="A27" s="7" t="s">
         <v>207</v>
       </c>
@@ -4655,7 +4655,7 @@
       </c>
       <c r="AW27" s="20"/>
     </row>
-    <row r="28" spans="1:67" ht="53.5" customHeight="1">
+    <row r="28" spans="1:67" ht="53.55" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>194</v>
       </c>
@@ -4934,69 +4934,69 @@
       <c r="BO32" s="74"/>
     </row>
     <row r="33" spans="1:67">
-      <c r="A33" s="59" t="s">
+      <c r="A33" s="62" t="s">
         <v>190</v>
       </c>
-      <c r="B33" s="60"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="60"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="60"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="60"/>
-      <c r="N33" s="60"/>
-      <c r="O33" s="60"/>
-      <c r="P33" s="60"/>
-      <c r="Q33" s="60"/>
-      <c r="R33" s="60"/>
-      <c r="S33" s="60"/>
-      <c r="T33" s="60"/>
-      <c r="U33" s="60"/>
-      <c r="V33" s="60"/>
-      <c r="W33" s="60"/>
-      <c r="X33" s="60"/>
-      <c r="Y33" s="60"/>
-      <c r="Z33" s="60"/>
-      <c r="AA33" s="61"/>
-      <c r="AB33" s="92" t="s">
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="63"/>
+      <c r="O33" s="63"/>
+      <c r="P33" s="63"/>
+      <c r="Q33" s="63"/>
+      <c r="R33" s="63"/>
+      <c r="S33" s="63"/>
+      <c r="T33" s="63"/>
+      <c r="U33" s="63"/>
+      <c r="V33" s="63"/>
+      <c r="W33" s="63"/>
+      <c r="X33" s="63"/>
+      <c r="Y33" s="63"/>
+      <c r="Z33" s="63"/>
+      <c r="AA33" s="64"/>
+      <c r="AB33" s="95" t="s">
         <v>257</v>
       </c>
-      <c r="AC33" s="93"/>
-      <c r="AD33" s="93"/>
-      <c r="AE33" s="93"/>
-      <c r="AF33" s="94" t="s">
+      <c r="AC33" s="96"/>
+      <c r="AD33" s="96"/>
+      <c r="AE33" s="96"/>
+      <c r="AF33" s="97" t="s">
         <v>256</v>
       </c>
-      <c r="AG33" s="94"/>
-      <c r="AH33" s="94"/>
-      <c r="AI33" s="93" t="s">
+      <c r="AG33" s="97"/>
+      <c r="AH33" s="97"/>
+      <c r="AI33" s="96" t="s">
         <v>258</v>
       </c>
-      <c r="AJ33" s="93"/>
+      <c r="AJ33" s="96"/>
       <c r="AK33" s="39"/>
-      <c r="AL33" s="93" t="s">
+      <c r="AL33" s="96" t="s">
         <v>259</v>
       </c>
-      <c r="AM33" s="93"/>
-      <c r="AN33" s="93"/>
-      <c r="AO33" s="93"/>
-      <c r="AP33" s="93"/>
-      <c r="AQ33" s="93"/>
-      <c r="AR33" s="93"/>
-      <c r="AS33" s="93"/>
+      <c r="AM33" s="96"/>
+      <c r="AN33" s="96"/>
+      <c r="AO33" s="96"/>
+      <c r="AP33" s="96"/>
+      <c r="AQ33" s="96"/>
+      <c r="AR33" s="96"/>
+      <c r="AS33" s="96"/>
       <c r="AT33" s="39"/>
       <c r="AU33" s="39"/>
-      <c r="AV33" s="93" t="s">
+      <c r="AV33" s="96" t="s">
         <v>260</v>
       </c>
-      <c r="AW33" s="93"/>
-      <c r="AX33" s="93"/>
-      <c r="AY33" s="93"/>
+      <c r="AW33" s="96"/>
+      <c r="AX33" s="96"/>
+      <c r="AY33" s="96"/>
       <c r="AZ33" s="39"/>
       <c r="BA33" s="39"/>
       <c r="BB33" s="39"/>
@@ -5025,24 +5025,24 @@
       <c r="D34" s="6">
         <v>1</v>
       </c>
-      <c r="E34" s="57"/>
+      <c r="E34" s="60"/>
       <c r="F34" s="78"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="57" t="s">
+      <c r="G34" s="61"/>
+      <c r="H34" s="60" t="s">
         <v>223</v>
       </c>
       <c r="I34" s="78"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="57" t="s">
+      <c r="J34" s="61"/>
+      <c r="K34" s="60" t="s">
         <v>229</v>
       </c>
       <c r="L34" s="78"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="57" t="s">
+      <c r="M34" s="61"/>
+      <c r="N34" s="60" t="s">
         <v>230</v>
       </c>
       <c r="O34" s="78"/>
-      <c r="P34" s="58"/>
+      <c r="P34" s="61"/>
       <c r="Q34" s="79"/>
       <c r="R34" s="80"/>
       <c r="S34" s="81"/>
@@ -5090,24 +5090,24 @@
       <c r="D35" s="6">
         <v>2</v>
       </c>
-      <c r="E35" s="57" t="s">
+      <c r="E35" s="60" t="s">
         <v>231</v>
       </c>
       <c r="F35" s="78"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="57" t="s">
+      <c r="G35" s="61"/>
+      <c r="H35" s="60" t="s">
         <v>134</v>
       </c>
       <c r="I35" s="78"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="57" t="s">
+      <c r="J35" s="61"/>
+      <c r="K35" s="60" t="s">
         <v>230</v>
       </c>
       <c r="L35" s="78"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="57"/>
+      <c r="M35" s="61"/>
+      <c r="N35" s="60"/>
       <c r="O35" s="78"/>
-      <c r="P35" s="58"/>
+      <c r="P35" s="61"/>
       <c r="Q35" s="79"/>
       <c r="R35" s="80"/>
       <c r="S35" s="81"/>
@@ -5155,24 +5155,24 @@
       <c r="D36" s="6">
         <v>2</v>
       </c>
-      <c r="E36" s="57"/>
+      <c r="E36" s="60"/>
       <c r="F36" s="78"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="57" t="s">
+      <c r="G36" s="61"/>
+      <c r="H36" s="60" t="s">
         <v>134</v>
       </c>
       <c r="I36" s="78"/>
-      <c r="J36" s="58"/>
-      <c r="K36" s="57" t="s">
+      <c r="J36" s="61"/>
+      <c r="K36" s="60" t="s">
         <v>241</v>
       </c>
       <c r="L36" s="78"/>
-      <c r="M36" s="58"/>
-      <c r="N36" s="57" t="s">
+      <c r="M36" s="61"/>
+      <c r="N36" s="60" t="s">
         <v>230</v>
       </c>
       <c r="O36" s="78"/>
-      <c r="P36" s="58"/>
+      <c r="P36" s="61"/>
       <c r="Q36" s="79"/>
       <c r="R36" s="80"/>
       <c r="S36" s="81"/>
@@ -5220,18 +5220,18 @@
       <c r="D37" s="6">
         <v>3</v>
       </c>
-      <c r="E37" s="57"/>
+      <c r="E37" s="60"/>
       <c r="F37" s="78"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="57"/>
+      <c r="G37" s="61"/>
+      <c r="H37" s="60"/>
       <c r="I37" s="78"/>
-      <c r="J37" s="58"/>
-      <c r="K37" s="57"/>
+      <c r="J37" s="61"/>
+      <c r="K37" s="60"/>
       <c r="L37" s="78"/>
-      <c r="M37" s="58"/>
-      <c r="N37" s="57"/>
+      <c r="M37" s="61"/>
+      <c r="N37" s="60"/>
       <c r="O37" s="78"/>
-      <c r="P37" s="58"/>
+      <c r="P37" s="61"/>
       <c r="Q37" s="79"/>
       <c r="R37" s="80"/>
       <c r="S37" s="81"/>
@@ -5275,26 +5275,26 @@
       <c r="D38" s="6">
         <v>4</v>
       </c>
-      <c r="E38" s="57" t="s">
+      <c r="E38" s="60" t="s">
         <v>353</v>
       </c>
       <c r="F38" s="78"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="57" t="s">
+      <c r="G38" s="61"/>
+      <c r="H38" s="60" t="s">
         <v>134</v>
       </c>
       <c r="I38" s="78"/>
-      <c r="J38" s="58"/>
-      <c r="K38" s="57" t="s">
+      <c r="J38" s="61"/>
+      <c r="K38" s="60" t="s">
         <v>233</v>
       </c>
       <c r="L38" s="78"/>
-      <c r="M38" s="58"/>
-      <c r="N38" s="57" t="s">
+      <c r="M38" s="61"/>
+      <c r="N38" s="60" t="s">
         <v>214</v>
       </c>
       <c r="O38" s="78"/>
-      <c r="P38" s="58"/>
+      <c r="P38" s="61"/>
       <c r="Q38" s="79"/>
       <c r="R38" s="80"/>
       <c r="S38" s="81"/>
@@ -5348,11 +5348,11 @@
       </c>
       <c r="I39" s="69"/>
       <c r="J39" s="69"/>
-      <c r="K39" s="57" t="s">
+      <c r="K39" s="60" t="s">
         <v>240</v>
       </c>
       <c r="L39" s="78"/>
-      <c r="M39" s="58"/>
+      <c r="M39" s="61"/>
       <c r="N39" s="69"/>
       <c r="O39" s="69"/>
       <c r="P39" s="69"/>
@@ -5783,25 +5783,25 @@
       <c r="D46" s="6">
         <v>4</v>
       </c>
-      <c r="E46" s="57"/>
+      <c r="E46" s="60"/>
       <c r="F46" s="78"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="57" t="s">
+      <c r="G46" s="61"/>
+      <c r="H46" s="60" t="s">
         <v>134</v>
       </c>
       <c r="I46" s="78"/>
-      <c r="J46" s="58"/>
-      <c r="K46" s="57" t="s">
+      <c r="J46" s="61"/>
+      <c r="K46" s="60" t="s">
         <v>232</v>
       </c>
       <c r="L46" s="78"/>
-      <c r="M46" s="58"/>
-      <c r="N46" s="57"/>
+      <c r="M46" s="61"/>
+      <c r="N46" s="60"/>
       <c r="O46" s="78"/>
-      <c r="P46" s="58"/>
-      <c r="Q46" s="57"/>
+      <c r="P46" s="61"/>
+      <c r="Q46" s="60"/>
       <c r="R46" s="78"/>
-      <c r="S46" s="58"/>
+      <c r="S46" s="61"/>
       <c r="T46" s="75" t="s">
         <v>135</v>
       </c>
@@ -5860,9 +5860,9 @@
       <c r="N47" s="69"/>
       <c r="O47" s="69"/>
       <c r="P47" s="69"/>
-      <c r="Q47" s="57"/>
+      <c r="Q47" s="60"/>
       <c r="R47" s="78"/>
-      <c r="S47" s="58"/>
+      <c r="S47" s="61"/>
       <c r="T47" s="70"/>
       <c r="U47" s="69"/>
       <c r="V47" s="69"/>
@@ -5907,11 +5907,11 @@
       <c r="D48" s="6">
         <v>6</v>
       </c>
-      <c r="E48" s="57" t="s">
+      <c r="E48" s="60" t="s">
         <v>353</v>
       </c>
       <c r="F48" s="78"/>
-      <c r="G48" s="58"/>
+      <c r="G48" s="61"/>
       <c r="H48" s="69" t="s">
         <v>250</v>
       </c>
@@ -5925,9 +5925,9 @@
       <c r="N48" s="69"/>
       <c r="O48" s="69"/>
       <c r="P48" s="69"/>
-      <c r="Q48" s="57"/>
+      <c r="Q48" s="60"/>
       <c r="R48" s="78"/>
-      <c r="S48" s="58"/>
+      <c r="S48" s="61"/>
       <c r="T48" s="70"/>
       <c r="U48" s="69"/>
       <c r="V48" s="69"/>
@@ -5990,9 +5990,9 @@
       </c>
       <c r="O49" s="69"/>
       <c r="P49" s="69"/>
-      <c r="Q49" s="57"/>
+      <c r="Q49" s="60"/>
       <c r="R49" s="78"/>
-      <c r="S49" s="58"/>
+      <c r="S49" s="61"/>
       <c r="T49" s="70"/>
       <c r="U49" s="69"/>
       <c r="V49" s="69"/>
@@ -6036,23 +6036,23 @@
       <c r="D50" s="6">
         <v>5</v>
       </c>
-      <c r="E50" s="57" t="s">
+      <c r="E50" s="60" t="s">
         <v>262</v>
       </c>
       <c r="F50" s="78"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="57"/>
+      <c r="G50" s="61"/>
+      <c r="H50" s="60"/>
       <c r="I50" s="78"/>
-      <c r="J50" s="58"/>
-      <c r="K50" s="57"/>
+      <c r="J50" s="61"/>
+      <c r="K50" s="60"/>
       <c r="L50" s="78"/>
-      <c r="M50" s="58"/>
-      <c r="N50" s="57"/>
+      <c r="M50" s="61"/>
+      <c r="N50" s="60"/>
       <c r="O50" s="78"/>
-      <c r="P50" s="58"/>
-      <c r="Q50" s="57"/>
+      <c r="P50" s="61"/>
+      <c r="Q50" s="60"/>
       <c r="R50" s="78"/>
-      <c r="S50" s="58"/>
+      <c r="S50" s="61"/>
       <c r="T50" s="75"/>
       <c r="U50" s="76"/>
       <c r="V50" s="76"/>
@@ -6095,23 +6095,23 @@
       <c r="D51" s="6">
         <v>7</v>
       </c>
-      <c r="E51" s="57" t="s">
+      <c r="E51" s="60" t="s">
         <v>198</v>
       </c>
       <c r="F51" s="78"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="57"/>
+      <c r="G51" s="61"/>
+      <c r="H51" s="60"/>
       <c r="I51" s="78"/>
-      <c r="J51" s="58"/>
-      <c r="K51" s="57"/>
+      <c r="J51" s="61"/>
+      <c r="K51" s="60"/>
       <c r="L51" s="78"/>
-      <c r="M51" s="58"/>
-      <c r="N51" s="57"/>
+      <c r="M51" s="61"/>
+      <c r="N51" s="60"/>
       <c r="O51" s="78"/>
-      <c r="P51" s="58"/>
-      <c r="Q51" s="57"/>
+      <c r="P51" s="61"/>
+      <c r="Q51" s="60"/>
       <c r="R51" s="78"/>
-      <c r="S51" s="58"/>
+      <c r="S51" s="61"/>
       <c r="T51" s="75"/>
       <c r="U51" s="76"/>
       <c r="V51" s="76"/>
@@ -6154,11 +6154,11 @@
       <c r="D52" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="E52" s="57" t="s">
+      <c r="E52" s="60" t="s">
         <v>206</v>
       </c>
       <c r="F52" s="78"/>
-      <c r="G52" s="58"/>
+      <c r="G52" s="61"/>
       <c r="H52" s="69"/>
       <c r="I52" s="69"/>
       <c r="J52" s="69"/>
@@ -6168,9 +6168,9 @@
       <c r="N52" s="69"/>
       <c r="O52" s="69"/>
       <c r="P52" s="69"/>
-      <c r="Q52" s="57"/>
+      <c r="Q52" s="60"/>
       <c r="R52" s="78"/>
-      <c r="S52" s="58"/>
+      <c r="S52" s="61"/>
       <c r="T52" s="70"/>
       <c r="U52" s="69"/>
       <c r="V52" s="69"/>
@@ -6221,9 +6221,9 @@
       <c r="N53" s="69"/>
       <c r="O53" s="69"/>
       <c r="P53" s="69"/>
-      <c r="Q53" s="57"/>
+      <c r="Q53" s="60"/>
       <c r="R53" s="78"/>
-      <c r="S53" s="58"/>
+      <c r="S53" s="61"/>
       <c r="T53" s="70"/>
       <c r="U53" s="69"/>
       <c r="V53" s="69"/>
@@ -6285,11 +6285,11 @@
       </c>
       <c r="O54" s="69"/>
       <c r="P54" s="69"/>
-      <c r="Q54" s="57" t="s">
+      <c r="Q54" s="60" t="s">
         <v>367</v>
       </c>
       <c r="R54" s="78"/>
-      <c r="S54" s="58"/>
+      <c r="S54" s="61"/>
       <c r="T54" s="70" t="s">
         <v>248</v>
       </c>
@@ -6408,11 +6408,11 @@
       <c r="D56" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E56" s="57" t="s">
+      <c r="E56" s="60" t="s">
         <v>210</v>
       </c>
       <c r="F56" s="78"/>
-      <c r="G56" s="58"/>
+      <c r="G56" s="61"/>
       <c r="H56" s="69"/>
       <c r="I56" s="69"/>
       <c r="J56" s="69"/>
@@ -6752,11 +6752,11 @@
       </c>
       <c r="O61" s="69"/>
       <c r="P61" s="69"/>
-      <c r="Q61" s="57" t="s">
+      <c r="Q61" s="60" t="s">
         <v>228</v>
       </c>
       <c r="R61" s="78"/>
-      <c r="S61" s="58"/>
+      <c r="S61" s="61"/>
       <c r="T61" s="70"/>
       <c r="U61" s="69"/>
       <c r="V61" s="69"/>
@@ -6853,35 +6853,35 @@
       <c r="BF62" s="30"/>
     </row>
     <row r="63" spans="1:68">
-      <c r="A63" s="88" t="s">
+      <c r="A63" s="91" t="s">
         <v>195</v>
       </c>
-      <c r="B63" s="89"/>
-      <c r="C63" s="89"/>
-      <c r="D63" s="89"/>
-      <c r="E63" s="89"/>
-      <c r="F63" s="89"/>
-      <c r="G63" s="89"/>
-      <c r="H63" s="89"/>
-      <c r="I63" s="89"/>
-      <c r="J63" s="89"/>
-      <c r="K63" s="89"/>
-      <c r="L63" s="89"/>
-      <c r="M63" s="89"/>
-      <c r="N63" s="89"/>
-      <c r="O63" s="89"/>
-      <c r="P63" s="89"/>
-      <c r="Q63" s="89"/>
-      <c r="R63" s="89"/>
-      <c r="S63" s="89"/>
-      <c r="T63" s="89"/>
-      <c r="U63" s="89"/>
-      <c r="V63" s="89"/>
-      <c r="W63" s="89"/>
-      <c r="X63" s="89"/>
-      <c r="Y63" s="89"/>
-      <c r="Z63" s="89"/>
-      <c r="AA63" s="90"/>
+      <c r="B63" s="92"/>
+      <c r="C63" s="92"/>
+      <c r="D63" s="92"/>
+      <c r="E63" s="92"/>
+      <c r="F63" s="92"/>
+      <c r="G63" s="92"/>
+      <c r="H63" s="92"/>
+      <c r="I63" s="92"/>
+      <c r="J63" s="92"/>
+      <c r="K63" s="92"/>
+      <c r="L63" s="92"/>
+      <c r="M63" s="92"/>
+      <c r="N63" s="92"/>
+      <c r="O63" s="92"/>
+      <c r="P63" s="92"/>
+      <c r="Q63" s="92"/>
+      <c r="R63" s="92"/>
+      <c r="S63" s="92"/>
+      <c r="T63" s="92"/>
+      <c r="U63" s="92"/>
+      <c r="V63" s="92"/>
+      <c r="W63" s="92"/>
+      <c r="X63" s="92"/>
+      <c r="Y63" s="92"/>
+      <c r="Z63" s="92"/>
+      <c r="AA63" s="93"/>
       <c r="AB63" s="51"/>
       <c r="AC63" s="52"/>
       <c r="AD63" s="52"/>
@@ -7217,35 +7217,35 @@
       <c r="BO68" s="37"/>
     </row>
     <row r="69" spans="1:67">
-      <c r="A69" s="62" t="s">
+      <c r="A69" s="65" t="s">
         <v>189</v>
       </c>
-      <c r="B69" s="63"/>
-      <c r="C69" s="63"/>
-      <c r="D69" s="63"/>
-      <c r="E69" s="63"/>
-      <c r="F69" s="63"/>
-      <c r="G69" s="63"/>
-      <c r="H69" s="63"/>
-      <c r="I69" s="63"/>
-      <c r="J69" s="63"/>
-      <c r="K69" s="63"/>
-      <c r="L69" s="63"/>
-      <c r="M69" s="63"/>
-      <c r="N69" s="63"/>
-      <c r="O69" s="63"/>
-      <c r="P69" s="63"/>
-      <c r="Q69" s="63"/>
-      <c r="R69" s="63"/>
-      <c r="S69" s="63"/>
-      <c r="T69" s="63"/>
-      <c r="U69" s="63"/>
-      <c r="V69" s="63"/>
-      <c r="W69" s="63"/>
-      <c r="X69" s="63"/>
-      <c r="Y69" s="63"/>
-      <c r="Z69" s="63"/>
-      <c r="AA69" s="64"/>
+      <c r="B69" s="66"/>
+      <c r="C69" s="66"/>
+      <c r="D69" s="66"/>
+      <c r="E69" s="66"/>
+      <c r="F69" s="66"/>
+      <c r="G69" s="66"/>
+      <c r="H69" s="66"/>
+      <c r="I69" s="66"/>
+      <c r="J69" s="66"/>
+      <c r="K69" s="66"/>
+      <c r="L69" s="66"/>
+      <c r="M69" s="66"/>
+      <c r="N69" s="66"/>
+      <c r="O69" s="66"/>
+      <c r="P69" s="66"/>
+      <c r="Q69" s="66"/>
+      <c r="R69" s="66"/>
+      <c r="S69" s="66"/>
+      <c r="T69" s="66"/>
+      <c r="U69" s="66"/>
+      <c r="V69" s="66"/>
+      <c r="W69" s="66"/>
+      <c r="X69" s="66"/>
+      <c r="Y69" s="66"/>
+      <c r="Z69" s="66"/>
+      <c r="AA69" s="67"/>
       <c r="AB69" s="51"/>
       <c r="AC69" s="52"/>
       <c r="AD69" s="52"/>
@@ -7350,18 +7350,18 @@
       <c r="AV70" s="19"/>
       <c r="AW70" s="20"/>
       <c r="AX70" s="20"/>
-      <c r="BF70" s="91" t="s">
+      <c r="BF70" s="94" t="s">
         <v>263</v>
       </c>
-      <c r="BG70" s="91"/>
-      <c r="BH70" s="91"/>
-      <c r="BI70" s="91"/>
-      <c r="BJ70" s="91"/>
-      <c r="BK70" s="91"/>
-      <c r="BL70" s="91"/>
-      <c r="BM70" s="91"/>
-      <c r="BN70" s="91"/>
-      <c r="BO70" s="91"/>
+      <c r="BG70" s="94"/>
+      <c r="BH70" s="94"/>
+      <c r="BI70" s="94"/>
+      <c r="BJ70" s="94"/>
+      <c r="BK70" s="94"/>
+      <c r="BL70" s="94"/>
+      <c r="BM70" s="94"/>
+      <c r="BN70" s="94"/>
+      <c r="BO70" s="94"/>
     </row>
     <row r="71" spans="1:67">
       <c r="A71" s="7" t="s">
@@ -7424,16 +7424,16 @@
       <c r="AV71" s="19"/>
       <c r="AW71" s="20"/>
       <c r="AX71" s="20"/>
-      <c r="BF71" s="91"/>
-      <c r="BG71" s="91"/>
-      <c r="BH71" s="91"/>
-      <c r="BI71" s="91"/>
-      <c r="BJ71" s="91"/>
-      <c r="BK71" s="91"/>
-      <c r="BL71" s="91"/>
-      <c r="BM71" s="91"/>
-      <c r="BN71" s="91"/>
-      <c r="BO71" s="91"/>
+      <c r="BF71" s="94"/>
+      <c r="BG71" s="94"/>
+      <c r="BH71" s="94"/>
+      <c r="BI71" s="94"/>
+      <c r="BJ71" s="94"/>
+      <c r="BK71" s="94"/>
+      <c r="BL71" s="94"/>
+      <c r="BM71" s="94"/>
+      <c r="BN71" s="94"/>
+      <c r="BO71" s="94"/>
     </row>
     <row r="72" spans="1:67">
       <c r="A72" s="7"/>
@@ -7488,16 +7488,16 @@
       <c r="AV72" s="19"/>
       <c r="AW72" s="20"/>
       <c r="AX72" s="20"/>
-      <c r="BF72" s="91"/>
-      <c r="BG72" s="91"/>
-      <c r="BH72" s="91"/>
-      <c r="BI72" s="91"/>
-      <c r="BJ72" s="91"/>
-      <c r="BK72" s="91"/>
-      <c r="BL72" s="91"/>
-      <c r="BM72" s="91"/>
-      <c r="BN72" s="91"/>
-      <c r="BO72" s="91"/>
+      <c r="BF72" s="94"/>
+      <c r="BG72" s="94"/>
+      <c r="BH72" s="94"/>
+      <c r="BI72" s="94"/>
+      <c r="BJ72" s="94"/>
+      <c r="BK72" s="94"/>
+      <c r="BL72" s="94"/>
+      <c r="BM72" s="94"/>
+      <c r="BN72" s="94"/>
+      <c r="BO72" s="94"/>
     </row>
     <row r="73" spans="1:67">
       <c r="A73" s="7" t="s">
@@ -7566,16 +7566,16 @@
       <c r="AV73" s="19"/>
       <c r="AW73" s="20"/>
       <c r="AX73" s="20"/>
-      <c r="BF73" s="91"/>
-      <c r="BG73" s="91"/>
-      <c r="BH73" s="91"/>
-      <c r="BI73" s="91"/>
-      <c r="BJ73" s="91"/>
-      <c r="BK73" s="91"/>
-      <c r="BL73" s="91"/>
-      <c r="BM73" s="91"/>
-      <c r="BN73" s="91"/>
-      <c r="BO73" s="91"/>
+      <c r="BF73" s="94"/>
+      <c r="BG73" s="94"/>
+      <c r="BH73" s="94"/>
+      <c r="BI73" s="94"/>
+      <c r="BJ73" s="94"/>
+      <c r="BK73" s="94"/>
+      <c r="BL73" s="94"/>
+      <c r="BM73" s="94"/>
+      <c r="BN73" s="94"/>
+      <c r="BO73" s="94"/>
     </row>
     <row r="74" spans="1:67">
       <c r="A74" s="7" t="s">
@@ -7642,16 +7642,16 @@
       <c r="AV74" s="19"/>
       <c r="AW74" s="20"/>
       <c r="AX74" s="20"/>
-      <c r="BF74" s="91"/>
-      <c r="BG74" s="91"/>
-      <c r="BH74" s="91"/>
-      <c r="BI74" s="91"/>
-      <c r="BJ74" s="91"/>
-      <c r="BK74" s="91"/>
-      <c r="BL74" s="91"/>
-      <c r="BM74" s="91"/>
-      <c r="BN74" s="91"/>
-      <c r="BO74" s="91"/>
+      <c r="BF74" s="94"/>
+      <c r="BG74" s="94"/>
+      <c r="BH74" s="94"/>
+      <c r="BI74" s="94"/>
+      <c r="BJ74" s="94"/>
+      <c r="BK74" s="94"/>
+      <c r="BL74" s="94"/>
+      <c r="BM74" s="94"/>
+      <c r="BN74" s="94"/>
+      <c r="BO74" s="94"/>
     </row>
     <row r="75" spans="1:67">
       <c r="A75" s="7" t="s">
@@ -7720,16 +7720,16 @@
       <c r="AV75" s="19"/>
       <c r="AW75" s="20"/>
       <c r="AX75" s="20"/>
-      <c r="BF75" s="91"/>
-      <c r="BG75" s="91"/>
-      <c r="BH75" s="91"/>
-      <c r="BI75" s="91"/>
-      <c r="BJ75" s="91"/>
-      <c r="BK75" s="91"/>
-      <c r="BL75" s="91"/>
-      <c r="BM75" s="91"/>
-      <c r="BN75" s="91"/>
-      <c r="BO75" s="91"/>
+      <c r="BF75" s="94"/>
+      <c r="BG75" s="94"/>
+      <c r="BH75" s="94"/>
+      <c r="BI75" s="94"/>
+      <c r="BJ75" s="94"/>
+      <c r="BK75" s="94"/>
+      <c r="BL75" s="94"/>
+      <c r="BM75" s="94"/>
+      <c r="BN75" s="94"/>
+      <c r="BO75" s="94"/>
     </row>
     <row r="76" spans="1:67">
       <c r="A76" s="29" t="s">
@@ -7805,16 +7805,16 @@
       <c r="BC76" s="32"/>
       <c r="BD76" s="32"/>
       <c r="BE76" s="32"/>
-      <c r="BF76" s="91"/>
-      <c r="BG76" s="91"/>
-      <c r="BH76" s="91"/>
-      <c r="BI76" s="91"/>
-      <c r="BJ76" s="91"/>
-      <c r="BK76" s="91"/>
-      <c r="BL76" s="91"/>
-      <c r="BM76" s="91"/>
-      <c r="BN76" s="91"/>
-      <c r="BO76" s="91"/>
+      <c r="BF76" s="94"/>
+      <c r="BG76" s="94"/>
+      <c r="BH76" s="94"/>
+      <c r="BI76" s="94"/>
+      <c r="BJ76" s="94"/>
+      <c r="BK76" s="94"/>
+      <c r="BL76" s="94"/>
+      <c r="BM76" s="94"/>
+      <c r="BN76" s="94"/>
+      <c r="BO76" s="94"/>
     </row>
     <row r="77" spans="1:67">
       <c r="A77" s="12"/>
@@ -9295,6 +9295,15 @@
       <c r="B123" t="s">
         <v>70</v>
       </c>
+      <c r="P123" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q123" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="R123" s="20" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="124" spans="1:18">
       <c r="A124" t="s">
@@ -9303,14 +9312,14 @@
       <c r="B124" t="s">
         <v>71</v>
       </c>
-      <c r="P124" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="Q124" s="20" t="s">
-        <v>285</v>
-      </c>
-      <c r="R124" s="20" t="s">
-        <v>287</v>
+      <c r="P124" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>288</v>
+      </c>
+      <c r="R124" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="125" spans="1:18">
@@ -9320,14 +9329,14 @@
       <c r="B125" t="s">
         <v>72</v>
       </c>
-      <c r="P125" s="43" t="s">
-        <v>284</v>
+      <c r="P125" s="44" t="s">
+        <v>10</v>
       </c>
       <c r="Q125" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="R125" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="126" spans="1:18">
@@ -9337,48 +9346,48 @@
       <c r="B126" t="s">
         <v>73</v>
       </c>
-      <c r="P126" s="44" t="s">
-        <v>10</v>
+      <c r="P126" s="45" t="s">
+        <v>133</v>
       </c>
       <c r="Q126" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="R126" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="127" spans="1:18">
-      <c r="P127" s="45" t="s">
-        <v>133</v>
+      <c r="P127" s="46" t="s">
+        <v>11</v>
       </c>
       <c r="Q127" t="s">
-        <v>295</v>
+        <v>78</v>
       </c>
       <c r="R127" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="128" spans="1:18">
-      <c r="P128" s="46" t="s">
-        <v>11</v>
+      <c r="P128" s="47" t="s">
+        <v>282</v>
       </c>
       <c r="Q128" t="s">
-        <v>78</v>
+        <v>290</v>
       </c>
       <c r="R128" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="129" spans="1:21">
       <c r="B129" s="42"/>
-      <c r="P129" s="47" t="s">
-        <v>282</v>
+      <c r="P129" s="48" t="s">
+        <v>283</v>
       </c>
       <c r="Q129" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="R129" t="s">
-        <v>294</v>
+        <v>340</v>
       </c>
     </row>
     <row r="130" spans="1:21">
@@ -9399,15 +9408,6 @@
       </c>
       <c r="G130" s="48" t="s">
         <v>283</v>
-      </c>
-      <c r="P130" s="48" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q130" t="s">
-        <v>291</v>
-      </c>
-      <c r="R130" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="131" spans="1:21">
@@ -9814,13 +9814,13 @@
     </row>
     <row r="145" spans="1:43">
       <c r="A145" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B145" s="44" t="s">
         <v>10</v>
       </c>
       <c r="C145" s="19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D145" s="19"/>
       <c r="E145" s="19"/>
@@ -9844,13 +9844,13 @@
     </row>
     <row r="146" spans="1:43">
       <c r="A146" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="B146" s="44" t="s">
-        <v>10</v>
+        <v>279</v>
+      </c>
+      <c r="B146" s="43" t="s">
+        <v>284</v>
       </c>
       <c r="C146" s="19" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D146" s="19"/>
       <c r="E146" s="19"/>
@@ -10252,14 +10252,14 @@
       <c r="U159" s="19"/>
     </row>
     <row r="160" spans="1:43">
-      <c r="A160" s="6" t="s">
-        <v>312</v>
+      <c r="A160" s="49" t="s">
+        <v>323</v>
       </c>
       <c r="B160" s="44" t="s">
         <v>10</v>
       </c>
       <c r="C160" s="19" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="D160" s="19"/>
       <c r="E160" s="19"/>
@@ -10272,7 +10272,6 @@
       <c r="L160" s="19"/>
       <c r="M160" s="19"/>
       <c r="N160" s="19"/>
-      <c r="O160" s="19"/>
       <c r="P160" s="2" t="s">
         <v>356</v>
       </c>
@@ -10283,14 +10282,14 @@
       <c r="U160" s="19"/>
     </row>
     <row r="161" spans="1:21">
-      <c r="A161" s="49" t="s">
-        <v>323</v>
+      <c r="A161" s="6" t="s">
+        <v>313</v>
       </c>
       <c r="B161" s="44" t="s">
         <v>10</v>
       </c>
       <c r="C161" s="19" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="D161" s="19"/>
       <c r="E161" s="19"/>
@@ -10303,6 +10302,7 @@
       <c r="L161" s="19"/>
       <c r="M161" s="19"/>
       <c r="N161" s="19"/>
+      <c r="O161" s="19"/>
       <c r="P161" s="2" t="s">
         <v>356</v>
       </c>
@@ -10314,13 +10314,13 @@
     </row>
     <row r="162" spans="1:21">
       <c r="A162" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B162" s="43" t="s">
         <v>284</v>
       </c>
       <c r="C162" s="19" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D162" s="19"/>
       <c r="E162" s="19"/>
@@ -11396,9 +11396,6 @@
       <c r="C226" t="s">
         <v>387</v>
       </c>
-      <c r="P226" s="2" t="s">
-        <v>356</v>
-      </c>
     </row>
     <row r="227" spans="1:16">
       <c r="A227" s="6" t="s">
@@ -11410,7 +11407,9 @@
       <c r="C227" t="s">
         <v>403</v>
       </c>
-      <c r="P227" s="55"/>
+      <c r="P227" s="2" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="228" spans="1:16">
       <c r="A228" s="6"/>
@@ -11883,6 +11882,8 @@
     <mergeCell ref="K41:M41"/>
     <mergeCell ref="K42:M42"/>
     <mergeCell ref="K43:M43"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H26:I26"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="H19:I19"/>
@@ -11905,12 +11906,6 @@
     <mergeCell ref="E40:G40"/>
     <mergeCell ref="E41:G41"/>
     <mergeCell ref="E42:G42"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="AG24:AH24"/>
-    <mergeCell ref="AG26:AH26"/>
-    <mergeCell ref="AG27:AH27"/>
-    <mergeCell ref="AG28:AH28"/>
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="H18:I18"/>
@@ -11920,17 +11915,8 @@
     <mergeCell ref="AG20:AH20"/>
     <mergeCell ref="AG21:AH21"/>
     <mergeCell ref="AG22:AH22"/>
-    <mergeCell ref="AG23:AH23"/>
-    <mergeCell ref="AC26:AD26"/>
-    <mergeCell ref="AC27:AD27"/>
-    <mergeCell ref="AC28:AD28"/>
     <mergeCell ref="AC22:AD22"/>
-    <mergeCell ref="AC23:AD23"/>
-    <mergeCell ref="AC24:AD24"/>
-    <mergeCell ref="Y28:Z28"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="Y15:Z15"/>
     <mergeCell ref="AG16:AH16"/>
     <mergeCell ref="AG15:AH15"/>
     <mergeCell ref="AG12:AH12"/>
@@ -11945,10 +11931,6 @@
     <mergeCell ref="AC12:AD12"/>
     <mergeCell ref="AC17:AD17"/>
     <mergeCell ref="AC19:AD19"/>
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="Y19:Z19"/>
-    <mergeCell ref="Y20:Z20"/>
-    <mergeCell ref="Y21:Z21"/>
     <mergeCell ref="Q26:R26"/>
     <mergeCell ref="Q27:R27"/>
     <mergeCell ref="Q28:R28"/>
@@ -11961,6 +11943,18 @@
     <mergeCell ref="U28:V28"/>
     <mergeCell ref="U22:V22"/>
     <mergeCell ref="A25:AL25"/>
+    <mergeCell ref="AG24:AH24"/>
+    <mergeCell ref="AG26:AH26"/>
+    <mergeCell ref="AG27:AH27"/>
+    <mergeCell ref="AG28:AH28"/>
+    <mergeCell ref="AG23:AH23"/>
+    <mergeCell ref="AC26:AD26"/>
+    <mergeCell ref="AC27:AD27"/>
+    <mergeCell ref="AC28:AD28"/>
+    <mergeCell ref="AC23:AD23"/>
+    <mergeCell ref="AC24:AD24"/>
+    <mergeCell ref="Y28:Z28"/>
+    <mergeCell ref="H23:I23"/>
     <mergeCell ref="U11:V11"/>
     <mergeCell ref="Y13:Z13"/>
     <mergeCell ref="U14:V14"/>
@@ -11974,6 +11968,11 @@
     <mergeCell ref="U19:V19"/>
     <mergeCell ref="U20:V20"/>
     <mergeCell ref="U21:V21"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="Y20:Z20"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="Y12:Z12"/>
     <mergeCell ref="M15:N15"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="M17:N17"/>
@@ -12371,7 +12370,6 @@
     <mergeCell ref="T73:Y73"/>
     <mergeCell ref="T74:Y74"/>
     <mergeCell ref="T75:Y75"/>
-    <mergeCell ref="T76:Y76"/>
     <mergeCell ref="T101:Y101"/>
     <mergeCell ref="T77:Y77"/>
     <mergeCell ref="T78:Y78"/>
@@ -12409,6 +12407,7 @@
     <mergeCell ref="Q95:S95"/>
     <mergeCell ref="Q96:S96"/>
     <mergeCell ref="Q97:S97"/>
+    <mergeCell ref="T76:Y76"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>